<commit_message>
🔄 Actualización automática del mapa (2025-07-21 07:30:56)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2163,6 +2163,82 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>-522</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>7/21/2025</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Uruguay 1090</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>808430941</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Reclaman columna corroida y rienda fuera de norma pero no se ve en la foto.</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M25" t="n">
+        <v>-58.387175</v>
+      </c>
+      <c r="N25" t="n">
+        <v>-34.596</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>Recoleta</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-21 15:08:56)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -559,8 +559,16 @@
       <c r="I2" t="n">
         <v>0</v>
       </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr">
         <is>
           <t>Pasante</t>
@@ -627,8 +635,16 @@
       <c r="I3" t="n">
         <v>1</v>
       </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>Pasante</t>
@@ -691,8 +707,16 @@
       <c r="I4" t="n">
         <v>0</v>
       </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr">
         <is>
           <t>Pasante</t>
@@ -759,8 +783,16 @@
       <c r="I5" t="n">
         <v>0</v>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>Pasante</t>
@@ -827,8 +859,16 @@
       <c r="I6" t="n">
         <v>0</v>
       </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>Pasante</t>
@@ -891,8 +931,16 @@
       <c r="I7" t="n">
         <v>0</v>
       </c>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>Pasante</t>
@@ -959,8 +1007,16 @@
       <c r="I8" t="n">
         <v>0</v>
       </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
       <c r="L8" t="inlineStr">
         <is>
           <t>Pasante</t>
@@ -1027,8 +1083,16 @@
       <c r="I9" t="n">
         <v>0</v>
       </c>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
       <c r="L9" t="inlineStr">
         <is>
           <t>Pasante</t>
@@ -1095,8 +1159,16 @@
       <c r="I10" t="n">
         <v>0</v>
       </c>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
       <c r="L10" t="inlineStr">
         <is>
           <t>Pasante</t>
@@ -1163,8 +1235,16 @@
       <c r="I11" t="n">
         <v>0</v>
       </c>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
       <c r="L11" t="inlineStr">
         <is>
           <t>Pasante</t>
@@ -1231,8 +1311,16 @@
       <c r="I12" t="n">
         <v>0</v>
       </c>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
       <c r="L12" t="inlineStr">
         <is>
           <t>Pasante</t>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-23 07:17:17)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1646,27 +1646,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>6180</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>5/4/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>AZARA 15</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>805655333</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1681,11 +1681,11 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1703,46 +1703,46 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.372751</v>
+        <v>-58.439727</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.631917</v>
+        <v>-34.556261</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>HERNANDEZ JOSE 1451</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1757,11 +1757,11 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1770,7 +1770,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1779,10 +1779,10 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.473937</v>
+        <v>-58.443936</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.557355</v>
+        <v>-34.560145</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1798,27 +1798,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>-508</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Moldes 2463</t>
+          <t>Conesa 2195</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>808194234</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1837,7 +1837,7 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1846,7 +1846,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1855,14 +1855,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.462281</v>
+        <v>-58.463015</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.560321</v>
+        <v>-34.564505</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1874,27 +1874,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>-509</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Paso 58</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>808194240</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1931,46 +1931,46 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.403422</v>
+        <v>-58.466348</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.609195</v>
+        <v>-34.556028</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-510</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Larrea 590</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>808194254</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1998,55 +1998,55 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.402353</v>
+        <v>-58.454065</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.602205</v>
+        <v>-34.57105</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-512</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 3742</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>808240230</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2083,46 +2083,46 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.470347</v>
+        <v>-58.436255</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.547965</v>
+        <v>-34.567733</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-514</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Bilbao 2452</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>808243829</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2155,18 +2155,18 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.460594</v>
+        <v>-58.43247</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.635581</v>
+        <v>-34.566492</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2178,27 +2178,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-516</t>
+          <t>6180</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>5/4/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Olazabal 4417</t>
+          <t>AZARA 15</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>808373646</t>
+          <t>805655333</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2235,46 +2235,46 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.478941</v>
+        <v>-58.372751</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.57242</v>
+        <v>-34.631917</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-522</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Uruguay 1090</t>
+          <t>Soldado de la Independencia 1298</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2289,7 +2289,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Reclaman columna corroida y rienda fuera de norma pero no se ve en la foto.</t>
+          <t>Picada - Con fuente teco</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2302,26 +2302,862 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M25" t="n">
+        <v>-58.440507</v>
+      </c>
+      <c r="N25" t="n">
+        <v>-34.564016</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>805722772</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>5/7/2025</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Luis Maria Campos 1336</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>805722772</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr">
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M26" t="n">
+        <v>-58.44191</v>
+      </c>
+      <c r="N26" t="n">
+        <v>-34.564245</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>-507</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>7/14/2025</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Tamborini 3291</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>808194229</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M27" t="n">
+        <v>-58.473937</v>
+      </c>
+      <c r="N27" t="n">
+        <v>-34.557355</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>-508</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>7/14/2025</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Moldes 2463</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>808194234</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>1</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M28" t="n">
+        <v>-58.462281</v>
+      </c>
+      <c r="N28" t="n">
+        <v>-34.560321</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>-509</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>7/14/2025</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Paso 58</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>808194240</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>1</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M29" t="n">
+        <v>-58.403422</v>
+      </c>
+      <c r="N29" t="n">
+        <v>-34.609195</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>-510</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>7/14/2025</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Larrea 590</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>808194254</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M30" t="n">
+        <v>-58.402353</v>
+      </c>
+      <c r="N30" t="n">
+        <v>-34.602205</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>-512</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>7/15/2025</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Ciudad de la Paz 3742</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>808240230</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M31" t="n">
+        <v>-58.470347</v>
+      </c>
+      <c r="N31" t="n">
+        <v>-34.547965</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>-514</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>7/15/2025</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Bilbao 2452</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>808243829</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>1</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M32" t="n">
+        <v>-58.460594</v>
+      </c>
+      <c r="N32" t="n">
+        <v>-34.635581</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>-516</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>7/16/2025</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Olazabal 4417</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>808373646</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M33" t="n">
+        <v>-58.478941</v>
+      </c>
+      <c r="N33" t="n">
+        <v>-34.57242</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>-522</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>7/21/2025</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Uruguay 1090</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>808430941</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Reclaman columna corroida y rienda fuera de norma pero no se ve en la foto.</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>1</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
         <is>
           <t>Terminal</t>
         </is>
       </c>
-      <c r="M25" t="n">
+      <c r="M34" t="n">
         <v>-58.387175</v>
       </c>
-      <c r="N25" t="n">
+      <c r="N34" t="n">
         <v>-34.596</v>
       </c>
-      <c r="O25" t="inlineStr">
+      <c r="O34" t="inlineStr">
         <is>
           <t>Recoleta</t>
         </is>
       </c>
-      <c r="P25" t="inlineStr">
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>-523</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>7/20/2025</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Luis Maria Campos 585</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>808460898</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>1</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M35" t="n">
+        <v>-58.434668</v>
+      </c>
+      <c r="N35" t="n">
+        <v>-34.571258</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>-524</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>7/21/2025</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Luis Maria Campos 509</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>808460897</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>1</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M36" t="n">
+        <v>-58.434194</v>
+      </c>
+      <c r="N36" t="n">
+        <v>-34.571754</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-23 11:53:11)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1874,27 +1874,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1909,11 +1909,11 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1931,14 +1931,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.466348</v>
+        <v>-58.507569</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.556028</v>
+        <v>-34.579623</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1950,17 +1950,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1970,7 +1970,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2003,18 +2003,18 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.454065</v>
+        <v>-58.466348</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.57105</v>
+        <v>-34.556028</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2026,27 +2026,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2061,7 +2061,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2083,46 +2083,46 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.436255</v>
+        <v>-58.497446</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.567733</v>
+        <v>-34.583455</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2159,46 +2159,46 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.43247</v>
+        <v>-58.454065</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.566492</v>
+        <v>-34.57105</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>6180</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5/4/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>AZARA 15</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>805655333</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2235,14 +2235,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.372751</v>
+        <v>-58.436255</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.631917</v>
+        <v>-34.567733</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2254,17 +2254,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Soldado de la Independencia 1298</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2274,7 +2274,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2289,7 +2289,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada - Con fuente teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2302,55 +2302,55 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.440507</v>
+        <v>-58.43247</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.564016</v>
+        <v>-34.566492</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>6180</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/4/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>AZARA 15</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>805655333</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2387,46 +2387,46 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.44191</v>
+        <v>-58.372751</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.564245</v>
+        <v>-34.631917</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Soldado de la Independencia 1298</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2441,7 +2441,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada - Con fuente teco</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2454,7 +2454,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2463,14 +2463,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.473937</v>
+        <v>-58.440507</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.557355</v>
+        <v>-34.564016</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2482,27 +2482,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-508</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Moldes 2463</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>808194234</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2530,7 +2530,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2539,14 +2539,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.462281</v>
+        <v>-58.44191</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.560321</v>
+        <v>-34.564245</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-509</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2568,17 +2568,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Paso 58</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808194240</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2615,26 +2615,26 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.403422</v>
+        <v>-58.473937</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.609195</v>
+        <v>-34.557355</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-510</t>
+          <t>-508</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2644,17 +2644,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Larrea 590</t>
+          <t>Moldes 2463</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808194254</t>
+          <t>808194234</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2682,7 +2682,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2691,46 +2691,46 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.402353</v>
+        <v>-58.462281</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.602205</v>
+        <v>-34.560321</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-512</t>
+          <t>-509</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 3742</t>
+          <t>Paso 58</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808240230</t>
+          <t>808194240</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2767,46 +2767,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.470347</v>
+        <v>-58.403422</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.547965</v>
+        <v>-34.609195</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-514</t>
+          <t>-510</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Bilbao 2452</t>
+          <t>Larrea 590</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808243829</t>
+          <t>808194254</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2834,7 +2834,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2843,14 +2843,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.460594</v>
+        <v>-58.402353</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.635581</v>
+        <v>-34.602205</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2862,17 +2862,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-516</t>
+          <t>-512</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Olazabal 4417</t>
+          <t>Ciudad de la Paz 3742</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2882,7 +2882,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808373646</t>
+          <t>808240230</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2919,14 +2919,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.478941</v>
+        <v>-58.470347</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.57242</v>
+        <v>-34.547965</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2938,27 +2938,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-522</t>
+          <t>-514</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Uruguay 1090</t>
+          <t>Bilbao 2452</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>808243829</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2973,7 +2973,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Reclaman columna corroida y rienda fuera de norma pero no se ve en la foto.</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2991,18 +2991,18 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.387175</v>
+        <v>-58.460594</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.596</v>
+        <v>-34.635581</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3014,27 +3014,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-516</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Olazabal 4417</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>808373646</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3071,26 +3071,26 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.434668</v>
+        <v>-58.478941</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.571258</v>
+        <v>-34.57242</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-522</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3100,17 +3100,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Uruguay 1090</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>808430941</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3125,7 +3125,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reclaman columna corroida y rienda fuera de norma pero no se ve en la foto.</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3143,21 +3143,173 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M36" t="n">
+        <v>-58.387175</v>
+      </c>
+      <c r="N36" t="n">
+        <v>-34.596</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>Recoleta</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>-523</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>7/20/2025</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Luis Maria Campos 585</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>808460898</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>1</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M36" t="n">
+      <c r="M37" t="n">
+        <v>-58.434668</v>
+      </c>
+      <c r="N37" t="n">
+        <v>-34.571258</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>-524</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>7/21/2025</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Luis Maria Campos 509</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>808460897</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M38" t="n">
         <v>-58.434194</v>
       </c>
-      <c r="N36" t="n">
+      <c r="N38" t="n">
         <v>-34.571754</v>
       </c>
-      <c r="O36" t="inlineStr">
+      <c r="O38" t="inlineStr">
         <is>
           <t>Palermo</t>
         </is>
       </c>
-      <c r="P36" t="inlineStr">
+      <c r="P38" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-24 12:17:13)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1798,27 +1798,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Conesa 2195</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1855,46 +1855,46 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.463015</v>
+        <v>-58.415566</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.564505</v>
+        <v>-34.613244</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804161220</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Carlos Calvo 4009</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804161220</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1909,7 +1909,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1931,46 +1931,46 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.507569</v>
+        <v>-58.422147</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.579623</v>
+        <v>-34.624736</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Treinta y Tres Orientales 905</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1989,7 +1989,7 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2007,46 +2007,46 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.466348</v>
+        <v>-58.423229</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.556028</v>
+        <v>-34.625103</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2061,11 +2061,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2083,46 +2083,46 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.497446</v>
+        <v>-58.418089</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.583455</v>
+        <v>-34.620313</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,7 +2141,7 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2155,50 +2155,50 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.454065</v>
+        <v>-58.427201</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.57105</v>
+        <v>-34.617131</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2217,7 +2217,7 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2235,14 +2235,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.436255</v>
+        <v>-58.414984</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.567733</v>
+        <v>-34.621386</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2254,27 +2254,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>Conesa 2195</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,7 +2293,7 @@
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2307,50 +2307,50 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.43247</v>
+        <v>-58.463015</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.566492</v>
+        <v>-34.564505</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>6180</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/4/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>AZARA 15</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805655333</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2365,11 +2365,11 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2387,46 +2387,46 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.372751</v>
+        <v>-58.507569</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.631917</v>
+        <v>-34.579623</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Soldado de la Independencia 1298</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2441,7 +2441,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada - Con fuente teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2454,7 +2454,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2463,14 +2463,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.440507</v>
+        <v>-58.466348</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.564016</v>
+        <v>-34.556028</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2482,27 +2482,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2517,7 +2517,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2539,14 +2539,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.44191</v>
+        <v>-58.497446</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.564245</v>
+        <v>-34.583455</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2558,27 +2558,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2611,18 +2611,18 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.473937</v>
+        <v>-58.454065</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.557355</v>
+        <v>-34.57105</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2634,27 +2634,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-508</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Moldes 2463</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808194234</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2682,7 +2682,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2691,46 +2691,46 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.462281</v>
+        <v>-58.436255</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.560321</v>
+        <v>-34.567733</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-509</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Paso 58</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808194240</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2763,18 +2763,18 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.403422</v>
+        <v>-58.43247</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.609195</v>
+        <v>-34.566492</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -2786,27 +2786,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-510</t>
+          <t>6180</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>5/4/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Larrea 590</t>
+          <t>AZARA 15</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808194254</t>
+          <t>805655333</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2834,7 +2834,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2843,14 +2843,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.402353</v>
+        <v>-58.372751</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.602205</v>
+        <v>-34.631917</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2862,27 +2862,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-512</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 3742</t>
+          <t>Soldado de la Independencia 1298</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808240230</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2897,7 +2897,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada - Con fuente teco</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2910,7 +2910,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2919,14 +2919,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.470347</v>
+        <v>-58.440507</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.547965</v>
+        <v>-34.564016</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2938,27 +2938,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-514</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Bilbao 2452</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808243829</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2995,46 +2995,46 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.460594</v>
+        <v>-58.44191</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.635581</v>
+        <v>-34.564245</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-516</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Olazabal 4417</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808373646</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3067,50 +3067,50 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.478941</v>
+        <v>-58.438744</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.57242</v>
+        <v>-34.629929</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-522</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Uruguay 1090</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3125,7 +3125,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Reclaman columna corroida y rienda fuera de norma pero no se ve en la foto.</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3143,50 +3143,50 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.387175</v>
+        <v>-58.473937</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.596</v>
+        <v>-34.557355</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-508</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Moldes 2463</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>808194234</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3214,7 +3214,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -3223,46 +3223,46 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.434668</v>
+        <v>-58.462281</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.571258</v>
+        <v>-34.560321</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-509</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Paso 58</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>808194240</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3299,17 +3299,625 @@
         </is>
       </c>
       <c r="M38" t="n">
+        <v>-58.403422</v>
+      </c>
+      <c r="N38" t="n">
+        <v>-34.609195</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>-510</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>7/14/2025</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Larrea 590</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>808194254</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>1</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M39" t="n">
+        <v>-58.402353</v>
+      </c>
+      <c r="N39" t="n">
+        <v>-34.602205</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>-512</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>7/15/2025</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Ciudad de la Paz 3742</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>808240230</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>1</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M40" t="n">
+        <v>-58.470347</v>
+      </c>
+      <c r="N40" t="n">
+        <v>-34.547965</v>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>6486</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>7/15/2025</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>BILBAO, FRANCISCO 2442</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>808243829</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>1</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M41" t="n">
+        <v>-58.460522</v>
+      </c>
+      <c r="N41" t="n">
+        <v>-34.635514</v>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>-516</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>7/16/2025</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Olazabal 4417</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>808373646</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>1</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M42" t="n">
+        <v>-58.478941</v>
+      </c>
+      <c r="N42" t="n">
+        <v>-34.57242</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>-522</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>7/21/2025</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Uruguay 1090</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>808430941</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Reclaman columna corroida y rienda fuera de norma pero no se ve en la foto.</t>
+        </is>
+      </c>
+      <c r="I43" t="n">
+        <v>1</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M43" t="n">
+        <v>-58.387175</v>
+      </c>
+      <c r="N43" t="n">
+        <v>-34.596</v>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>Recoleta</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>-523</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>7/20/2025</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Luis Maria Campos 585</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>808460898</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I44" t="n">
+        <v>1</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M44" t="n">
+        <v>-58.434668</v>
+      </c>
+      <c r="N44" t="n">
+        <v>-34.571258</v>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>-524</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>7/21/2025</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Luis Maria Campos 509</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>808460897</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
+        <v>1</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M45" t="n">
         <v>-58.434194</v>
       </c>
-      <c r="N38" t="n">
+      <c r="N45" t="n">
         <v>-34.571754</v>
       </c>
-      <c r="O38" t="inlineStr">
+      <c r="O45" t="inlineStr">
         <is>
           <t>Palermo</t>
         </is>
       </c>
-      <c r="P38" t="inlineStr">
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>6478</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>7/24/2025</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>JUJUY AV. 1647</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>808509387</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I46" t="n">
+        <v>1</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M46" t="n">
+        <v>-58.401083</v>
+      </c>
+      <c r="N46" t="n">
+        <v>-34.629397</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-25 07:05:27)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -1432,7 +1432,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>GURRUCHAGA /ALT/ 408</t>
+          <t>Gurruchaga 410</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1455,7 +1455,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Colocar columna para pedir traspaso de equipos</t>
+        </is>
+      </c>
       <c r="I14" t="n">
         <v>1</v>
       </c>
@@ -1466,7 +1470,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1475,10 +1479,10 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.442667</v>
+        <v>-58.442601</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.597977</v>
+        <v>-34.597923</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-05 08:03:59)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3626,27 +3626,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-522</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Uruguay 1090</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Reclaman columna corroida y rienda fuera de norma pero no se ve en la foto.</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3679,18 +3679,18 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.387175</v>
+        <v>-58.434668</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.596</v>
+        <v>-34.571258</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3702,17 +3702,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3759,10 +3759,10 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.434668</v>
+        <v>-58.434194</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.571258</v>
+        <v>-34.571754</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3778,27 +3778,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>6478</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>JUJUY AV. 1647</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>808509387</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3835,93 +3835,17 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.434194</v>
+        <v>-58.401083</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.571754</v>
+        <v>-34.629397</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>6478</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>7/24/2025</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>JUJUY AV. 1647</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>808509387</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I46" t="n">
-        <v>1</v>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M46" t="n">
-        <v>-58.401083</v>
-      </c>
-      <c r="N46" t="n">
-        <v>-34.629397</v>
-      </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P46" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-06 07:05:54)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3851,6 +3851,82 @@
         </is>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>-546</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>8/5/2025</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Albarellos 3031</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>808720857</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I46" t="n">
+        <v>1</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M46" t="n">
+        <v>-58.511732</v>
+      </c>
+      <c r="N46" t="n">
+        <v>-34.578688</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-13 08:41:16)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -3550,7 +3550,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-516</t>
+          <t>6695</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3560,7 +3560,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Olazabal 4417</t>
+          <t>OLAZABAL AV. 4417</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-15 11:42:19)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3854,27 +3854,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3907,25 +3907,585 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M46" t="n">
+        <v>-58.440748</v>
+      </c>
+      <c r="N46" t="n">
+        <v>-34.63245</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>-540</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>7/31/2025</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Tejedor 1071</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>808615948</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I47" t="n">
+        <v>1</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M47" t="n">
+        <v>-58.44037</v>
+      </c>
+      <c r="N47" t="n">
+        <v>-34.632249</v>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>-542</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>8/1/2025</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Cramer 2141</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>808663881</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+        </is>
+      </c>
+      <c r="I48" t="n">
+        <v>1</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M48" t="n">
+        <v>-58.461582</v>
+      </c>
+      <c r="N48" t="n">
+        <v>-34.564296</v>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>-544</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>8/2/2025</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Vera 453</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>808669129</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Columna corroída en base</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
+        <v>1</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M49" t="n">
+        <v>-58.437239</v>
+      </c>
+      <c r="N49" t="n">
+        <v>-34.599438</v>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>-546</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>8/5/2025</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Albarellos 3031</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>808720857</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I50" t="n">
+        <v>1</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M50" t="n">
         <v>-58.511732</v>
       </c>
-      <c r="N46" t="n">
+      <c r="N50" t="n">
         <v>-34.578688</v>
       </c>
-      <c r="O46" t="inlineStr">
+      <c r="O50" t="inlineStr">
         <is>
           <t>Paternal</t>
         </is>
       </c>
-      <c r="P46" t="inlineStr">
+      <c r="P50" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>
       </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>-552</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>8/14/2025</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Catulo Castillo 2890</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>808973183</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I51" t="n">
+        <v>1</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr"/>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>-553</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>8/14/2025</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Holmberg 4002</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>808973192</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+        </is>
+      </c>
+      <c r="I52" t="n">
+        <v>1</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>-554</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>8/14/2025</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Lima Oeste 1697</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>808973197</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Columna inclinada</t>
+        </is>
+      </c>
+      <c r="I53" t="n">
+        <v>1</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>-555</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>8/14/2025</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Lima Oeste 1649</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>808973201</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>INCO</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I54" t="n">
+        <v>1</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-15 11:45:55)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -4290,10 +4290,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M51" t="inlineStr"/>
-      <c r="N51" t="inlineStr"/>
-      <c r="O51" t="inlineStr"/>
-      <c r="P51" t="inlineStr"/>
+      <c r="M51" t="n">
+        <v>-58.404058</v>
+      </c>
+      <c r="N51" t="n">
+        <v>-34.634341</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -4354,10 +4366,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr"/>
-      <c r="O52" t="inlineStr"/>
-      <c r="P52" t="inlineStr"/>
+      <c r="M52" t="n">
+        <v>-58.487821</v>
+      </c>
+      <c r="N52" t="n">
+        <v>-34.554603</v>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -4420,8 +4444,16 @@
       </c>
       <c r="M53" t="inlineStr"/>
       <c r="N53" t="inlineStr"/>
-      <c r="O53" t="inlineStr"/>
-      <c r="P53" t="inlineStr"/>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>No ubicado</t>
+        </is>
+      </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>No clasificado, consultar con mantenimiento</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -4484,8 +4516,16 @@
       </c>
       <c r="M54" t="inlineStr"/>
       <c r="N54" t="inlineStr"/>
-      <c r="O54" t="inlineStr"/>
-      <c r="P54" t="inlineStr"/>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>No ubicado</t>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>No clasificado, consultar con mantenimiento</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-22 08:55:12)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P54"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1346,27 +1346,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-247</t>
+          <t>-255</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>12/26/2024</t>
+          <t>1/8/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CONCORDIA /ALT/ 925</t>
+          <t>Gurruchaga 410</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>802055232</t>
+          <t>802393948</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Pasante con priroidad</t>
+          <t>Colocar columna para pedir traspaso de equipos</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1394,7 +1394,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1403,14 +1403,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.479695</v>
+        <v>-58.442601</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.622867</v>
+        <v>-34.597923</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1422,27 +1422,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-255</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1/8/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Gurruchaga 410</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>802393948</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1457,7 +1457,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de equipos</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1470,7 +1470,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1479,10 +1479,10 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.442601</v>
+        <v>-58.480871</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.597923</v>
+        <v>-34.616598</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1498,27 +1498,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1533,7 +1533,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1555,46 +1555,46 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.480871</v>
+        <v>-58.407076</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.616598</v>
+        <v>-34.616016</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1609,11 +1609,11 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1631,26 +1631,26 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.407076</v>
+        <v>-58.439727</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.616016</v>
+        <v>-34.556261</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1660,7 +1660,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>HERNANDEZ JOSE 1451</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1670,7 +1670,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1698,7 +1698,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1707,10 +1707,10 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.439727</v>
+        <v>-58.443936</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.556261</v>
+        <v>-34.560145</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1726,27 +1726,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>HERNANDEZ JOSE 1451</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1774,7 +1774,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1783,26 +1783,26 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.443936</v>
+        <v>-58.415566</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.560145</v>
+        <v>-34.613244</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>804161220</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1812,7 +1812,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Carlos Calvo 4009</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1822,7 +1822,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>804161220</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1859,14 +1859,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.415566</v>
+        <v>-58.422147</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.613244</v>
+        <v>-34.624736</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1878,7 +1878,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804161220</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Carlos Calvo 4009</t>
+          <t>Treinta y Tres Orientales 905</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1898,7 +1898,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804161220</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1935,10 +1935,10 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.422147</v>
+        <v>-58.423229</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.624736</v>
+        <v>-34.625103</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1954,17 +1954,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Treinta y Tres Orientales 905</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1974,7 +1974,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2011,14 +2011,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.423229</v>
+        <v>-58.418089</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.625103</v>
+        <v>-34.620313</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2030,7 +2030,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2040,7 +2040,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2050,7 +2050,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2087,10 +2087,10 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.418089</v>
+        <v>-58.427201</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.620313</v>
+        <v>-34.617131</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2106,7 +2106,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2116,7 +2116,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2126,7 +2126,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2163,14 +2163,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.427201</v>
+        <v>-58.414984</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.617131</v>
+        <v>-34.621386</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2182,27 +2182,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Conesa 2195</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2239,26 +2239,26 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.414984</v>
+        <v>-58.463015</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.621386</v>
+        <v>-34.564505</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2268,17 +2268,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Conesa 2195</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2315,14 +2315,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.463015</v>
+        <v>-58.507569</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.564505</v>
+        <v>-34.579623</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2334,27 +2334,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,11 +2369,11 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2391,14 +2391,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.507569</v>
+        <v>-58.466348</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.579623</v>
+        <v>-34.556028</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2410,27 +2410,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2467,14 +2467,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.466348</v>
+        <v>-58.497446</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.556028</v>
+        <v>-34.583455</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2486,27 +2486,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2539,18 +2539,18 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.497446</v>
+        <v>-58.454065</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.583455</v>
+        <v>-34.57105</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2562,27 +2562,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2615,30 +2615,30 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.454065</v>
+        <v>-58.436255</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.57105</v>
+        <v>-34.567733</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2648,7 +2648,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2691,14 +2691,14 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.436255</v>
+        <v>-58.43247</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.567733</v>
+        <v>-34.566492</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2714,27 +2714,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>6180</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>5/4/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>AZARA 15</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>805655333</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2767,18 +2767,18 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.43247</v>
+        <v>-58.372751</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.566492</v>
+        <v>-34.631917</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -2790,27 +2790,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>6180</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/4/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>AZARA 15</t>
+          <t>Soldado de la Independencia 1298</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805655333</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada - Con fuente teco</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2847,36 +2847,36 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.372751</v>
+        <v>-58.440507</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.631917</v>
+        <v>-34.564016</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Soldado de la Independencia 1298</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2886,7 +2886,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada - Con fuente teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2914,7 +2914,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2923,10 +2923,10 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.440507</v>
+        <v>-58.44191</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.564016</v>
+        <v>-34.564245</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2942,27 +2942,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2995,50 +2995,50 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.44191</v>
+        <v>-58.438744</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.564245</v>
+        <v>-34.629929</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3071,30 +3071,30 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.438744</v>
+        <v>-58.473937</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.629929</v>
+        <v>-34.557355</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-508</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3104,7 +3104,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Moldes 2463</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3114,7 +3114,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808194234</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3142,7 +3142,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3151,10 +3151,10 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.473937</v>
+        <v>-58.462281</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.557355</v>
+        <v>-34.560321</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3170,7 +3170,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-508</t>
+          <t>-509</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3180,17 +3180,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Moldes 2463</t>
+          <t>Paso 58</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808194234</t>
+          <t>808194240</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3218,7 +3218,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -3227,26 +3227,26 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.462281</v>
+        <v>-58.403422</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.560321</v>
+        <v>-34.609195</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-509</t>
+          <t>-510</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3256,7 +3256,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Paso 58</t>
+          <t>Larrea 590</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3266,7 +3266,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808194240</t>
+          <t>808194254</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3294,7 +3294,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3303,10 +3303,10 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.403422</v>
+        <v>-58.402353</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.609195</v>
+        <v>-34.602205</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3322,27 +3322,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-510</t>
+          <t>6580</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Larrea 590</t>
+          <t>Ciudad de la Paz 3742</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>808194254</t>
+          <t>808240230</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3370,7 +3370,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3379,26 +3379,26 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.402353</v>
+        <v>-58.470347</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.602205</v>
+        <v>-34.547965</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6580</t>
+          <t>6486</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3408,17 +3408,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 3742</t>
+          <t>BILBAO, FRANCISCO 2442</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>808240230</t>
+          <t>808243829</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3455,46 +3455,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.470347</v>
+        <v>-58.460522</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.547965</v>
+        <v>-34.635514</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6486</t>
+          <t>6695</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2442</t>
+          <t>OLAZABAL AV. 4417</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>808243829</t>
+          <t>808373646</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3531,46 +3531,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.460522</v>
+        <v>-58.478941</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.635514</v>
+        <v>-34.57242</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6695</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>OLAZABAL AV. 4417</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>808373646</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3607,36 +3607,36 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.478941</v>
+        <v>-58.434668</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.57242</v>
+        <v>-34.571258</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3646,7 +3646,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3683,10 +3683,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.434668</v>
+        <v>-58.434194</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.571258</v>
+        <v>-34.571754</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3702,27 +3702,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>6478</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>JUJUY AV. 1647</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>808509387</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3759,14 +3759,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.434194</v>
+        <v>-58.401083</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.571754</v>
+        <v>-34.629397</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3778,27 +3778,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6478</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>JUJUY AV. 1647</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808509387</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3831,18 +3831,18 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.401083</v>
+        <v>-58.440748</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.629397</v>
+        <v>-34.63245</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3854,7 +3854,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3864,7 +3864,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3874,7 +3874,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3907,14 +3907,14 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.440748</v>
+        <v>-58.44037</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.63245</v>
+        <v>-34.632249</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3930,27 +3930,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-542</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Cramer 2141</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3987,46 +3987,46 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.44037</v>
+        <v>-58.461582</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.632249</v>
+        <v>-34.564296</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-542</t>
+          <t>-544</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>8/2/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Cramer 2141</t>
+          <t>Vera 453</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>808669129</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Columna corroída en base</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4063,46 +4063,46 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.461582</v>
+        <v>-58.437239</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.564296</v>
+        <v>-34.599438</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-544</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>8/2/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Vera 453</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808669129</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Columna corroída en base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4139,46 +4139,46 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.437239</v>
+        <v>-58.511732</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.599438</v>
+        <v>-34.578688</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4215,26 +4215,26 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.511732</v>
+        <v>-58.404058</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.578688</v>
+        <v>-34.634341</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4244,17 +4244,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4291,26 +4291,26 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.404058</v>
+        <v>-58.487821</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.634341</v>
+        <v>-34.554603</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4320,17 +4320,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Lima Oeste 1697</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4353,7 +4353,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4363,30 +4363,26 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M52" t="n">
-        <v>-58.487821</v>
-      </c>
-      <c r="N52" t="n">
-        <v>-34.554603</v>
-      </c>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4396,7 +4392,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Lima Oeste 1697</t>
+          <t>Lima Oeste 1649</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4406,7 +4402,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4421,7 +4417,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4429,7 +4425,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4439,7 +4435,7 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M53" t="inlineStr"/>
@@ -4450,78 +4446,6 @@
         </is>
       </c>
       <c r="P53" t="inlineStr">
-        <is>
-          <t>No clasificado, consultar con mantenimiento</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>-555</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Lima Oeste 1649</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>808973201</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I54" t="n">
-        <v>1</v>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L54" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr"/>
-      <c r="N54" t="inlineStr"/>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>No ubicado</t>
-        </is>
-      </c>
-      <c r="P54" t="inlineStr">
         <is>
           <t>No clasificado, consultar con mantenimiento</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-26 15:13:09)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P53"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4006,27 +4006,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-544</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>8/2/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Vera 453</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808669129</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Columna corroída en base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4063,46 +4063,46 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.437239</v>
+        <v>-58.511732</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.599438</v>
+        <v>-34.578688</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4139,26 +4139,26 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.511732</v>
+        <v>-58.404058</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.578688</v>
+        <v>-34.634341</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4168,17 +4168,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4215,26 +4215,26 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.404058</v>
+        <v>-58.487821</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.634341</v>
+        <v>-34.554603</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4244,17 +4244,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Lima Oeste 1697</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4277,7 +4277,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4287,30 +4287,26 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M51" t="n">
-        <v>-58.487821</v>
-      </c>
-      <c r="N51" t="n">
-        <v>-34.554603</v>
-      </c>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr"/>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4320,7 +4316,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Lima Oeste 1697</t>
+          <t>Lima Oeste 1649</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4330,7 +4326,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4345,7 +4341,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4353,7 +4349,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4363,7 +4359,7 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M52" t="inlineStr"/>
@@ -4374,78 +4370,6 @@
         </is>
       </c>
       <c r="P52" t="inlineStr">
-        <is>
-          <t>No clasificado, consultar con mantenimiento</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>-555</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Lima Oeste 1649</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>808973201</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I53" t="n">
-        <v>1</v>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr"/>
-      <c r="N53" t="inlineStr"/>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>No ubicado</t>
-        </is>
-      </c>
-      <c r="P53" t="inlineStr">
         <is>
           <t>No clasificado, consultar con mantenimiento</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-28 13:14:06)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -518,27 +518,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -553,11 +553,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -571,18 +571,18 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.390269</v>
+        <v>-58.438744</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.625079</v>
+        <v>-34.629929</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -594,17 +594,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BAEZ 489</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -651,46 +651,46 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.432978</v>
+        <v>-58.44191</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.57094</v>
+        <v>-34.564245</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Soldado de la Independencia 1298</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -703,9 +703,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Picada - Con fuente teco</t>
+        </is>
+      </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -714,7 +718,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -723,46 +727,46 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.39894</v>
+        <v>-58.440507</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.591084</v>
+        <v>-34.564016</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-28</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2/20/2024</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ZABALA /ALT/ 2836</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>780340125</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -777,11 +781,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>ZABALA 2836 - Reemplazar C114</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -795,50 +799,50 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.452298</v>
+        <v>-58.43247</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.572157</v>
+        <v>-34.566492</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -853,11 +857,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -875,14 +879,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.390198</v>
+        <v>-58.436255</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.637568</v>
+        <v>-34.567733</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -894,27 +898,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -927,9 +931,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -943,40 +951,40 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.400047</v>
+        <v>-58.454065</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.586358</v>
+        <v>-34.57105</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -986,7 +994,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1001,11 +1009,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1023,10 +1031,10 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.499823</v>
+        <v>-58.497446</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.563809</v>
+        <v>-34.583455</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1042,27 +1050,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1077,11 +1085,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1099,46 +1107,46 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.386058</v>
+        <v>-58.466348</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.621209</v>
+        <v>-34.556028</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1153,7 +1161,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1175,46 +1183,46 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.395465</v>
+        <v>-58.507569</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.622784</v>
+        <v>-34.579623</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Conesa 2195</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1229,7 +1237,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1251,46 +1259,46 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.394079</v>
+        <v>-58.463015</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.61051</v>
+        <v>-34.564505</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1305,7 +1313,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1327,14 +1335,14 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.404265</v>
+        <v>-58.414984</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.623154</v>
+        <v>-34.621386</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1346,27 +1354,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-255</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1/8/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Gurruchaga 410</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>802393948</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1381,11 +1389,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de equipos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1394,7 +1402,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1403,46 +1411,46 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.442601</v>
+        <v>-58.427201</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.597923</v>
+        <v>-34.617131</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1457,11 +1465,11 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1479,46 +1487,46 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.480871</v>
+        <v>-58.418089</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.616598</v>
+        <v>-34.620313</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Treinta y Tres Orientales 905</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1533,11 +1541,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1555,14 +1563,14 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.407076</v>
+        <v>-58.423229</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.616016</v>
+        <v>-34.625103</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1574,27 +1582,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804161220</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Carlos Calvo 4009</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804161220</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1609,7 +1617,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1631,46 +1639,46 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.439727</v>
+        <v>-58.422147</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.556261</v>
+        <v>-34.624736</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>HERNANDEZ JOSE 1451</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1685,7 +1693,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1698,7 +1706,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1707,46 +1715,46 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.443936</v>
+        <v>-58.415566</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.560145</v>
+        <v>-34.613244</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1761,7 +1769,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1783,46 +1791,46 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.415566</v>
+        <v>-58.439727</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.613244</v>
+        <v>-34.556261</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804161220</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Carlos Calvo 4009</t>
+          <t>HERNANDEZ JOSE 1451</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804161220</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1837,7 +1845,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1850,7 +1858,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1859,46 +1867,46 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.422147</v>
+        <v>-58.443936</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.624736</v>
+        <v>-34.560145</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Treinta y Tres Orientales 905</t>
+          <t>BAEZ 489</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1913,11 +1921,11 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1935,14 +1943,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.423229</v>
+        <v>-58.432978</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.625103</v>
+        <v>-34.57094</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1954,27 +1962,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1989,7 +1997,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2011,46 +2019,46 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.418089</v>
+        <v>-58.499823</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.620313</v>
+        <v>-34.563809</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2063,11 +2071,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H22" t="inlineStr"/>
       <c r="I22" t="n">
         <v>0</v>
       </c>
@@ -2087,14 +2091,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.427201</v>
+        <v>-58.400047</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.617131</v>
+        <v>-34.586358</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2106,27 +2110,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>6695</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>OLAZABAL AV. 4417</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>808373646</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2145,7 +2149,7 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2163,46 +2167,46 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.414984</v>
+        <v>-58.478941</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.621386</v>
+        <v>-34.57242</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>6580</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Conesa 2195</t>
+          <t>Ciudad de la Paz 3742</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>808240230</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2221,7 +2225,7 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2239,14 +2243,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.463015</v>
+        <v>-58.470347</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.564505</v>
+        <v>-34.547965</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2258,27 +2262,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>6486</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>BILBAO, FRANCISCO 2442</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>808243829</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,11 +2297,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2315,46 +2319,46 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.507569</v>
+        <v>-58.460522</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.579623</v>
+        <v>-34.635514</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>6478</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>JUJUY AV. 1647</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>808509387</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2391,46 +2395,46 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.466348</v>
+        <v>-58.401083</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.556028</v>
+        <v>-34.629397</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>6180</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>5/4/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>AZARA 15</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>805655333</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,7 +2449,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2467,46 +2471,46 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.497446</v>
+        <v>-58.372751</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.583455</v>
+        <v>-34.631917</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Lima Oeste 1649</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2539,50 +2543,46 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M28" t="n">
-        <v>-58.454065</v>
-      </c>
-      <c r="N28" t="n">
-        <v>-34.57105</v>
-      </c>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Lima Oeste 1697</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2605,7 +2605,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2615,50 +2615,46 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M29" t="n">
-        <v>-58.436255</v>
-      </c>
-      <c r="N29" t="n">
-        <v>-34.567733</v>
-      </c>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2673,7 +2669,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2691,40 +2687,40 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.43247</v>
+        <v>-58.487821</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.566492</v>
+        <v>-34.554603</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>6180</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/4/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>AZARA 15</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2734,7 +2730,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805655333</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2771,10 +2767,10 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.372751</v>
+        <v>-58.404058</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.631917</v>
+        <v>-34.634341</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2790,27 +2786,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Soldado de la Independencia 1298</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2821,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada - Con fuente teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2838,7 +2834,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2847,14 +2843,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.440507</v>
+        <v>-58.511732</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.564016</v>
+        <v>-34.578688</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2866,27 +2862,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>-542</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>Cramer 2141</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2901,7 +2897,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2923,14 +2919,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.44191</v>
+        <v>-58.461582</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.564245</v>
+        <v>-34.564296</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2942,17 +2938,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2962,7 +2958,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2977,7 +2973,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2995,14 +2991,14 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.438744</v>
+        <v>-58.44037</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.629929</v>
+        <v>-34.632249</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3018,27 +3014,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3071,50 +3067,50 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.473937</v>
+        <v>-58.440748</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.557355</v>
+        <v>-34.63245</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-508</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Moldes 2463</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808194234</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3142,7 +3138,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3151,46 +3147,46 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.462281</v>
+        <v>-58.434194</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.560321</v>
+        <v>-34.571754</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-509</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Paso 58</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808194240</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3227,14 +3223,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.403422</v>
+        <v>-58.434668</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.609195</v>
+        <v>-34.571258</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3322,27 +3318,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6580</t>
+          <t>-509</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 3742</t>
+          <t>Paso 58</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>808240230</t>
+          <t>808194240</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3379,46 +3375,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.470347</v>
+        <v>-58.403422</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.547965</v>
+        <v>-34.609195</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6486</t>
+          <t>-508</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2442</t>
+          <t>Moldes 2463</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>808243829</t>
+          <t>808194234</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3446,7 +3442,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3455,36 +3451,36 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.460522</v>
+        <v>-58.462281</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.635514</v>
+        <v>-34.560321</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6695</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>OLAZABAL AV. 4417</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3494,7 +3490,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>808373646</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3531,14 +3527,14 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.478941</v>
+        <v>-58.473937</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.57242</v>
+        <v>-34.557355</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3550,27 +3546,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3585,11 +3581,11 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3607,14 +3603,14 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.434668</v>
+        <v>-58.390198</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.571258</v>
+        <v>-34.637568</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3626,27 +3622,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-28</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>2/20/2024</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>ZABALA /ALT/ 2836</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>780340125</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3661,11 +3657,11 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>ZABALA 2836 - Reemplazar C114</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3683,46 +3679,46 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.434194</v>
+        <v>-58.452298</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.571754</v>
+        <v>-34.572157</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6478</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>JUJUY AV. 1647</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808509387</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3737,7 +3733,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3759,14 +3755,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.401083</v>
+        <v>-58.407076</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.629397</v>
+        <v>-34.616016</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3778,27 +3774,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3813,7 +3809,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3831,50 +3827,50 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.440748</v>
+        <v>-58.480871</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.63245</v>
+        <v>-34.616598</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-255</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>1/8/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Gurruchaga 410</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>802393948</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3889,7 +3885,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna para pedir traspaso de equipos</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3902,7 +3898,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3911,46 +3907,46 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.44037</v>
+        <v>-58.442601</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.632249</v>
+        <v>-34.597923</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-542</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Cramer 2141</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3963,13 +3959,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
-        </is>
-      </c>
+      <c r="H47" t="inlineStr"/>
       <c r="I47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -3987,46 +3979,46 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.461582</v>
+        <v>-58.39894</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.564296</v>
+        <v>-34.591084</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,11 +4033,11 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -4063,46 +4055,46 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.511732</v>
+        <v>-58.390269</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.578688</v>
+        <v>-34.625079</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-111</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>7/12/2024</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>CATAMARCA /ALT/ 1127</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>790298182</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4117,11 +4109,11 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -4139,10 +4131,10 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.404058</v>
+        <v>-58.404265</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.634341</v>
+        <v>-34.623154</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4158,27 +4150,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4193,11 +4185,11 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -4215,46 +4207,46 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.487821</v>
+        <v>-58.394079</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.554603</v>
+        <v>-34.61051</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Lima Oeste 1697</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4269,15 +4261,15 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4287,36 +4279,40 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr"/>
-      <c r="N51" t="inlineStr"/>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M51" t="n">
+        <v>-58.395465</v>
+      </c>
+      <c r="N51" t="n">
+        <v>-34.622784</v>
+      </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Lima Oeste 1649</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4326,7 +4322,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4341,11 +4337,11 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -4362,16 +4358,20 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr"/>
+      <c r="M52" t="n">
+        <v>-58.386058</v>
+      </c>
+      <c r="N52" t="n">
+        <v>-34.621209</v>
+      </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-28 14:59:14)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -518,27 +518,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -553,11 +553,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -571,18 +571,18 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.438744</v>
+        <v>-58.390269</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.629929</v>
+        <v>-34.625079</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -594,17 +594,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>BAEZ 489</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -651,46 +651,46 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.44191</v>
+        <v>-58.432978</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.564245</v>
+        <v>-34.57094</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Soldado de la Independencia 1298</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -703,13 +703,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Picada - Con fuente teco</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -718,7 +714,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -727,46 +723,46 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.440507</v>
+        <v>-58.39894</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.564016</v>
+        <v>-34.591084</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>-28</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>2/20/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>ZABALA /ALT/ 2836</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>780340125</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -781,11 +777,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>ZABALA 2836 - Reemplazar C114</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -799,50 +795,50 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.43247</v>
+        <v>-58.452298</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.566492</v>
+        <v>-34.572157</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -857,11 +853,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -879,14 +875,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.436255</v>
+        <v>-58.390198</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.567733</v>
+        <v>-34.637568</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -898,27 +894,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -931,13 +927,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -951,40 +943,40 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.454065</v>
+        <v>-58.400047</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.57105</v>
+        <v>-34.586358</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -994,7 +986,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1009,11 +1001,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1031,10 +1023,10 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.497446</v>
+        <v>-58.499823</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.583455</v>
+        <v>-34.563809</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1050,27 +1042,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1085,11 +1077,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1107,46 +1099,46 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.466348</v>
+        <v>-58.386058</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.556028</v>
+        <v>-34.621209</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1161,7 +1153,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1183,46 +1175,46 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.507569</v>
+        <v>-58.395465</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.579623</v>
+        <v>-34.622784</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Conesa 2195</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1237,7 +1229,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1259,46 +1251,46 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.463015</v>
+        <v>-58.394079</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.564505</v>
+        <v>-34.61051</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>-111</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>7/12/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>CATAMARCA /ALT/ 1127</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>790298182</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1313,7 +1305,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1335,14 +1327,14 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.414984</v>
+        <v>-58.404265</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.621386</v>
+        <v>-34.623154</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1354,27 +1346,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>-255</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>1/8/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Gurruchaga 410</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>802393948</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1389,11 +1381,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna para pedir traspaso de equipos</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1402,7 +1394,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1411,46 +1403,46 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.427201</v>
+        <v>-58.442601</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.617131</v>
+        <v>-34.597923</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1465,11 +1457,11 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1487,46 +1479,46 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.418089</v>
+        <v>-58.480871</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.620313</v>
+        <v>-34.616598</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Treinta y Tres Orientales 905</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1541,11 +1533,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1563,14 +1555,14 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.423229</v>
+        <v>-58.407076</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.625103</v>
+        <v>-34.616016</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1582,27 +1574,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>804161220</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Carlos Calvo 4009</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804161220</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1617,7 +1609,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1639,46 +1631,46 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.422147</v>
+        <v>-58.439727</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.624736</v>
+        <v>-34.556261</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>HERNANDEZ JOSE 1451</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1693,7 +1685,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1706,7 +1698,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1715,46 +1707,46 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.415566</v>
+        <v>-58.443936</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.613244</v>
+        <v>-34.560145</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1769,7 +1761,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1791,46 +1783,46 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.439727</v>
+        <v>-58.415566</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.556261</v>
+        <v>-34.613244</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>804161220</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>HERNANDEZ JOSE 1451</t>
+          <t>Carlos Calvo 4009</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>804161220</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1845,7 +1837,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1858,7 +1850,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1867,46 +1859,46 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.443936</v>
+        <v>-58.422147</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.560145</v>
+        <v>-34.624736</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>BAEZ 489</t>
+          <t>Treinta y Tres Orientales 905</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1921,11 +1913,11 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1943,14 +1935,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.432978</v>
+        <v>-58.423229</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.57094</v>
+        <v>-34.625103</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1962,27 +1954,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1997,7 +1989,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2019,46 +2011,46 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.499823</v>
+        <v>-58.418089</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.563809</v>
+        <v>-34.620313</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2071,7 +2063,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I22" t="n">
         <v>0</v>
       </c>
@@ -2091,14 +2087,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.400047</v>
+        <v>-58.427201</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.586358</v>
+        <v>-34.617131</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2110,27 +2106,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>6695</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>OLAZABAL AV. 4417</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>808373646</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2149,7 +2145,7 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2167,46 +2163,46 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.478941</v>
+        <v>-58.414984</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.57242</v>
+        <v>-34.621386</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>6580</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 3742</t>
+          <t>Conesa 2195</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>808240230</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2225,7 +2221,7 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2243,14 +2239,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.470347</v>
+        <v>-58.463015</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.547965</v>
+        <v>-34.564505</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2262,27 +2258,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>6486</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2442</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>808243829</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2297,11 +2293,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2319,46 +2315,46 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.460522</v>
+        <v>-58.507569</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.635514</v>
+        <v>-34.579623</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>6478</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>JUJUY AV. 1647</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>808509387</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2395,46 +2391,46 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.401083</v>
+        <v>-58.466348</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.629397</v>
+        <v>-34.556028</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6180</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/4/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>AZARA 15</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805655333</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2449,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2471,46 +2467,46 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.372751</v>
+        <v>-58.497446</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.631917</v>
+        <v>-34.583455</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Lima Oeste 1649</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2543,46 +2539,50 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr"/>
-      <c r="N28" t="inlineStr"/>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M28" t="n">
+        <v>-58.454065</v>
+      </c>
+      <c r="N28" t="n">
+        <v>-34.57105</v>
+      </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Lima Oeste 1697</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2605,7 +2605,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2615,46 +2615,50 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M29" t="n">
+        <v>-58.436255</v>
+      </c>
+      <c r="N29" t="n">
+        <v>-34.567733</v>
+      </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2669,7 +2673,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2687,40 +2691,40 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.487821</v>
+        <v>-58.43247</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.554603</v>
+        <v>-34.566492</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>6180</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/4/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>AZARA 15</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2730,7 +2734,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>805655333</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2767,10 +2771,10 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.404058</v>
+        <v>-58.372751</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.634341</v>
+        <v>-34.631917</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2786,27 +2790,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Soldado de la Independencia 1298</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2821,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada - Con fuente teco</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2834,7 +2838,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2843,14 +2847,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.511732</v>
+        <v>-58.440507</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.578688</v>
+        <v>-34.564016</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2862,27 +2866,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-542</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Cramer 2141</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2897,7 +2901,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2919,14 +2923,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.461582</v>
+        <v>-58.44191</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.564296</v>
+        <v>-34.564245</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2938,17 +2942,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2958,7 +2962,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2973,7 +2977,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2991,14 +2995,14 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.44037</v>
+        <v>-58.438744</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.632249</v>
+        <v>-34.629929</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3014,27 +3018,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3067,50 +3071,50 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.440748</v>
+        <v>-58.473937</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.63245</v>
+        <v>-34.557355</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-508</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Moldes 2463</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>808194234</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3138,7 +3142,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3147,46 +3151,46 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.434194</v>
+        <v>-58.462281</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.571754</v>
+        <v>-34.560321</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-509</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Paso 58</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>808194240</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3223,14 +3227,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.434668</v>
+        <v>-58.403422</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.571258</v>
+        <v>-34.609195</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3318,27 +3322,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-509</t>
+          <t>6580</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Paso 58</t>
+          <t>Ciudad de la Paz 3742</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>808194240</t>
+          <t>808240230</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3375,46 +3379,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.403422</v>
+        <v>-58.470347</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.609195</v>
+        <v>-34.547965</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-508</t>
+          <t>6486</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Moldes 2463</t>
+          <t>BILBAO, FRANCISCO 2442</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>808194234</t>
+          <t>808243829</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3442,7 +3446,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3451,36 +3455,36 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.462281</v>
+        <v>-58.460522</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.560321</v>
+        <v>-34.635514</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>6695</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>OLAZABAL AV. 4417</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3490,7 +3494,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808373646</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3527,14 +3531,14 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.473937</v>
+        <v>-58.478941</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.557355</v>
+        <v>-34.57242</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3546,27 +3550,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3581,11 +3585,11 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3603,14 +3607,14 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.390198</v>
+        <v>-58.434668</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.637568</v>
+        <v>-34.571258</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3622,27 +3626,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-28</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2/20/2024</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ZABALA /ALT/ 2836</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>780340125</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3657,11 +3661,11 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>ZABALA 2836 - Reemplazar C114</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3679,46 +3683,46 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.452298</v>
+        <v>-58.434194</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.572157</v>
+        <v>-34.571754</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>6478</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>JUJUY AV. 1647</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>808509387</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3733,7 +3737,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3755,14 +3759,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.407076</v>
+        <v>-58.401083</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.616016</v>
+        <v>-34.629397</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3774,27 +3778,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3809,7 +3813,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3827,50 +3831,50 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.480871</v>
+        <v>-58.440748</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.616598</v>
+        <v>-34.63245</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-255</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>1/8/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Gurruchaga 410</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>802393948</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3885,7 +3889,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de equipos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3898,7 +3902,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3907,46 +3911,46 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.442601</v>
+        <v>-58.44037</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.597923</v>
+        <v>-34.632249</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>-542</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Cramer 2141</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3959,9 +3963,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H47" t="inlineStr"/>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+        </is>
+      </c>
       <c r="I47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -3979,46 +3987,46 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.39894</v>
+        <v>-58.461582</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.591084</v>
+        <v>-34.564296</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4033,11 +4041,11 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -4055,46 +4063,46 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.390269</v>
+        <v>-58.511732</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.625079</v>
+        <v>-34.578688</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4109,11 +4117,11 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -4131,10 +4139,10 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.404265</v>
+        <v>-58.404058</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.623154</v>
+        <v>-34.634341</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4150,27 +4158,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,11 +4193,11 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -4207,46 +4215,46 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.394079</v>
+        <v>-58.487821</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.61051</v>
+        <v>-34.554603</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Lima Oeste 1697</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,15 +4269,15 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4279,40 +4287,36 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M51" t="n">
-        <v>-58.395465</v>
-      </c>
-      <c r="N51" t="n">
-        <v>-34.622784</v>
-      </c>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr"/>
       <c r="O51" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Lima Oeste 1649</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4322,7 +4326,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,11 +4341,11 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -4358,20 +4362,16 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M52" t="n">
-        <v>-58.386058</v>
-      </c>
-      <c r="N52" t="n">
-        <v>-34.621209</v>
-      </c>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
       <c r="O52" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-03 22:05:40)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P52"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1802,7 +1802,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804161220</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1812,7 +1812,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Carlos Calvo 4009</t>
+          <t>Treinta y Tres Orientales 905</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1822,7 +1822,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804161220</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1859,10 +1859,10 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.422147</v>
+        <v>-58.423229</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.624736</v>
+        <v>-34.625103</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1878,17 +1878,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Treinta y Tres Orientales 905</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1898,7 +1898,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1935,14 +1935,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.423229</v>
+        <v>-58.418089</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.625103</v>
+        <v>-34.620313</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1954,7 +1954,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1964,7 +1964,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1974,7 +1974,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2011,10 +2011,10 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.418089</v>
+        <v>-58.427201</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.620313</v>
+        <v>-34.617131</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2030,7 +2030,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2040,7 +2040,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2050,7 +2050,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2087,14 +2087,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.427201</v>
+        <v>-58.414984</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.617131</v>
+        <v>-34.621386</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2106,27 +2106,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Conesa 2195</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2163,26 +2163,26 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.414984</v>
+        <v>-58.463015</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.621386</v>
+        <v>-34.564505</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2192,17 +2192,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Conesa 2195</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2239,14 +2239,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.463015</v>
+        <v>-58.507569</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.564505</v>
+        <v>-34.579623</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2258,27 +2258,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,11 +2293,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2315,14 +2315,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.507569</v>
+        <v>-58.466348</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.579623</v>
+        <v>-34.556028</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2334,27 +2334,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2391,14 +2391,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.466348</v>
+        <v>-58.497446</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.556028</v>
+        <v>-34.583455</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2410,27 +2410,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2463,18 +2463,18 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.497446</v>
+        <v>-58.454065</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.583455</v>
+        <v>-34.57105</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2486,27 +2486,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2539,30 +2539,30 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.454065</v>
+        <v>-58.436255</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.57105</v>
+        <v>-34.567733</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2572,7 +2572,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2615,14 +2615,14 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.436255</v>
+        <v>-58.43247</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.567733</v>
+        <v>-34.566492</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2638,27 +2638,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>6180</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>5/4/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>AZARA 15</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>805655333</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2691,18 +2691,18 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.43247</v>
+        <v>-58.372751</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.566492</v>
+        <v>-34.631917</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2714,27 +2714,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>6180</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/4/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>AZARA 15</t>
+          <t>Soldado de la Independencia 1298</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805655333</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada - Con fuente teco</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2762,7 +2762,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2771,36 +2771,36 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.372751</v>
+        <v>-58.440507</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.631917</v>
+        <v>-34.564016</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Soldado de la Independencia 1298</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2810,7 +2810,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada - Con fuente teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2847,10 +2847,10 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.440507</v>
+        <v>-58.44191</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.564016</v>
+        <v>-34.564245</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2866,27 +2866,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2919,50 +2919,50 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.44191</v>
+        <v>-58.438744</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.564245</v>
+        <v>-34.629929</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2995,30 +2995,30 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.438744</v>
+        <v>-58.473937</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.629929</v>
+        <v>-34.557355</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-508</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3028,7 +3028,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Moldes 2463</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808194234</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -3075,10 +3075,10 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.473937</v>
+        <v>-58.462281</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.557355</v>
+        <v>-34.560321</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -3094,7 +3094,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-508</t>
+          <t>-509</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3104,17 +3104,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Moldes 2463</t>
+          <t>Paso 58</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808194234</t>
+          <t>808194240</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3142,7 +3142,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3151,26 +3151,26 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.462281</v>
+        <v>-58.403422</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.560321</v>
+        <v>-34.609195</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-509</t>
+          <t>-510</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3180,7 +3180,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Paso 58</t>
+          <t>Larrea 590</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -3190,7 +3190,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808194240</t>
+          <t>808194254</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3218,7 +3218,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -3227,10 +3227,10 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.403422</v>
+        <v>-58.402353</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.609195</v>
+        <v>-34.602205</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -3246,27 +3246,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-510</t>
+          <t>6580</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Larrea 590</t>
+          <t>Ciudad de la Paz 3742</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808194254</t>
+          <t>808240230</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3294,7 +3294,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3303,26 +3303,26 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.402353</v>
+        <v>-58.470347</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.602205</v>
+        <v>-34.547965</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6580</t>
+          <t>6486</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3332,17 +3332,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 3742</t>
+          <t>BILBAO, FRANCISCO 2442</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>808240230</t>
+          <t>808243829</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3379,46 +3379,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.470347</v>
+        <v>-58.460522</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.547965</v>
+        <v>-34.635514</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6486</t>
+          <t>6695</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2442</t>
+          <t>OLAZABAL AV. 4417</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>808243829</t>
+          <t>808373646</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3455,46 +3455,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.460522</v>
+        <v>-58.478941</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.635514</v>
+        <v>-34.57242</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6695</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>OLAZABAL AV. 4417</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>808373646</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3531,36 +3531,36 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.478941</v>
+        <v>-58.434668</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.57242</v>
+        <v>-34.571258</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3570,7 +3570,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3607,10 +3607,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.434668</v>
+        <v>-58.434194</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.571258</v>
+        <v>-34.571754</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3626,27 +3626,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>6478</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>JUJUY AV. 1647</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>808509387</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3683,14 +3683,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.434194</v>
+        <v>-58.401083</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.571754</v>
+        <v>-34.629397</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3702,27 +3702,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6478</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>JUJUY AV. 1647</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808509387</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3755,18 +3755,18 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.401083</v>
+        <v>-58.440748</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.629397</v>
+        <v>-34.63245</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3778,7 +3778,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3798,7 +3798,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3831,14 +3831,14 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.440748</v>
+        <v>-58.44037</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.63245</v>
+        <v>-34.632249</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3854,27 +3854,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-542</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Cramer 2141</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3911,46 +3911,46 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.44037</v>
+        <v>-58.461582</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.632249</v>
+        <v>-34.564296</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-542</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Cramer 2141</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3987,14 +3987,14 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.461582</v>
+        <v>-58.511732</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.564296</v>
+        <v>-34.578688</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -4006,27 +4006,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4063,26 +4063,26 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.511732</v>
+        <v>-58.404058</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.578688</v>
+        <v>-34.634341</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4092,17 +4092,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4139,26 +4139,26 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.404058</v>
+        <v>-58.487821</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.634341</v>
+        <v>-34.554603</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4168,17 +4168,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Lima Oeste 1697</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4201,7 +4201,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4211,30 +4211,26 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M50" t="n">
-        <v>-58.487821</v>
-      </c>
-      <c r="N50" t="n">
-        <v>-34.554603</v>
-      </c>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4244,7 +4240,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Lima Oeste 1697</t>
+          <t>Lima Oeste 1649</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -4254,7 +4250,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4269,7 +4265,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4277,7 +4273,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4287,7 +4283,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="inlineStr"/>
@@ -4298,78 +4294,6 @@
         </is>
       </c>
       <c r="P51" t="inlineStr">
-        <is>
-          <t>No clasificado, consultar con mantenimiento</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>-555</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Lima Oeste 1649</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>808973201</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I52" t="n">
-        <v>1</v>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr"/>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>No ubicado</t>
-        </is>
-      </c>
-      <c r="P52" t="inlineStr">
         <is>
           <t>No clasificado, consultar con mantenimiento</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-04 08:03:48)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2638,27 +2638,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>6180</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/4/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>AZARA 15</t>
+          <t>Soldado de la Independencia 1298</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805655333</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada - Con fuente teco</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2686,7 +2686,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2695,36 +2695,36 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.372751</v>
+        <v>-58.440507</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.631917</v>
+        <v>-34.564016</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Soldado de la Independencia 1298</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2734,7 +2734,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Picada - Con fuente teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2762,7 +2762,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2771,10 +2771,10 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.440507</v>
+        <v>-58.44191</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.564016</v>
+        <v>-34.564245</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2790,27 +2790,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2843,50 +2843,50 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.44191</v>
+        <v>-58.438744</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.564245</v>
+        <v>-34.629929</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2919,30 +2919,30 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.438744</v>
+        <v>-58.473937</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.629929</v>
+        <v>-34.557355</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-508</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2952,7 +2952,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Moldes 2463</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2962,7 +2962,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808194234</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2990,7 +2990,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2999,10 +2999,10 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.473937</v>
+        <v>-58.462281</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.557355</v>
+        <v>-34.560321</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3018,7 +3018,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-508</t>
+          <t>-509</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3028,17 +3028,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Moldes 2463</t>
+          <t>Paso 58</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808194234</t>
+          <t>808194240</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -3075,26 +3075,26 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.462281</v>
+        <v>-58.403422</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.560321</v>
+        <v>-34.609195</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-509</t>
+          <t>-510</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3104,7 +3104,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Paso 58</t>
+          <t>Larrea 590</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3114,7 +3114,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808194240</t>
+          <t>808194254</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3142,7 +3142,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3151,10 +3151,10 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.403422</v>
+        <v>-58.402353</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.609195</v>
+        <v>-34.602205</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3170,27 +3170,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-510</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Larrea 590</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808194254</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3218,7 +3218,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -3227,14 +3227,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.402353</v>
+        <v>-58.434668</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.602205</v>
+        <v>-34.571258</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3246,27 +3246,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6580</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 3742</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808240230</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3303,36 +3303,36 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.470347</v>
+        <v>-58.434194</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.547965</v>
+        <v>-34.571754</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6486</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2442</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3342,7 +3342,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>808243829</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3375,14 +3375,14 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.460522</v>
+        <v>-58.440748</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.635514</v>
+        <v>-34.63245</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3398,27 +3398,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6695</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>OLAZABAL AV. 4417</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>808373646</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3455,46 +3455,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.478941</v>
+        <v>-58.44037</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.57242</v>
+        <v>-34.632249</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-542</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Cramer 2141</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3531,46 +3531,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.434668</v>
+        <v>-58.461582</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.571258</v>
+        <v>-34.564296</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3607,36 +3607,36 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.434194</v>
+        <v>-58.511732</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.571754</v>
+        <v>-34.578688</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6478</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>JUJUY AV. 1647</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3646,7 +3646,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808509387</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3683,10 +3683,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.401083</v>
+        <v>-58.404058</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.629397</v>
+        <v>-34.634341</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3702,27 +3702,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3755,50 +3755,50 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.440748</v>
+        <v>-58.487821</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.63245</v>
+        <v>-34.554603</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Lima Oeste 1697</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3821,7 +3821,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3831,50 +3831,46 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M45" t="n">
-        <v>-58.44037</v>
-      </c>
-      <c r="N45" t="n">
-        <v>-34.632249</v>
-      </c>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-542</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Cramer 2141</t>
+          <t>Lima Oeste 1649</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3889,7 +3885,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3910,390 +3906,14 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M46" t="n">
-        <v>-58.461582</v>
-      </c>
-      <c r="N46" t="n">
-        <v>-34.564296</v>
-      </c>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>-546</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>8/5/2025</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Albarellos 3031</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>808720857</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I47" t="n">
-        <v>1</v>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M47" t="n">
-        <v>-58.511732</v>
-      </c>
-      <c r="N47" t="n">
-        <v>-34.578688</v>
-      </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P47" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>-552</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Catulo Castillo 2890</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>808973183</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I48" t="n">
-        <v>1</v>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M48" t="n">
-        <v>-58.404058</v>
-      </c>
-      <c r="N48" t="n">
-        <v>-34.634341</v>
-      </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>-553</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Holmberg 4002</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>808973192</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
-        </is>
-      </c>
-      <c r="I49" t="n">
-        <v>1</v>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M49" t="n">
-        <v>-58.487821</v>
-      </c>
-      <c r="N49" t="n">
-        <v>-34.554603</v>
-      </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P49" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>-554</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Lima Oeste 1697</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>808973197</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>Columna inclinada</t>
-        </is>
-      </c>
-      <c r="I50" t="n">
-        <v>1</v>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr"/>
-      <c r="N50" t="inlineStr"/>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>No ubicado</t>
-        </is>
-      </c>
-      <c r="P50" t="inlineStr">
-        <is>
-          <t>No clasificado, consultar con mantenimiento</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>-555</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Lima Oeste 1649</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>808973201</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I51" t="n">
-        <v>1</v>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr"/>
-      <c r="N51" t="inlineStr"/>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>No ubicado</t>
-        </is>
-      </c>
-      <c r="P51" t="inlineStr">
         <is>
           <t>No clasificado, consultar con mantenimiento</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-09 08:16:59)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -518,27 +518,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -553,11 +553,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -571,18 +571,18 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.390269</v>
+        <v>-58.438744</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.625079</v>
+        <v>-34.629929</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -594,17 +594,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BAEZ 489</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -651,46 +651,46 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.432978</v>
+        <v>-58.44191</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.57094</v>
+        <v>-34.564245</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Soldado de la Independencia 1298</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -703,9 +703,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Picada - Con fuente teco</t>
+        </is>
+      </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -714,7 +718,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -723,46 +727,46 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.39894</v>
+        <v>-58.440507</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.591084</v>
+        <v>-34.564016</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-28</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2/20/2024</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ZABALA /ALT/ 2836</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>780340125</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -777,11 +781,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>ZABALA 2836 - Reemplazar C114</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -795,50 +799,50 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.452298</v>
+        <v>-58.43247</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.572157</v>
+        <v>-34.566492</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -853,11 +857,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -875,14 +879,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.390198</v>
+        <v>-58.436255</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.637568</v>
+        <v>-34.567733</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -894,27 +898,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -927,9 +931,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -943,40 +951,40 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.400047</v>
+        <v>-58.454065</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.586358</v>
+        <v>-34.57105</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -986,7 +994,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1001,11 +1009,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1023,10 +1031,10 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.499823</v>
+        <v>-58.497446</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.563809</v>
+        <v>-34.583455</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1042,27 +1050,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1077,11 +1085,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1099,46 +1107,46 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.386058</v>
+        <v>-58.466348</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.621209</v>
+        <v>-34.556028</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1153,7 +1161,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1175,46 +1183,46 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.395465</v>
+        <v>-58.507569</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.622784</v>
+        <v>-34.579623</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Conesa 2195</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1229,7 +1237,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1251,46 +1259,46 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.394079</v>
+        <v>-58.463015</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.61051</v>
+        <v>-34.564505</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1305,7 +1313,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1327,14 +1335,14 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.404265</v>
+        <v>-58.414984</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.623154</v>
+        <v>-34.621386</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1346,27 +1354,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-255</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1/8/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Gurruchaga 410</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>802393948</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1381,11 +1389,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de equipos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1394,7 +1402,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1403,46 +1411,46 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.442601</v>
+        <v>-58.427201</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.597923</v>
+        <v>-34.617131</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1457,11 +1465,11 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1479,46 +1487,46 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.480871</v>
+        <v>-58.418089</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.616598</v>
+        <v>-34.620313</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Treinta y Tres Orientales 905</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1533,11 +1541,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1555,14 +1563,14 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.407076</v>
+        <v>-58.423229</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.616016</v>
+        <v>-34.625103</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1574,27 +1582,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1609,7 +1617,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1631,26 +1639,26 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.439727</v>
+        <v>-58.415566</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.556261</v>
+        <v>-34.613244</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1660,7 +1668,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>HERNANDEZ JOSE 1451</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1670,7 +1678,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1685,7 +1693,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1698,7 +1706,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1707,10 +1715,10 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.443936</v>
+        <v>-58.439727</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.560145</v>
+        <v>-34.556261</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1726,27 +1734,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>HERNANDEZ JOSE 1451</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1761,7 +1769,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1774,7 +1782,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1783,46 +1791,46 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.415566</v>
+        <v>-58.443936</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.613244</v>
+        <v>-34.560145</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Treinta y Tres Orientales 905</t>
+          <t>BAEZ 489</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1837,11 +1845,11 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1859,14 +1867,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.423229</v>
+        <v>-58.432978</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.625103</v>
+        <v>-34.57094</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1878,27 +1886,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1913,7 +1921,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1935,46 +1943,46 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.418089</v>
+        <v>-58.499823</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.620313</v>
+        <v>-34.563809</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1987,11 +1995,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
         <v>0</v>
       </c>
@@ -2011,14 +2015,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.427201</v>
+        <v>-58.400047</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.617131</v>
+        <v>-34.586358</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2030,27 +2034,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Lima Oeste 1649</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2069,7 +2073,7 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2086,47 +2090,43 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M22" t="n">
-        <v>-58.414984</v>
-      </c>
-      <c r="N22" t="n">
-        <v>-34.621386</v>
-      </c>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Conesa 2195</t>
+          <t>Lima Oeste 1697</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,15 +2141,15 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2159,40 +2159,36 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M23" t="n">
-        <v>-58.463015</v>
-      </c>
-      <c r="N23" t="n">
-        <v>-34.564505</v>
-      </c>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2202,7 +2198,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2217,11 +2213,11 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2239,14 +2235,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.507569</v>
+        <v>-58.487821</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.579623</v>
+        <v>-34.554603</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2258,27 +2254,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2315,36 +2311,36 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.466348</v>
+        <v>-58.404058</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.556028</v>
+        <v>-34.634341</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2354,7 +2350,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2365,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2391,10 +2387,10 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.497446</v>
+        <v>-58.511732</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.583455</v>
+        <v>-34.578688</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2410,17 +2406,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>-542</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Cramer 2141</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2430,7 +2426,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,7 +2441,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2463,18 +2459,18 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.454065</v>
+        <v>-58.461582</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.57105</v>
+        <v>-34.564296</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2486,27 +2482,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2543,14 +2539,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.436255</v>
+        <v>-58.44037</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.567733</v>
+        <v>-34.632249</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2562,27 +2558,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2619,14 +2615,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.43247</v>
+        <v>-58.440748</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.566492</v>
+        <v>-34.63245</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2638,17 +2634,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Soldado de la Independencia 1298</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2658,7 +2654,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2673,7 +2669,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada - Con fuente teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2686,7 +2682,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2695,36 +2691,36 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.440507</v>
+        <v>-58.434194</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.564016</v>
+        <v>-34.571754</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2734,7 +2730,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2771,46 +2767,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.44191</v>
+        <v>-58.434668</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.564245</v>
+        <v>-34.571258</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-510</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Larrea 590</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>808194254</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2821,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2838,23 +2834,23 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.438744</v>
+        <v>-58.402353</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.629929</v>
+        <v>-34.602205</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2866,7 +2862,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-509</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2876,17 +2872,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Paso 58</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808194240</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2923,19 +2919,19 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.473937</v>
+        <v>-58.403422</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.557355</v>
+        <v>-34.609195</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
@@ -3018,7 +3014,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-509</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3028,17 +3024,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Paso 58</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808194240</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3075,46 +3071,46 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.403422</v>
+        <v>-58.473937</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.609195</v>
+        <v>-34.557355</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-510</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Larrea 590</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808194254</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3129,11 +3125,11 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -3142,7 +3138,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3151,14 +3147,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.402353</v>
+        <v>-58.390198</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.602205</v>
+        <v>-34.637568</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3170,27 +3166,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-28</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>2/20/2024</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>ZABALA /ALT/ 2836</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>780340125</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3205,11 +3201,11 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>ZABALA 2836 - Reemplazar C114</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -3227,46 +3223,46 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.434668</v>
+        <v>-58.452298</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.571258</v>
+        <v>-34.572157</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3281,7 +3277,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3303,14 +3299,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.434194</v>
+        <v>-58.407076</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.571754</v>
+        <v>-34.616016</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3322,27 +3318,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3357,7 +3353,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3375,50 +3371,50 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.440748</v>
+        <v>-58.480871</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.63245</v>
+        <v>-34.616598</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-255</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>1/8/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Gurruchaga 410</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>802393948</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3433,7 +3429,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna para pedir traspaso de equipos</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3446,7 +3442,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3455,46 +3451,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.44037</v>
+        <v>-58.442601</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.632249</v>
+        <v>-34.597923</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-542</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Cramer 2141</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3507,13 +3503,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
-        </is>
-      </c>
+      <c r="H41" t="inlineStr"/>
       <c r="I41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3531,46 +3523,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.461582</v>
+        <v>-58.39894</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.564296</v>
+        <v>-34.591084</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3585,11 +3577,11 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3607,46 +3599,46 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.511732</v>
+        <v>-58.390269</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.578688</v>
+        <v>-34.625079</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-111</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>7/12/2024</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>CATAMARCA /ALT/ 1127</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>790298182</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3661,11 +3653,11 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3683,10 +3675,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.404058</v>
+        <v>-58.404265</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.634341</v>
+        <v>-34.623154</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3702,27 +3694,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3737,11 +3729,11 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -3759,46 +3751,46 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.487821</v>
+        <v>-58.394079</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.554603</v>
+        <v>-34.61051</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Lima Oeste 1697</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3813,15 +3805,15 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3831,36 +3823,40 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr"/>
-      <c r="N45" t="inlineStr"/>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M45" t="n">
+        <v>-58.395465</v>
+      </c>
+      <c r="N45" t="n">
+        <v>-34.622784</v>
+      </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Lima Oeste 1649</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3870,7 +3866,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3885,11 +3881,11 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -3906,16 +3902,20 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr"/>
+      <c r="M46" t="n">
+        <v>-58.386058</v>
+      </c>
+      <c r="N46" t="n">
+        <v>-34.621209</v>
+      </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-09 09:00:17)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -518,27 +518,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -553,11 +553,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -571,18 +571,18 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.438744</v>
+        <v>-58.390269</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.629929</v>
+        <v>-34.625079</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -594,17 +594,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>BAEZ 489</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -651,46 +651,46 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.44191</v>
+        <v>-58.432978</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.564245</v>
+        <v>-34.57094</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Soldado de la Independencia 1298</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -703,13 +703,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Picada - Con fuente teco</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -718,7 +714,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -727,46 +723,46 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.440507</v>
+        <v>-58.39894</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.564016</v>
+        <v>-34.591084</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>-28</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>2/20/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>ZABALA /ALT/ 2836</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>780340125</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -781,11 +777,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>ZABALA 2836 - Reemplazar C114</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -799,50 +795,50 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.43247</v>
+        <v>-58.452298</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.566492</v>
+        <v>-34.572157</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -857,11 +853,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -879,14 +875,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.436255</v>
+        <v>-58.390198</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.567733</v>
+        <v>-34.637568</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -898,27 +894,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -931,13 +927,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -951,40 +943,40 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.454065</v>
+        <v>-58.400047</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.57105</v>
+        <v>-34.586358</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -994,7 +986,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1009,11 +1001,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1031,10 +1023,10 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.497446</v>
+        <v>-58.499823</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.583455</v>
+        <v>-34.563809</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1050,27 +1042,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1085,11 +1077,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1107,46 +1099,46 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.466348</v>
+        <v>-58.386058</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.556028</v>
+        <v>-34.621209</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1161,7 +1153,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1183,46 +1175,46 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.507569</v>
+        <v>-58.395465</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.579623</v>
+        <v>-34.622784</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Conesa 2195</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1237,7 +1229,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1259,46 +1251,46 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.463015</v>
+        <v>-58.394079</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.564505</v>
+        <v>-34.61051</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>-111</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>7/12/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>CATAMARCA /ALT/ 1127</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>790298182</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1313,7 +1305,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1335,14 +1327,14 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.414984</v>
+        <v>-58.404265</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.621386</v>
+        <v>-34.623154</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1354,27 +1346,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>-255</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>1/8/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Gurruchaga 410</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>802393948</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1389,11 +1381,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna para pedir traspaso de equipos</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1402,7 +1394,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1411,46 +1403,46 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.427201</v>
+        <v>-58.442601</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.617131</v>
+        <v>-34.597923</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1465,11 +1457,11 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1487,46 +1479,46 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.418089</v>
+        <v>-58.480871</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.620313</v>
+        <v>-34.616598</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Treinta y Tres Orientales 905</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1541,11 +1533,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1563,14 +1555,14 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.423229</v>
+        <v>-58.407076</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.625103</v>
+        <v>-34.616016</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1582,27 +1574,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1617,7 +1609,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1639,26 +1631,26 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.415566</v>
+        <v>-58.439727</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.613244</v>
+        <v>-34.556261</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1668,7 +1660,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>HERNANDEZ JOSE 1451</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1678,7 +1670,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1693,7 +1685,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1706,7 +1698,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1715,10 +1707,10 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.439727</v>
+        <v>-58.443936</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.556261</v>
+        <v>-34.560145</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1734,27 +1726,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>HERNANDEZ JOSE 1451</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1769,7 +1761,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1782,7 +1774,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1791,46 +1783,46 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.443936</v>
+        <v>-58.415566</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.560145</v>
+        <v>-34.613244</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>BAEZ 489</t>
+          <t>Treinta y Tres Orientales 905</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1845,11 +1837,11 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1867,14 +1859,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.432978</v>
+        <v>-58.423229</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.57094</v>
+        <v>-34.625103</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1886,27 +1878,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1921,7 +1913,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1943,46 +1935,46 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.499823</v>
+        <v>-58.418089</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.563809</v>
+        <v>-34.620313</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1995,7 +1987,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I21" t="n">
         <v>0</v>
       </c>
@@ -2015,14 +2011,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.400047</v>
+        <v>-58.427201</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.586358</v>
+        <v>-34.617131</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2034,27 +2030,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Lima Oeste 1649</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2073,7 +2069,7 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2090,43 +2086,47 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
+      <c r="M22" t="n">
+        <v>-58.414984</v>
+      </c>
+      <c r="N22" t="n">
+        <v>-34.621386</v>
+      </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Lima Oeste 1697</t>
+          <t>Conesa 2195</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,15 +2141,15 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2159,36 +2159,40 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M23" t="n">
+        <v>-58.463015</v>
+      </c>
+      <c r="N23" t="n">
+        <v>-34.564505</v>
+      </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2198,7 +2202,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2213,11 +2217,11 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2235,14 +2239,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.487821</v>
+        <v>-58.507569</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.554603</v>
+        <v>-34.579623</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2254,27 +2258,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2311,36 +2315,36 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.404058</v>
+        <v>-58.466348</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.634341</v>
+        <v>-34.556028</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2350,7 +2354,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2365,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2387,10 +2391,10 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.511732</v>
+        <v>-58.497446</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.578688</v>
+        <v>-34.583455</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2406,17 +2410,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-542</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Cramer 2141</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2426,7 +2430,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2441,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2459,18 +2463,18 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.461582</v>
+        <v>-58.454065</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.564296</v>
+        <v>-34.57105</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2482,27 +2486,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2539,14 +2543,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.44037</v>
+        <v>-58.436255</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.632249</v>
+        <v>-34.567733</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2558,27 +2562,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2615,14 +2619,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.440748</v>
+        <v>-58.43247</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.63245</v>
+        <v>-34.566492</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2634,17 +2638,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Soldado de la Independencia 1298</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2654,7 +2658,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2669,7 +2673,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada - Con fuente teco</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2682,7 +2686,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2691,36 +2695,36 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.434194</v>
+        <v>-58.440507</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.571754</v>
+        <v>-34.564016</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2730,7 +2734,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2767,46 +2771,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.434668</v>
+        <v>-58.44191</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.571258</v>
+        <v>-34.564245</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-510</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Larrea 590</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808194254</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2821,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2834,23 +2838,23 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.402353</v>
+        <v>-58.438744</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.602205</v>
+        <v>-34.629929</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2862,7 +2866,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-509</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2872,17 +2876,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Paso 58</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808194240</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2919,19 +2923,19 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.403422</v>
+        <v>-58.473937</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.609195</v>
+        <v>-34.557355</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
@@ -3014,7 +3018,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-509</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3024,17 +3028,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Paso 58</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808194240</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3071,46 +3075,46 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.473937</v>
+        <v>-58.403422</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.557355</v>
+        <v>-34.609195</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-510</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Larrea 590</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>808194254</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3125,11 +3129,11 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -3138,7 +3142,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3147,14 +3151,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.390198</v>
+        <v>-58.402353</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.637568</v>
+        <v>-34.602205</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3166,27 +3170,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-28</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2/20/2024</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>ZABALA /ALT/ 2836</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>780340125</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3201,11 +3205,11 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>ZABALA 2836 - Reemplazar C114</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -3223,46 +3227,46 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.452298</v>
+        <v>-58.434668</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.572157</v>
+        <v>-34.571258</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3277,7 +3281,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3299,14 +3303,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.407076</v>
+        <v>-58.434194</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.616016</v>
+        <v>-34.571754</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3318,27 +3322,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3353,7 +3357,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3371,50 +3375,50 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.480871</v>
+        <v>-58.440748</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.616598</v>
+        <v>-34.63245</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-255</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>1/8/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Gurruchaga 410</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>802393948</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3429,7 +3433,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de equipos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3442,7 +3446,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3451,46 +3455,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.442601</v>
+        <v>-58.44037</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.597923</v>
+        <v>-34.632249</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>-542</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Cramer 2141</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3503,9 +3507,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H41" t="inlineStr"/>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+        </is>
+      </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3523,46 +3531,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.39894</v>
+        <v>-58.461582</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.591084</v>
+        <v>-34.564296</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3577,11 +3585,11 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3599,46 +3607,46 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.390269</v>
+        <v>-58.511732</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.625079</v>
+        <v>-34.578688</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,11 +3661,11 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3675,10 +3683,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.404265</v>
+        <v>-58.404058</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.623154</v>
+        <v>-34.634341</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3694,27 +3702,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,11 +3737,11 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -3751,46 +3759,46 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.394079</v>
+        <v>-58.487821</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.61051</v>
+        <v>-34.554603</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Lima Oeste 1697</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,15 +3813,15 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3823,40 +3831,36 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M45" t="n">
-        <v>-58.395465</v>
-      </c>
-      <c r="N45" t="n">
-        <v>-34.622784</v>
-      </c>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Lima Oeste 1649</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3866,7 +3870,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3881,11 +3885,11 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -3902,20 +3906,16 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M46" t="n">
-        <v>-58.386058</v>
-      </c>
-      <c r="N46" t="n">
-        <v>-34.621209</v>
-      </c>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-09 14:46:40)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3018,7 +3018,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-509</t>
+          <t>-510</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3028,7 +3028,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Paso 58</t>
+          <t>Larrea 590</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808194240</t>
+          <t>808194254</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -3075,10 +3075,10 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.403422</v>
+        <v>-58.402353</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.609195</v>
+        <v>-34.602205</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -3094,27 +3094,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-510</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Larrea 590</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808194254</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3142,7 +3142,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3151,14 +3151,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.402353</v>
+        <v>-58.434668</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.602205</v>
+        <v>-34.571258</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3170,17 +3170,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -3190,7 +3190,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3227,10 +3227,10 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.434668</v>
+        <v>-58.434194</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.571258</v>
+        <v>-34.571754</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -3246,27 +3246,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3299,18 +3299,18 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.434194</v>
+        <v>-58.440748</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.571754</v>
+        <v>-34.63245</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3322,7 +3322,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3332,7 +3332,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3342,7 +3342,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3375,14 +3375,14 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.440748</v>
+        <v>-58.44037</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.63245</v>
+        <v>-34.632249</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3398,27 +3398,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-542</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Cramer 2141</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3455,46 +3455,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.44037</v>
+        <v>-58.461582</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.632249</v>
+        <v>-34.564296</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-542</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Cramer 2141</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3531,14 +3531,14 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.461582</v>
+        <v>-58.511732</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.564296</v>
+        <v>-34.578688</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3550,27 +3550,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3607,26 +3607,26 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.511732</v>
+        <v>-58.404058</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.578688</v>
+        <v>-34.634341</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3636,17 +3636,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3683,26 +3683,26 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.404058</v>
+        <v>-58.487821</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.634341</v>
+        <v>-34.554603</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3712,17 +3712,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Lima Oeste 1697</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3745,7 +3745,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3755,30 +3755,26 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M44" t="n">
-        <v>-58.487821</v>
-      </c>
-      <c r="N44" t="n">
-        <v>-34.554603</v>
-      </c>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3788,7 +3784,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Lima Oeste 1697</t>
+          <t>Lima Oeste 1649</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3798,7 +3794,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3813,7 +3809,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3821,7 +3817,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3831,7 +3827,7 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M45" t="inlineStr"/>
@@ -3842,78 +3838,6 @@
         </is>
       </c>
       <c r="P45" t="inlineStr">
-        <is>
-          <t>No clasificado, consultar con mantenimiento</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>-555</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Lima Oeste 1649</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>808973201</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I46" t="n">
-        <v>1</v>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr"/>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>No ubicado</t>
-        </is>
-      </c>
-      <c r="P46" t="inlineStr">
         <is>
           <t>No clasificado, consultar con mantenimiento</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-15 07:10:32)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -518,27 +518,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -553,11 +553,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -571,18 +571,18 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.390269</v>
+        <v>-58.438744</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.625079</v>
+        <v>-34.629929</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -594,17 +594,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BAEZ 489</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -651,46 +651,46 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.432978</v>
+        <v>-58.44191</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.57094</v>
+        <v>-34.564245</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Soldado de la Independencia 1298</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -703,9 +703,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Picada - Con fuente teco</t>
+        </is>
+      </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -714,7 +718,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -723,46 +727,46 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.39894</v>
+        <v>-58.440507</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.591084</v>
+        <v>-34.564016</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-28</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2/20/2024</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ZABALA /ALT/ 2836</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>780340125</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -777,11 +781,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>ZABALA 2836 - Reemplazar C114</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -795,50 +799,50 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.452298</v>
+        <v>-58.43247</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.572157</v>
+        <v>-34.566492</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -853,11 +857,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -875,14 +879,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.390198</v>
+        <v>-58.436255</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.637568</v>
+        <v>-34.567733</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -894,27 +898,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -927,9 +931,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -943,40 +951,40 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.400047</v>
+        <v>-58.454065</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.586358</v>
+        <v>-34.57105</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -986,7 +994,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1001,11 +1009,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1023,10 +1031,10 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.499823</v>
+        <v>-58.497446</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.563809</v>
+        <v>-34.583455</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1042,27 +1050,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1077,11 +1085,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1099,46 +1107,46 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.386058</v>
+        <v>-58.466348</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.621209</v>
+        <v>-34.556028</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1153,7 +1161,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1175,46 +1183,46 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.395465</v>
+        <v>-58.507569</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.622784</v>
+        <v>-34.579623</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Conesa 2195</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1229,7 +1237,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1251,46 +1259,46 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.394079</v>
+        <v>-58.463015</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.61051</v>
+        <v>-34.564505</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1305,7 +1313,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1327,14 +1335,14 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.404265</v>
+        <v>-58.414984</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.623154</v>
+        <v>-34.621386</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1346,27 +1354,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-255</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1/8/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Gurruchaga 410</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>802393948</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1381,11 +1389,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de equipos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1394,7 +1402,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1403,46 +1411,46 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.442601</v>
+        <v>-58.427201</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.597923</v>
+        <v>-34.617131</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1457,11 +1465,11 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1479,46 +1487,46 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.480871</v>
+        <v>-58.418089</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.616598</v>
+        <v>-34.620313</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Treinta y Tres Orientales 905</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1533,11 +1541,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1555,14 +1563,14 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.407076</v>
+        <v>-58.423229</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.616016</v>
+        <v>-34.625103</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1574,27 +1582,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1609,7 +1617,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1631,26 +1639,26 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.439727</v>
+        <v>-58.415566</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.556261</v>
+        <v>-34.613244</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1660,7 +1668,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>HERNANDEZ JOSE 1451</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1670,7 +1678,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1685,7 +1693,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1698,7 +1706,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1707,10 +1715,10 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.443936</v>
+        <v>-58.439727</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.560145</v>
+        <v>-34.556261</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1726,27 +1734,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>HERNANDEZ JOSE 1451</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1761,7 +1769,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1774,7 +1782,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1783,46 +1791,46 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.415566</v>
+        <v>-58.443936</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.613244</v>
+        <v>-34.560145</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Treinta y Tres Orientales 905</t>
+          <t>BAEZ 489</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1837,11 +1845,11 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1859,14 +1867,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.423229</v>
+        <v>-58.432978</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.625103</v>
+        <v>-34.57094</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1878,27 +1886,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1913,7 +1921,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1935,46 +1943,46 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.418089</v>
+        <v>-58.499823</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.620313</v>
+        <v>-34.563809</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1987,11 +1995,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
         <v>0</v>
       </c>
@@ -2011,14 +2015,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.427201</v>
+        <v>-58.400047</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.617131</v>
+        <v>-34.586358</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2030,27 +2034,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Lima Oeste 1649</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2069,7 +2073,7 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2086,47 +2090,43 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M22" t="n">
-        <v>-58.414984</v>
-      </c>
-      <c r="N22" t="n">
-        <v>-34.621386</v>
-      </c>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Conesa 2195</t>
+          <t>Lima Oeste 1697</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,15 +2141,15 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2159,40 +2159,36 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M23" t="n">
-        <v>-58.463015</v>
-      </c>
-      <c r="N23" t="n">
-        <v>-34.564505</v>
-      </c>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2202,7 +2198,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2217,11 +2213,11 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2239,14 +2235,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.507569</v>
+        <v>-58.487821</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.579623</v>
+        <v>-34.554603</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2258,27 +2254,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2315,36 +2311,36 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.466348</v>
+        <v>-58.404058</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.556028</v>
+        <v>-34.634341</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2354,7 +2350,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2365,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2391,10 +2387,10 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.497446</v>
+        <v>-58.511732</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.583455</v>
+        <v>-34.578688</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2410,17 +2406,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>-542</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Cramer 2141</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2430,7 +2426,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,7 +2441,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2463,18 +2459,18 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.454065</v>
+        <v>-58.461582</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.57105</v>
+        <v>-34.564296</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2486,27 +2482,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2543,14 +2539,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.436255</v>
+        <v>-58.44037</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.567733</v>
+        <v>-34.632249</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2562,27 +2558,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2619,14 +2615,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.43247</v>
+        <v>-58.440748</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.566492</v>
+        <v>-34.63245</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2638,17 +2634,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Soldado de la Independencia 1298</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2658,7 +2654,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2673,7 +2669,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada - Con fuente teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2686,7 +2682,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2695,36 +2691,36 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.440507</v>
+        <v>-58.434194</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.564016</v>
+        <v>-34.571754</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2734,7 +2730,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2771,46 +2767,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.44191</v>
+        <v>-58.434668</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.564245</v>
+        <v>-34.571258</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-510</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Larrea 590</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>808194254</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2821,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2838,23 +2834,23 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.438744</v>
+        <v>-58.402353</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.629929</v>
+        <v>-34.602205</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2866,7 +2862,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-508</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2876,7 +2872,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Moldes 2463</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2886,7 +2882,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808194234</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2914,7 +2910,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2923,10 +2919,10 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.473937</v>
+        <v>-58.462281</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.557355</v>
+        <v>-34.560321</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2942,7 +2938,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-508</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2952,7 +2948,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Moldes 2463</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2962,7 +2958,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808194234</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2990,7 +2986,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2999,10 +2995,10 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.462281</v>
+        <v>-58.473937</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.560321</v>
+        <v>-34.557355</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3018,27 +3014,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-510</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Larrea 590</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808194254</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3053,11 +3049,11 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3066,7 +3062,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -3075,14 +3071,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.402353</v>
+        <v>-58.390198</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.602205</v>
+        <v>-34.637568</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3094,27 +3090,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-28</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>2/20/2024</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>ZABALA /ALT/ 2836</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>780340125</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3129,11 +3125,11 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>ZABALA 2836 - Reemplazar C114</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -3151,46 +3147,46 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.434668</v>
+        <v>-58.452298</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.571258</v>
+        <v>-34.572157</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3205,7 +3201,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3227,14 +3223,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.434194</v>
+        <v>-58.407076</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.571754</v>
+        <v>-34.616016</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3246,27 +3242,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3281,7 +3277,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3299,50 +3295,50 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.440748</v>
+        <v>-58.480871</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.63245</v>
+        <v>-34.616598</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-255</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>1/8/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Gurruchaga 410</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>802393948</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3357,7 +3353,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna para pedir traspaso de equipos</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3370,7 +3366,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3379,46 +3375,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.44037</v>
+        <v>-58.442601</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.632249</v>
+        <v>-34.597923</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-542</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Cramer 2141</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3431,13 +3427,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
-        </is>
-      </c>
+      <c r="H40" t="inlineStr"/>
       <c r="I40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -3455,46 +3447,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.461582</v>
+        <v>-58.39894</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.564296</v>
+        <v>-34.591084</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3509,11 +3501,11 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3531,46 +3523,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.511732</v>
+        <v>-58.390269</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.578688</v>
+        <v>-34.625079</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-111</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>7/12/2024</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>CATAMARCA /ALT/ 1127</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>790298182</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3585,11 +3577,11 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3607,10 +3599,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.404058</v>
+        <v>-58.404265</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.634341</v>
+        <v>-34.623154</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3626,27 +3618,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3661,11 +3653,11 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3683,46 +3675,46 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.487821</v>
+        <v>-58.394079</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.554603</v>
+        <v>-34.61051</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Lima Oeste 1697</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3737,15 +3729,15 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3755,36 +3747,40 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr"/>
-      <c r="N44" t="inlineStr"/>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M44" t="n">
+        <v>-58.395465</v>
+      </c>
+      <c r="N44" t="n">
+        <v>-34.622784</v>
+      </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Lima Oeste 1649</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3794,7 +3790,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3809,11 +3805,11 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -3830,16 +3826,20 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M45" t="inlineStr"/>
-      <c r="N45" t="inlineStr"/>
+      <c r="M45" t="n">
+        <v>-58.386058</v>
+      </c>
+      <c r="N45" t="n">
+        <v>-34.621209</v>
+      </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-15 11:59:06)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -518,27 +518,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -553,11 +553,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -571,18 +571,18 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.438744</v>
+        <v>-58.390269</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.629929</v>
+        <v>-34.625079</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -594,17 +594,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>BAEZ 489</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -651,46 +651,46 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.44191</v>
+        <v>-58.432978</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.564245</v>
+        <v>-34.57094</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Soldado de la Independencia 1298</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -703,13 +703,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Picada - Con fuente teco</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -718,7 +714,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -727,46 +723,46 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.440507</v>
+        <v>-58.39894</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.564016</v>
+        <v>-34.591084</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>-28</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>2/20/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>ZABALA /ALT/ 2836</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>780340125</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -781,11 +777,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>ZABALA 2836 - Reemplazar C114</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -799,50 +795,50 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.43247</v>
+        <v>-58.452298</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.566492</v>
+        <v>-34.572157</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -857,11 +853,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -879,14 +875,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.436255</v>
+        <v>-58.390198</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.567733</v>
+        <v>-34.637568</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -898,27 +894,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -931,13 +927,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -951,40 +943,40 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.454065</v>
+        <v>-58.400047</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.57105</v>
+        <v>-34.586358</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -994,7 +986,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1009,11 +1001,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1031,10 +1023,10 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.497446</v>
+        <v>-58.499823</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.583455</v>
+        <v>-34.563809</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1050,27 +1042,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1085,11 +1077,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1107,46 +1099,46 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.466348</v>
+        <v>-58.386058</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.556028</v>
+        <v>-34.621209</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1161,7 +1153,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1183,46 +1175,46 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.507569</v>
+        <v>-58.395465</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.579623</v>
+        <v>-34.622784</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Conesa 2195</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1237,7 +1229,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1259,46 +1251,46 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.463015</v>
+        <v>-58.394079</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.564505</v>
+        <v>-34.61051</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>-111</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>7/12/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>CATAMARCA /ALT/ 1127</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>790298182</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1313,7 +1305,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1335,14 +1327,14 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.414984</v>
+        <v>-58.404265</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.621386</v>
+        <v>-34.623154</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1354,27 +1346,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>-255</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>1/8/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Gurruchaga 410</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>802393948</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1389,11 +1381,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna para pedir traspaso de equipos</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1402,7 +1394,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1411,46 +1403,46 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.427201</v>
+        <v>-58.442601</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.617131</v>
+        <v>-34.597923</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1465,11 +1457,11 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1487,46 +1479,46 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.418089</v>
+        <v>-58.480871</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.620313</v>
+        <v>-34.616598</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Treinta y Tres Orientales 905</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1541,11 +1533,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1563,14 +1555,14 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.423229</v>
+        <v>-58.407076</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.625103</v>
+        <v>-34.616016</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1582,27 +1574,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1617,7 +1609,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1639,26 +1631,26 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.415566</v>
+        <v>-58.439727</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.613244</v>
+        <v>-34.556261</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1668,7 +1660,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>HERNANDEZ JOSE 1451</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1678,7 +1670,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1693,7 +1685,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1706,7 +1698,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1715,10 +1707,10 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.439727</v>
+        <v>-58.443936</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.556261</v>
+        <v>-34.560145</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1734,27 +1726,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>HERNANDEZ JOSE 1451</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1769,7 +1761,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1782,7 +1774,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1791,46 +1783,46 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.443936</v>
+        <v>-58.415566</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.560145</v>
+        <v>-34.613244</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>BAEZ 489</t>
+          <t>Treinta y Tres Orientales 905</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1845,11 +1837,11 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1867,14 +1859,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.432978</v>
+        <v>-58.423229</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.57094</v>
+        <v>-34.625103</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1886,27 +1878,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1921,7 +1913,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1943,46 +1935,46 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.499823</v>
+        <v>-58.418089</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.563809</v>
+        <v>-34.620313</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1995,7 +1987,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I21" t="n">
         <v>0</v>
       </c>
@@ -2015,14 +2011,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.400047</v>
+        <v>-58.427201</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.586358</v>
+        <v>-34.617131</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2034,27 +2030,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Lima Oeste 1649</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2073,7 +2069,7 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2090,43 +2086,47 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
+      <c r="M22" t="n">
+        <v>-58.414984</v>
+      </c>
+      <c r="N22" t="n">
+        <v>-34.621386</v>
+      </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Lima Oeste 1697</t>
+          <t>Conesa 2195</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,15 +2141,15 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2159,36 +2159,40 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M23" t="n">
+        <v>-58.463015</v>
+      </c>
+      <c r="N23" t="n">
+        <v>-34.564505</v>
+      </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2198,7 +2202,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2213,11 +2217,11 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2235,14 +2239,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.487821</v>
+        <v>-58.507569</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.554603</v>
+        <v>-34.579623</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2254,27 +2258,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2311,36 +2315,36 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.404058</v>
+        <v>-58.466348</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.634341</v>
+        <v>-34.556028</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2350,7 +2354,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2365,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2387,10 +2391,10 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.511732</v>
+        <v>-58.497446</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.578688</v>
+        <v>-34.583455</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2406,17 +2410,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-542</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Cramer 2141</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2426,7 +2430,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2441,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2459,18 +2463,18 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.461582</v>
+        <v>-58.454065</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.564296</v>
+        <v>-34.57105</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2482,27 +2486,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2539,14 +2543,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.44037</v>
+        <v>-58.436255</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.632249</v>
+        <v>-34.567733</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2558,27 +2562,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2615,14 +2619,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.440748</v>
+        <v>-58.43247</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.63245</v>
+        <v>-34.566492</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2634,17 +2638,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Soldado de la Independencia 1298</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2654,7 +2658,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2669,7 +2673,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada - Con fuente teco</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2682,7 +2686,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2691,36 +2695,36 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.434194</v>
+        <v>-58.440507</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.571754</v>
+        <v>-34.564016</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2730,7 +2734,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2767,46 +2771,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.434668</v>
+        <v>-58.44191</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.571258</v>
+        <v>-34.564245</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-510</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Larrea 590</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808194254</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2821,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2834,23 +2838,23 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.402353</v>
+        <v>-58.438744</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.602205</v>
+        <v>-34.629929</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2862,7 +2866,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-508</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2872,7 +2876,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Moldes 2463</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2882,7 +2886,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808194234</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2910,7 +2914,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2919,10 +2923,10 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.462281</v>
+        <v>-58.473937</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.560321</v>
+        <v>-34.557355</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2938,7 +2942,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-508</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2948,7 +2952,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Moldes 2463</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2958,7 +2962,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808194234</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2986,7 +2990,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2995,10 +2999,10 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.473937</v>
+        <v>-58.462281</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.557355</v>
+        <v>-34.560321</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3014,27 +3018,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-510</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Larrea 590</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>808194254</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3049,11 +3053,11 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3062,7 +3066,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -3071,14 +3075,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.390198</v>
+        <v>-58.402353</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.637568</v>
+        <v>-34.602205</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3090,27 +3094,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-28</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2/20/2024</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ZABALA /ALT/ 2836</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>780340125</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3125,11 +3129,11 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>ZABALA 2836 - Reemplazar C114</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -3147,46 +3151,46 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.452298</v>
+        <v>-58.434668</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.572157</v>
+        <v>-34.571258</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3201,7 +3205,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3223,14 +3227,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.407076</v>
+        <v>-58.434194</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.616016</v>
+        <v>-34.571754</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3242,27 +3246,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3277,7 +3281,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3295,50 +3299,50 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.480871</v>
+        <v>-58.440748</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.616598</v>
+        <v>-34.63245</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-255</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>1/8/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Gurruchaga 410</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>802393948</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3353,7 +3357,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de equipos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3366,7 +3370,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3375,46 +3379,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.442601</v>
+        <v>-58.44037</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.597923</v>
+        <v>-34.632249</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>-542</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Cramer 2141</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3427,9 +3431,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr"/>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+        </is>
+      </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -3447,46 +3455,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.39894</v>
+        <v>-58.461582</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.591084</v>
+        <v>-34.564296</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3501,11 +3509,11 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3523,46 +3531,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.390269</v>
+        <v>-58.511732</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.625079</v>
+        <v>-34.578688</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3577,11 +3585,11 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3599,10 +3607,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.404265</v>
+        <v>-58.404058</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.623154</v>
+        <v>-34.634341</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3618,27 +3626,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,11 +3661,11 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3675,46 +3683,46 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.394079</v>
+        <v>-58.487821</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.61051</v>
+        <v>-34.554603</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Lima Oeste 1697</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,15 +3737,15 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3747,40 +3755,36 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M44" t="n">
-        <v>-58.395465</v>
-      </c>
-      <c r="N44" t="n">
-        <v>-34.622784</v>
-      </c>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
       <c r="O44" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Lima Oeste 1649</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3790,7 +3794,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,11 +3809,11 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -3826,20 +3830,16 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M45" t="n">
-        <v>-58.386058</v>
-      </c>
-      <c r="N45" t="n">
-        <v>-34.621209</v>
-      </c>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-19 08:03:53)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -518,27 +518,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -553,11 +553,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -571,18 +571,18 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.390269</v>
+        <v>-58.438744</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.625079</v>
+        <v>-34.629929</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -594,17 +594,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BAEZ 489</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -651,46 +651,46 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.432978</v>
+        <v>-58.44191</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.57094</v>
+        <v>-34.564245</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Soldado de la Independencia 1298</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -703,9 +703,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Picada - Con fuente teco</t>
+        </is>
+      </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -714,7 +718,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -723,46 +727,46 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.39894</v>
+        <v>-58.440507</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.591084</v>
+        <v>-34.564016</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-28</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2/20/2024</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ZABALA /ALT/ 2836</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>780340125</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -777,11 +781,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>ZABALA 2836 - Reemplazar C114</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -795,50 +799,50 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.452298</v>
+        <v>-58.43247</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.572157</v>
+        <v>-34.566492</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -853,11 +857,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -875,14 +879,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.390198</v>
+        <v>-58.436255</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.637568</v>
+        <v>-34.567733</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -894,27 +898,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -927,9 +931,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -943,40 +951,40 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.400047</v>
+        <v>-58.454065</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.586358</v>
+        <v>-34.57105</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -986,7 +994,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1001,11 +1009,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1023,10 +1031,10 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.499823</v>
+        <v>-58.497446</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.563809</v>
+        <v>-34.583455</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1042,27 +1050,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1077,11 +1085,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1099,46 +1107,46 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.386058</v>
+        <v>-58.466348</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.621209</v>
+        <v>-34.556028</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1153,7 +1161,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1175,46 +1183,46 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.395465</v>
+        <v>-58.507569</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.622784</v>
+        <v>-34.579623</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Conesa 2195</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1229,7 +1237,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1251,46 +1259,46 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.394079</v>
+        <v>-58.463015</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.61051</v>
+        <v>-34.564505</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1305,7 +1313,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1327,14 +1335,14 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.404265</v>
+        <v>-58.414984</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.623154</v>
+        <v>-34.621386</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1346,27 +1354,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-255</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1/8/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Gurruchaga 410</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>802393948</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1381,11 +1389,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de equipos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1394,7 +1402,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1403,46 +1411,46 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.442601</v>
+        <v>-58.427201</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.597923</v>
+        <v>-34.617131</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1457,11 +1465,11 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1479,46 +1487,46 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.480871</v>
+        <v>-58.418089</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.616598</v>
+        <v>-34.620313</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Treinta y Tres Orientales 905</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1533,11 +1541,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1555,14 +1563,14 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.407076</v>
+        <v>-58.423229</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.616016</v>
+        <v>-34.625103</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1574,27 +1582,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1609,7 +1617,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1631,26 +1639,26 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.439727</v>
+        <v>-58.415566</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.556261</v>
+        <v>-34.613244</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1660,7 +1668,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>HERNANDEZ JOSE 1451</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1670,7 +1678,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1685,7 +1693,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1698,7 +1706,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1707,10 +1715,10 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.443936</v>
+        <v>-58.439727</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.560145</v>
+        <v>-34.556261</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1726,27 +1734,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>HERNANDEZ JOSE 1451</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1761,7 +1769,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1774,7 +1782,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1783,46 +1791,46 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.415566</v>
+        <v>-58.443936</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.613244</v>
+        <v>-34.560145</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Treinta y Tres Orientales 905</t>
+          <t>BAEZ 489</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1837,11 +1845,11 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1859,14 +1867,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.423229</v>
+        <v>-58.432978</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.625103</v>
+        <v>-34.57094</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1878,27 +1886,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1913,7 +1921,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1935,46 +1943,46 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.418089</v>
+        <v>-58.499823</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.620313</v>
+        <v>-34.563809</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1987,11 +1995,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
         <v>0</v>
       </c>
@@ -2011,14 +2015,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.427201</v>
+        <v>-58.400047</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.617131</v>
+        <v>-34.586358</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2030,27 +2034,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Lima Oeste 1649</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2069,7 +2073,7 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2086,47 +2090,43 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M22" t="n">
-        <v>-58.414984</v>
-      </c>
-      <c r="N22" t="n">
-        <v>-34.621386</v>
-      </c>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Conesa 2195</t>
+          <t>Lima Oeste 1697</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,15 +2141,15 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2159,40 +2159,36 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M23" t="n">
-        <v>-58.463015</v>
-      </c>
-      <c r="N23" t="n">
-        <v>-34.564505</v>
-      </c>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2202,7 +2198,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2217,11 +2213,11 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2239,14 +2235,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.507569</v>
+        <v>-58.487821</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.579623</v>
+        <v>-34.554603</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2258,27 +2254,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2315,36 +2311,36 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.466348</v>
+        <v>-58.404058</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.556028</v>
+        <v>-34.634341</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2354,7 +2350,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2365,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2391,10 +2387,10 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.497446</v>
+        <v>-58.511732</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.583455</v>
+        <v>-34.578688</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2410,17 +2406,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>-542</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Cramer 2141</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2430,7 +2426,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,7 +2441,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2463,18 +2459,18 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.454065</v>
+        <v>-58.461582</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.57105</v>
+        <v>-34.564296</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2486,27 +2482,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2543,14 +2539,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.436255</v>
+        <v>-58.44037</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.567733</v>
+        <v>-34.632249</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2562,27 +2558,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2619,14 +2615,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.43247</v>
+        <v>-58.440748</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.566492</v>
+        <v>-34.63245</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2638,17 +2634,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Soldado de la Independencia 1298</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2658,7 +2654,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2673,7 +2669,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada - Con fuente teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2686,7 +2682,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2695,36 +2691,36 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.440507</v>
+        <v>-58.434194</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.564016</v>
+        <v>-34.571754</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2734,7 +2730,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2771,46 +2767,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.44191</v>
+        <v>-58.434668</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.564245</v>
+        <v>-34.571258</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-510</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Larrea 590</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>808194254</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2821,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2838,23 +2834,23 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.438744</v>
+        <v>-58.402353</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.629929</v>
+        <v>-34.602205</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2866,7 +2862,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-508</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2876,7 +2872,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Moldes 2463</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2886,7 +2882,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808194234</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2914,7 +2910,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2923,10 +2919,10 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.473937</v>
+        <v>-58.462281</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.557355</v>
+        <v>-34.560321</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2942,7 +2938,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-508</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2952,7 +2948,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Moldes 2463</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2962,7 +2958,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808194234</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2990,7 +2986,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2999,10 +2995,10 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.462281</v>
+        <v>-58.473937</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.560321</v>
+        <v>-34.557355</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3018,27 +3014,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-510</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Larrea 590</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808194254</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3053,11 +3049,11 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3066,7 +3062,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -3075,14 +3071,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.402353</v>
+        <v>-58.390198</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.602205</v>
+        <v>-34.637568</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3094,27 +3090,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-28</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>2/20/2024</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>ZABALA /ALT/ 2836</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>780340125</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3129,11 +3125,11 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>ZABALA 2836 - Reemplazar C114</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -3151,46 +3147,46 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.434668</v>
+        <v>-58.452298</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.571258</v>
+        <v>-34.572157</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3205,7 +3201,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3227,14 +3223,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.434194</v>
+        <v>-58.407076</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.571754</v>
+        <v>-34.616016</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3246,27 +3242,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3281,7 +3277,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3299,50 +3295,50 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.440748</v>
+        <v>-58.480871</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.63245</v>
+        <v>-34.616598</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-255</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>1/8/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Gurruchaga 410</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>802393948</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3357,7 +3353,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna para pedir traspaso de equipos</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3370,7 +3366,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3379,46 +3375,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.44037</v>
+        <v>-58.442601</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.632249</v>
+        <v>-34.597923</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-542</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Cramer 2141</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3431,13 +3427,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
-        </is>
-      </c>
+      <c r="H40" t="inlineStr"/>
       <c r="I40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -3455,46 +3447,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.461582</v>
+        <v>-58.39894</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.564296</v>
+        <v>-34.591084</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3509,11 +3501,11 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3531,46 +3523,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.511732</v>
+        <v>-58.390269</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.578688</v>
+        <v>-34.625079</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-111</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>7/12/2024</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>CATAMARCA /ALT/ 1127</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>790298182</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3585,11 +3577,11 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3607,10 +3599,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.404058</v>
+        <v>-58.404265</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.634341</v>
+        <v>-34.623154</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3626,27 +3618,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3661,11 +3653,11 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3683,46 +3675,46 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.487821</v>
+        <v>-58.394079</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.554603</v>
+        <v>-34.61051</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Lima Oeste 1697</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3737,15 +3729,15 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3755,36 +3747,40 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr"/>
-      <c r="N44" t="inlineStr"/>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M44" t="n">
+        <v>-58.395465</v>
+      </c>
+      <c r="N44" t="n">
+        <v>-34.622784</v>
+      </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Lima Oeste 1649</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3794,7 +3790,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3809,11 +3805,11 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -3830,16 +3826,20 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M45" t="inlineStr"/>
-      <c r="N45" t="inlineStr"/>
+      <c r="M45" t="n">
+        <v>-58.386058</v>
+      </c>
+      <c r="N45" t="n">
+        <v>-34.621209</v>
+      </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-23 08:47:41)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -518,27 +518,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -553,11 +553,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -571,18 +571,18 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.438744</v>
+        <v>-58.390269</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.629929</v>
+        <v>-34.625079</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -594,17 +594,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>BAEZ 489</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -651,46 +651,46 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.44191</v>
+        <v>-58.432978</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.564245</v>
+        <v>-34.57094</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Soldado de la Independencia 1298</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -703,13 +703,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Picada - Con fuente teco</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -718,7 +714,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -727,46 +723,46 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.440507</v>
+        <v>-58.39894</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.564016</v>
+        <v>-34.591084</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>-28</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>2/20/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>ZABALA /ALT/ 2836</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>780340125</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -781,11 +777,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>ZABALA 2836 - Reemplazar C114</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -799,50 +795,50 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.43247</v>
+        <v>-58.452298</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.566492</v>
+        <v>-34.572157</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -857,11 +853,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -879,14 +875,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.436255</v>
+        <v>-58.390198</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.567733</v>
+        <v>-34.637568</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -898,27 +894,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -931,13 +927,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -951,40 +943,40 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.454065</v>
+        <v>-58.400047</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.57105</v>
+        <v>-34.586358</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -994,7 +986,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1009,11 +1001,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1031,10 +1023,10 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.497446</v>
+        <v>-58.499823</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.583455</v>
+        <v>-34.563809</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1050,27 +1042,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1085,11 +1077,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1107,46 +1099,46 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.466348</v>
+        <v>-58.386058</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.556028</v>
+        <v>-34.621209</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1161,7 +1153,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1183,46 +1175,46 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.507569</v>
+        <v>-58.395465</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.579623</v>
+        <v>-34.622784</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Conesa 2195</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1237,7 +1229,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1259,46 +1251,46 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.463015</v>
+        <v>-58.394079</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.564505</v>
+        <v>-34.61051</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>-111</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>7/12/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>CATAMARCA /ALT/ 1127</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>790298182</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1313,7 +1305,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1335,14 +1327,14 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.414984</v>
+        <v>-58.404265</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.621386</v>
+        <v>-34.623154</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1354,27 +1346,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>-255</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>1/8/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Gurruchaga 410</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>802393948</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1389,11 +1381,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna para pedir traspaso de equipos</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1402,7 +1394,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1411,46 +1403,46 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.427201</v>
+        <v>-58.442601</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.617131</v>
+        <v>-34.597923</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1465,11 +1457,11 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1487,46 +1479,46 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.418089</v>
+        <v>-58.480871</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.620313</v>
+        <v>-34.616598</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Treinta y Tres Orientales 905</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1541,11 +1533,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1563,14 +1555,14 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.423229</v>
+        <v>-58.407076</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.625103</v>
+        <v>-34.616016</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1582,27 +1574,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1617,7 +1609,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1639,26 +1631,26 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.415566</v>
+        <v>-58.439727</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.613244</v>
+        <v>-34.556261</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1668,7 +1660,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>HERNANDEZ JOSE 1451</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1678,7 +1670,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>803608178</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1693,7 +1685,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1706,7 +1698,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1715,10 +1707,10 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.439727</v>
+        <v>-58.443936</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.556261</v>
+        <v>-34.560145</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1734,27 +1726,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>HERNANDEZ JOSE 1451</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1769,7 +1761,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1782,7 +1774,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1791,46 +1783,46 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.443936</v>
+        <v>-58.415566</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.560145</v>
+        <v>-34.613244</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>BAEZ 489</t>
+          <t>Treinta y Tres Orientales 905</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1845,11 +1837,11 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1867,14 +1859,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.432978</v>
+        <v>-58.423229</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.57094</v>
+        <v>-34.625103</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1886,27 +1878,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1921,7 +1913,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1943,46 +1935,46 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.499823</v>
+        <v>-58.418089</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.563809</v>
+        <v>-34.620313</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1995,7 +1987,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I21" t="n">
         <v>0</v>
       </c>
@@ -2015,14 +2011,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.400047</v>
+        <v>-58.427201</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.586358</v>
+        <v>-34.617131</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2034,27 +2030,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Lima Oeste 1649</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2073,7 +2069,7 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2090,43 +2086,47 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
+      <c r="M22" t="n">
+        <v>-58.414984</v>
+      </c>
+      <c r="N22" t="n">
+        <v>-34.621386</v>
+      </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Lima Oeste 1697</t>
+          <t>Conesa 2195</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,15 +2141,15 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2159,36 +2159,40 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M23" t="n">
+        <v>-58.463015</v>
+      </c>
+      <c r="N23" t="n">
+        <v>-34.564505</v>
+      </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2198,7 +2202,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2213,11 +2217,11 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2235,14 +2239,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.487821</v>
+        <v>-58.507569</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.554603</v>
+        <v>-34.579623</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2254,27 +2258,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2311,36 +2315,36 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.404058</v>
+        <v>-58.466348</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.634341</v>
+        <v>-34.556028</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2350,7 +2354,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2365,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2387,10 +2391,10 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.511732</v>
+        <v>-58.497446</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.578688</v>
+        <v>-34.583455</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2406,17 +2410,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-542</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Cramer 2141</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2426,7 +2430,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2441,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2459,18 +2463,18 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.461582</v>
+        <v>-58.454065</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.564296</v>
+        <v>-34.57105</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2482,27 +2486,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2539,14 +2543,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.44037</v>
+        <v>-58.436255</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.632249</v>
+        <v>-34.567733</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2558,27 +2562,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2615,14 +2619,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.440748</v>
+        <v>-58.43247</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.63245</v>
+        <v>-34.566492</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2634,17 +2638,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Soldado de la Independencia 1298</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2654,7 +2658,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2669,7 +2673,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada - Con fuente teco</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2682,7 +2686,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2691,36 +2695,36 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.434194</v>
+        <v>-58.440507</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.571754</v>
+        <v>-34.564016</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2730,7 +2734,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2767,46 +2771,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.434668</v>
+        <v>-58.44191</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.571258</v>
+        <v>-34.564245</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-510</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Larrea 590</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808194254</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2821,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2834,23 +2838,23 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.402353</v>
+        <v>-58.438744</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.602205</v>
+        <v>-34.629929</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2862,7 +2866,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-508</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2872,7 +2876,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Moldes 2463</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2882,7 +2886,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808194234</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2910,7 +2914,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2919,10 +2923,10 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.462281</v>
+        <v>-58.473937</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.560321</v>
+        <v>-34.557355</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2938,7 +2942,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-508</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2948,7 +2952,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Moldes 2463</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2958,7 +2962,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808194234</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2986,7 +2990,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2995,10 +2999,10 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.473937</v>
+        <v>-58.462281</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.557355</v>
+        <v>-34.560321</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3014,27 +3018,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-510</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Larrea 590</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>808194254</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3049,11 +3053,11 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3062,7 +3066,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -3071,14 +3075,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.390198</v>
+        <v>-58.402353</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.637568</v>
+        <v>-34.602205</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3090,27 +3094,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-28</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2/20/2024</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ZABALA /ALT/ 2836</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>780340125</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3125,11 +3129,11 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>ZABALA 2836 - Reemplazar C114</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -3147,46 +3151,46 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.452298</v>
+        <v>-58.434668</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.572157</v>
+        <v>-34.571258</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3201,7 +3205,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3223,14 +3227,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.407076</v>
+        <v>-58.434194</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.616016</v>
+        <v>-34.571754</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3242,27 +3246,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3277,7 +3281,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3295,50 +3299,50 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.480871</v>
+        <v>-58.440748</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.616598</v>
+        <v>-34.63245</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-255</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>1/8/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Gurruchaga 410</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>802393948</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3353,7 +3357,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de equipos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3366,7 +3370,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3375,46 +3379,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.442601</v>
+        <v>-58.44037</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.597923</v>
+        <v>-34.632249</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>-542</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Cramer 2141</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3427,9 +3431,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr"/>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+        </is>
+      </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -3447,46 +3455,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.39894</v>
+        <v>-58.461582</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.591084</v>
+        <v>-34.564296</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3501,11 +3509,11 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3523,46 +3531,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.390269</v>
+        <v>-58.511732</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.625079</v>
+        <v>-34.578688</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3577,11 +3585,11 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3599,10 +3607,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.404265</v>
+        <v>-58.404058</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.623154</v>
+        <v>-34.634341</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3618,27 +3626,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,11 +3661,11 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3675,46 +3683,46 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.394079</v>
+        <v>-58.487821</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.61051</v>
+        <v>-34.554603</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,15 +3737,15 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3747,14 +3755,14 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.395465</v>
+        <v>-58.382231</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.622784</v>
+        <v>-34.627676</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3770,17 +3778,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3790,7 +3798,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,11 +3813,11 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -3827,10 +3835,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.386058</v>
+        <v>-58.382261</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.621209</v>
+        <v>-34.62737</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-25 09:18:53)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1346,27 +1346,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-255</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1/8/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Gurruchaga 410</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>802393948</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de equipos</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1394,7 +1394,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1403,10 +1403,10 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.442601</v>
+        <v>-58.480871</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.597923</v>
+        <v>-34.616598</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1422,27 +1422,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1457,7 +1457,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1479,46 +1479,46 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.480871</v>
+        <v>-58.407076</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.616598</v>
+        <v>-34.616016</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1533,11 +1533,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1555,46 +1555,46 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.407076</v>
+        <v>-58.439727</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.616016</v>
+        <v>-34.556261</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1609,7 +1609,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1631,46 +1631,46 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.439727</v>
+        <v>-58.415566</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.556261</v>
+        <v>-34.613244</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>HERNANDEZ JOSE 1451</t>
+          <t>Treinta y Tres Orientales 905</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>803608178</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 y efectuar transferencias base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1698,7 +1698,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1707,36 +1707,36 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.443936</v>
+        <v>-58.423229</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.560145</v>
+        <v>-34.625103</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1783,10 +1783,10 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.415566</v>
+        <v>-58.418089</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.613244</v>
+        <v>-34.620313</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1802,17 +1802,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Treinta y Tres Orientales 905</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1822,7 +1822,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1859,14 +1859,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.423229</v>
+        <v>-58.427201</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.625103</v>
+        <v>-34.617131</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1878,7 +1878,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1898,7 +1898,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1935,14 +1935,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.418089</v>
+        <v>-58.414984</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.620313</v>
+        <v>-34.621386</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1954,27 +1954,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Conesa 2195</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2011,46 +2011,46 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.427201</v>
+        <v>-58.463015</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.617131</v>
+        <v>-34.564505</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2087,36 +2087,36 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.414984</v>
+        <v>-58.507569</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.621386</v>
+        <v>-34.579623</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Conesa 2195</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2126,7 +2126,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2145,7 +2145,7 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2163,14 +2163,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.463015</v>
+        <v>-58.466348</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.564505</v>
+        <v>-34.556028</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2182,17 +2182,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2202,7 +2202,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2221,7 +2221,7 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2239,10 +2239,10 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.507569</v>
+        <v>-58.497446</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.579623</v>
+        <v>-34.583455</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2258,17 +2258,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2278,7 +2278,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2311,18 +2311,18 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.466348</v>
+        <v>-58.454065</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.556028</v>
+        <v>-34.57105</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2334,27 +2334,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2391,46 +2391,46 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.497446</v>
+        <v>-58.436255</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.583455</v>
+        <v>-34.567733</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2467,36 +2467,36 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.454065</v>
+        <v>-58.43247</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.57105</v>
+        <v>-34.566492</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2543,46 +2543,46 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.436255</v>
+        <v>-58.44191</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.567733</v>
+        <v>-34.564245</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2619,14 +2619,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.43247</v>
+        <v>-58.438744</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.566492</v>
+        <v>-34.629929</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2638,27 +2638,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Soldado de la Independencia 1298</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada - Con fuente teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2686,7 +2686,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2695,14 +2695,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.440507</v>
+        <v>-58.473937</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.564016</v>
+        <v>-34.557355</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2714,17 +2714,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2734,7 +2734,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2771,46 +2771,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.44191</v>
+        <v>-58.434668</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.564245</v>
+        <v>-34.571258</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2843,18 +2843,18 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.438744</v>
+        <v>-58.434194</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.629929</v>
+        <v>-34.571754</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2866,27 +2866,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2919,50 +2919,50 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.473937</v>
+        <v>-58.440748</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.557355</v>
+        <v>-34.63245</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-508</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Moldes 2463</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808194234</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2990,7 +2990,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2999,46 +2999,46 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.462281</v>
+        <v>-58.44037</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.560321</v>
+        <v>-34.632249</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-510</t>
+          <t>-542</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Larrea 590</t>
+          <t>Cramer 2141</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808194254</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -3075,46 +3075,46 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.402353</v>
+        <v>-58.461582</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.602205</v>
+        <v>-34.564296</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3151,46 +3151,46 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.434668</v>
+        <v>-58.511732</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.571258</v>
+        <v>-34.578688</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3227,14 +3227,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.434194</v>
+        <v>-58.404058</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.571754</v>
+        <v>-34.634341</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3246,27 +3246,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3299,50 +3299,50 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.440748</v>
+        <v>-58.487821</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.63245</v>
+        <v>-34.554603</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3365,7 +3365,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3375,18 +3375,18 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.44037</v>
+        <v>-58.382231</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.632249</v>
+        <v>-34.627676</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3398,27 +3398,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-542</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Cramer 2141</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3455,397 +3455,17 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.461582</v>
+        <v>-58.382261</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.564296</v>
+        <v>-34.62737</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>-546</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>8/5/2025</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Albarellos 3031</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>808720857</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I41" t="n">
-        <v>1</v>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M41" t="n">
-        <v>-58.511732</v>
-      </c>
-      <c r="N41" t="n">
-        <v>-34.578688</v>
-      </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>-552</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Catulo Castillo 2890</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>808973183</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I42" t="n">
-        <v>1</v>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M42" t="n">
-        <v>-58.404058</v>
-      </c>
-      <c r="N42" t="n">
-        <v>-34.634341</v>
-      </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>-553</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Holmberg 4002</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>808973192</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
-        </is>
-      </c>
-      <c r="I43" t="n">
-        <v>1</v>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M43" t="n">
-        <v>-58.487821</v>
-      </c>
-      <c r="N43" t="n">
-        <v>-34.554603</v>
-      </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P43" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>-554</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Lima 1697</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>808973197</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>Columna inclinada</t>
-        </is>
-      </c>
-      <c r="I44" t="n">
-        <v>1</v>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M44" t="n">
-        <v>-58.382231</v>
-      </c>
-      <c r="N44" t="n">
-        <v>-34.627676</v>
-      </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P44" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>-555</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Lima 1649</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>808973201</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I45" t="n">
-        <v>1</v>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M45" t="n">
-        <v>-58.382261</v>
-      </c>
-      <c r="N45" t="n">
-        <v>-34.62737</v>
-      </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P45" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-25 12:08:40)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,6 +514,16 @@
           <t>Zona</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>PD</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>N2</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -590,6 +600,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>CON-M</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -664,6 +684,16 @@
       <c r="P3" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>BLO-H</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -738,6 +768,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>RET-E</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1RET</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -814,6 +854,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>ATH-Q</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -888,6 +938,16 @@
       <c r="P6" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>CON-K</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -962,6 +1022,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>AGU-H</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1038,6 +1108,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>PUE-?</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1114,6 +1194,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>CEN-A</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1190,6 +1280,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>CEN-B</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1266,6 +1366,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>CEN-G</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1342,6 +1452,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>CEN-K</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1418,6 +1538,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>NRA-M</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1494,6 +1624,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>CEN-J</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1570,6 +1710,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>BLO-B</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1646,6 +1796,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>CLI-I</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1722,6 +1882,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>ALM-A</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1798,6 +1968,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>ALM-B</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1874,6 +2054,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>ALM-D</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1950,6 +2140,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>CEN-P</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2026,6 +2226,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>COG-G</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2102,6 +2312,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>PUE-J</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2178,6 +2398,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>COG-L</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2254,6 +2484,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>PUE-K</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2330,6 +2570,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>ATH-H</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2406,6 +2656,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>BLO-J</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2482,6 +2742,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>BLO-I</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2558,6 +2828,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>BLO-L</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2634,6 +2914,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>PPT-P</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2710,6 +3000,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>COG-L</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2786,6 +3086,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>BLO-H</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2862,6 +3172,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>BLO-H</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2938,6 +3258,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>PPT-P</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3014,6 +3344,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>PPT-P</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3090,6 +3430,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>COG-H</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3166,6 +3516,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>PUE-J</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3242,6 +3602,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>PPT-K</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3318,6 +3688,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>COG-A</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3394,6 +3774,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>CON-M</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3468,6 +3858,16 @@
       <c r="P40" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>CON-K</t>
+        </is>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-27 09:16:16)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R40"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3358,27 +3358,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-542</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Cramer 2141</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3393,7 +3393,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3415,14 +3415,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.461582</v>
+        <v>-58.511732</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.564296</v>
+        <v>-34.578688</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3432,7 +3432,7 @@
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>COG-H</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
@@ -3444,27 +3444,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3501,24 +3501,24 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.511732</v>
+        <v>-58.404058</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.578688</v>
+        <v>-34.634341</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -3530,7 +3530,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3540,17 +3540,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3565,7 +3565,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3587,24 +3587,24 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.404058</v>
+        <v>-58.487821</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.634341</v>
+        <v>-34.554603</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
@@ -3616,7 +3616,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3626,17 +3626,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3659,7 +3659,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3669,28 +3669,28 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.487821</v>
+        <v>-58.382231</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.554603</v>
+        <v>-34.627676</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
@@ -3702,7 +3702,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3712,7 +3712,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3745,7 +3745,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3755,14 +3755,14 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.382231</v>
+        <v>-58.382261</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.627676</v>
+        <v>-34.62737</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3776,96 +3776,10 @@
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>-555</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Lima 1649</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>808973201</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I40" t="n">
-        <v>1</v>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M40" t="n">
-        <v>-58.382261</v>
-      </c>
-      <c r="N40" t="n">
-        <v>-34.62737</v>
-      </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P40" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q40" t="inlineStr">
-        <is>
-          <t>CON-K</t>
-        </is>
-      </c>
-      <c r="R40" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-10-01 08:29:07)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>-28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>2/20/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>ZABALA /ALT/ 2836</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>780340125</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,7 +563,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>ZABALA 2836 - Reemplazar C114</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -585,24 +585,24 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.390269</v>
+        <v>-58.452298</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.625079</v>
+        <v>-34.572157</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>ATH-Q</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -614,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BAEZ 489</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -649,11 +649,11 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -671,14 +671,14 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.432978</v>
+        <v>-58.394079</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.57094</v>
+        <v>-34.61051</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -700,27 +700,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -733,9 +733,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -749,60 +753,60 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.39894</v>
+        <v>-58.454065</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.591084</v>
+        <v>-34.57105</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>RET-E</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-28</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2/20/2024</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ZABALA /ALT/ 2836</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>780340125</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -817,7 +821,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>ZABALA 2836 - Reemplazar C114</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -839,24 +843,24 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.452298</v>
+        <v>-58.390198</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.572157</v>
+        <v>-34.637568</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>ATH-Q</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -868,27 +872,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Treinta y Tres Orientales 905</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -903,7 +907,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -925,14 +929,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.390198</v>
+        <v>-58.423229</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.637568</v>
+        <v>-34.625103</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -942,7 +946,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>ALM-A</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -954,27 +958,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -987,9 +991,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1003,18 +1011,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.400047</v>
+        <v>-58.440748</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.586358</v>
+        <v>-34.63245</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1024,7 +1032,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1036,27 +1044,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1071,11 +1079,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1093,24 +1101,24 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.499823</v>
+        <v>-58.44037</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.563809</v>
+        <v>-34.632249</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1122,27 +1130,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1157,11 +1165,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1179,24 +1187,24 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.386058</v>
+        <v>-58.473937</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.621209</v>
+        <v>-34.557355</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1294,27 +1302,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1329,7 +1337,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1351,10 +1359,10 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.394079</v>
+        <v>-58.427201</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.61051</v>
+        <v>-34.617131</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1368,7 +1376,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1380,27 +1388,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1415,11 +1423,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1437,24 +1445,24 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.404265</v>
+        <v>-58.466348</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.623154</v>
+        <v>-34.556028</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>CEN-K</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1466,27 +1474,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1501,11 +1509,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1523,24 +1531,24 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.480871</v>
+        <v>-58.414984</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.616598</v>
+        <v>-34.621386</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1552,27 +1560,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1587,7 +1595,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1609,14 +1617,14 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.407076</v>
+        <v>-58.434668</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.616016</v>
+        <v>-34.571258</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1626,7 +1634,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1638,27 +1646,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1673,11 +1681,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1695,24 +1703,24 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.439727</v>
+        <v>-58.434194</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.556261</v>
+        <v>-34.571754</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1724,27 +1732,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1763,7 +1771,7 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1781,24 +1789,24 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.415566</v>
+        <v>-58.44191</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.613244</v>
+        <v>-34.564245</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>BLO-L</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1810,27 +1818,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Treinta y Tres Orientales 905</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1845,15 +1853,15 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1863,18 +1871,18 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.423229</v>
+        <v>-58.382231</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.625103</v>
+        <v>-34.627676</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1884,7 +1892,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>ALM-A</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1896,27 +1904,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1935,7 +1943,7 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1953,14 +1961,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.418089</v>
+        <v>-58.382261</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.620313</v>
+        <v>-34.62737</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1970,7 +1978,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1982,27 +1990,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2017,7 +2025,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -2039,24 +2047,24 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.427201</v>
+        <v>-58.439727</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.617131</v>
+        <v>-34.556261</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2068,27 +2076,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2103,7 +2111,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -2125,14 +2133,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.414984</v>
+        <v>-58.386058</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.621386</v>
+        <v>-34.621209</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2142,7 +2150,7 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2154,27 +2162,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Conesa 2195</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2189,11 +2197,11 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2211,14 +2219,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.463015</v>
+        <v>-58.487821</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.564505</v>
+        <v>-34.554603</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2228,7 +2236,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>COG-G</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2240,27 +2248,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2275,11 +2283,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2297,10 +2305,10 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.507569</v>
+        <v>-58.480871</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.579623</v>
+        <v>-34.616598</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2314,7 +2322,7 @@
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2326,27 +2334,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2359,13 +2367,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2383,56 +2387,56 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.466348</v>
+        <v>-58.39894</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.556028</v>
+        <v>-34.591084</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>RET-E</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2465,28 +2469,28 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.497446</v>
+        <v>-58.438744</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.583455</v>
+        <v>-34.629929</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,27 +2502,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2533,7 +2537,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2551,28 +2555,28 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.454065</v>
+        <v>-58.407076</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.57105</v>
+        <v>-34.616016</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,27 +2588,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2619,11 +2623,11 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2641,14 +2645,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.436255</v>
+        <v>-58.390269</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.567733</v>
+        <v>-34.625079</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2658,7 +2662,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,27 +2674,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>Conesa 2195</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2709,7 +2713,7 @@
         </is>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2723,28 +2727,28 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.43247</v>
+        <v>-58.463015</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.566492</v>
+        <v>-34.564505</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>BLO-I</t>
+          <t>COG-G</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2760,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2795,7 +2799,7 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2813,24 +2817,24 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.44191</v>
+        <v>-58.418089</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.564245</v>
+        <v>-34.620313</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>BLO-L</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,27 +2846,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2881,7 +2885,7 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2895,28 +2899,28 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.438744</v>
+        <v>-58.507569</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.629929</v>
+        <v>-34.579623</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2928,27 +2932,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2985,24 +2989,24 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.473937</v>
+        <v>-58.404058</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.557355</v>
+        <v>-34.634341</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3014,27 +3018,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-111</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>7/12/2024</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>CATAMARCA /ALT/ 1127</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>790298182</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3049,11 +3053,11 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3071,14 +3075,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.434668</v>
+        <v>-58.404265</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.571258</v>
+        <v>-34.623154</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3088,7 +3092,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-K</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3100,17 +3104,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -3120,7 +3124,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3153,14 +3157,14 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.434194</v>
+        <v>-58.43247</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.571754</v>
+        <v>-34.566492</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3174,7 +3178,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>BLO-I</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3186,27 +3190,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>BAEZ 489</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3221,7 +3225,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -3239,18 +3243,18 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.440748</v>
+        <v>-58.432978</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.63245</v>
+        <v>-34.57094</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -3260,7 +3264,7 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3272,27 +3276,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3311,7 +3315,7 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3329,14 +3333,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.44037</v>
+        <v>-58.415566</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.632249</v>
+        <v>-34.613244</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3346,7 +3350,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -3358,17 +3362,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -3378,7 +3382,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3393,7 +3397,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3415,10 +3419,10 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.511732</v>
+        <v>-58.497446</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.578688</v>
+        <v>-34.583455</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -3432,7 +3436,7 @@
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
@@ -3444,27 +3448,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3501,14 +3505,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.404058</v>
+        <v>-58.436255</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.634341</v>
+        <v>-34.567733</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3518,7 +3522,7 @@
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -3530,17 +3534,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -3550,7 +3554,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3565,11 +3569,11 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -3587,14 +3591,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.487821</v>
+        <v>-58.499823</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.554603</v>
+        <v>-34.563809</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3604,7 +3608,7 @@
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
@@ -3616,27 +3620,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3651,7 +3655,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3659,7 +3663,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3669,28 +3673,28 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.382231</v>
+        <v>-58.511732</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.627676</v>
+        <v>-34.578688</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
@@ -3702,27 +3706,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Lima 1649</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3735,13 +3739,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H39" t="inlineStr"/>
       <c r="I39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -3759,14 +3759,14 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.382261</v>
+        <v>-58.400047</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.62737</v>
+        <v>-34.586358</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3776,7 +3776,7 @@
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-10-02 08:57:20)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-28</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2/20/2024</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ZABALA /ALT/ 2836</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>780340125</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,7 +563,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>ZABALA 2836 - Reemplazar C114</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -585,24 +585,24 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.452298</v>
+        <v>-58.390269</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.572157</v>
+        <v>-34.625079</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>ATH-Q</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -614,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>BAEZ 489</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -649,11 +649,11 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -671,14 +671,14 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.394079</v>
+        <v>-58.432978</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.61051</v>
+        <v>-34.57094</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -700,27 +700,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -733,13 +733,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -753,60 +749,60 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.454065</v>
+        <v>-58.39894</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.57105</v>
+        <v>-34.591084</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>RET-E</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-28</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>2/20/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>ZABALA /ALT/ 2836</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>780340125</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -821,7 +817,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>ZABALA 2836 - Reemplazar C114</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -843,24 +839,24 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.390198</v>
+        <v>-58.452298</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.637568</v>
+        <v>-34.572157</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>ATH-Q</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -872,27 +868,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Treinta y Tres Orientales 905</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -907,7 +903,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -929,14 +925,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.423229</v>
+        <v>-58.390198</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.625103</v>
+        <v>-34.637568</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -946,7 +942,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>ALM-A</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -958,27 +954,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -991,13 +987,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1011,18 +1003,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.440748</v>
+        <v>-58.400047</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.63245</v>
+        <v>-34.586358</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1032,7 +1024,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1044,27 +1036,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1079,11 +1071,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1101,24 +1093,24 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.44037</v>
+        <v>-58.499823</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.632249</v>
+        <v>-34.563809</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1130,27 +1122,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1165,11 +1157,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1187,24 +1179,24 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.473937</v>
+        <v>-58.386058</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.557355</v>
+        <v>-34.621209</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1302,27 +1294,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1337,7 +1329,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1359,10 +1351,10 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.427201</v>
+        <v>-58.394079</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.617131</v>
+        <v>-34.61051</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1376,7 +1368,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1388,27 +1380,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>-111</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>7/12/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>CATAMARCA /ALT/ 1127</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>790298182</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1423,11 +1415,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1445,24 +1437,24 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.466348</v>
+        <v>-58.404265</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.556028</v>
+        <v>-34.623154</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CEN-K</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1474,27 +1466,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1509,11 +1501,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1531,24 +1523,24 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.414984</v>
+        <v>-58.480871</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.621386</v>
+        <v>-34.616598</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1560,27 +1552,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1595,7 +1587,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1617,14 +1609,14 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.434668</v>
+        <v>-58.407076</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.571258</v>
+        <v>-34.616016</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1634,7 +1626,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1646,27 +1638,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1681,11 +1673,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1703,24 +1695,24 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.434194</v>
+        <v>-58.439727</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.571754</v>
+        <v>-34.556261</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1732,27 +1724,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1771,7 +1763,7 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1789,24 +1781,24 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.44191</v>
+        <v>-58.415566</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.564245</v>
+        <v>-34.613244</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>BLO-L</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1818,27 +1810,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>Treinta y Tres Orientales 905</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1853,15 +1845,15 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1871,18 +1863,18 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.382231</v>
+        <v>-58.423229</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.627676</v>
+        <v>-34.625103</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1892,7 +1884,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>ALM-A</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1904,27 +1896,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Lima 1649</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1943,7 +1935,7 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1961,14 +1953,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.382261</v>
+        <v>-58.418089</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.62737</v>
+        <v>-34.620313</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1978,7 +1970,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1990,27 +1982,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2025,7 +2017,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -2047,24 +2039,24 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.439727</v>
+        <v>-58.427201</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.556261</v>
+        <v>-34.617131</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2076,27 +2068,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2111,7 +2103,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -2133,14 +2125,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.386058</v>
+        <v>-58.414984</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.621209</v>
+        <v>-34.621386</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2150,7 +2142,7 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2162,27 +2154,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Conesa 2195</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>804427439</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2197,11 +2189,11 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2219,14 +2211,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.487821</v>
+        <v>-58.463015</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.554603</v>
+        <v>-34.564505</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2236,7 +2228,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>COG-G</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2248,27 +2240,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2283,11 +2275,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2305,10 +2297,10 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.480871</v>
+        <v>-58.507569</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.616598</v>
+        <v>-34.579623</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2322,7 +2314,7 @@
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2334,27 +2326,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2367,9 +2359,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2387,56 +2383,56 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.39894</v>
+        <v>-58.466348</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.591084</v>
+        <v>-34.556028</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>RET-E</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2469,28 +2465,28 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.438744</v>
+        <v>-58.497446</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.629929</v>
+        <v>-34.583455</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2502,27 +2498,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2537,7 +2533,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2555,28 +2551,28 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.407076</v>
+        <v>-58.454065</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.616016</v>
+        <v>-34.57105</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2588,27 +2584,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2623,11 +2619,11 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2645,14 +2641,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.390269</v>
+        <v>-58.436255</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.625079</v>
+        <v>-34.567733</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2662,7 +2658,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2674,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Conesa 2195</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2713,7 +2709,7 @@
         </is>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2727,28 +2723,28 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.463015</v>
+        <v>-58.43247</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.564505</v>
+        <v>-34.566492</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>COG-G</t>
+          <t>BLO-I</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2760,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2799,7 +2795,7 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2817,24 +2813,24 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.418089</v>
+        <v>-58.44191</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.620313</v>
+        <v>-34.564245</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>BLO-L</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2846,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2885,7 +2881,7 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2899,28 +2895,28 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.507569</v>
+        <v>-58.438744</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.579623</v>
+        <v>-34.629929</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2932,27 +2928,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2989,24 +2985,24 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.404058</v>
+        <v>-58.473937</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.634341</v>
+        <v>-34.557355</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3018,27 +3014,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3053,11 +3049,11 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3075,14 +3071,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.404265</v>
+        <v>-58.434668</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.623154</v>
+        <v>-34.571258</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3092,7 +3088,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>CEN-K</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3104,17 +3100,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -3124,7 +3120,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3157,14 +3153,14 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.43247</v>
+        <v>-58.434194</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.566492</v>
+        <v>-34.571754</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3178,7 +3174,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>BLO-I</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3190,27 +3186,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>BAEZ 489</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3225,7 +3221,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -3243,18 +3239,18 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.432978</v>
+        <v>-58.440748</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.57094</v>
+        <v>-34.63245</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -3264,7 +3260,7 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3276,27 +3272,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3315,7 +3311,7 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3333,14 +3329,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.415566</v>
+        <v>-58.44037</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.613244</v>
+        <v>-34.632249</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3350,7 +3346,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -3362,17 +3358,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -3382,7 +3378,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3397,7 +3393,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3419,10 +3415,10 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.497446</v>
+        <v>-58.511732</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.583455</v>
+        <v>-34.578688</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -3436,7 +3432,7 @@
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
@@ -3448,27 +3444,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3505,14 +3501,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.436255</v>
+        <v>-58.404058</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.567733</v>
+        <v>-34.634341</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3522,7 +3518,7 @@
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -3534,17 +3530,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -3554,7 +3550,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3569,11 +3565,11 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -3591,14 +3587,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.499823</v>
+        <v>-58.487821</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.563809</v>
+        <v>-34.554603</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3608,7 +3604,7 @@
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
@@ -3620,27 +3616,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3655,7 +3651,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3663,7 +3659,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3673,28 +3669,28 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.511732</v>
+        <v>-58.382231</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.578688</v>
+        <v>-34.627676</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
@@ -3706,27 +3702,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3739,9 +3735,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr"/>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -3759,14 +3759,14 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.400047</v>
+        <v>-58.382261</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.586358</v>
+        <v>-34.62737</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3776,7 +3776,7 @@
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-10-07 09:01:45)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R39"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,16 +514,6 @@
           <t>Zona</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>PD</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>N2</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -600,16 +590,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>CON-M</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -684,16 +664,6 @@
       <c r="P3" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>BLO-H</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -768,16 +738,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>RET-E</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.1RET</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -854,16 +814,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>ATH-Q</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -938,16 +888,6 @@
       <c r="P6" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>CON-K</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -1022,16 +962,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>AGU-H</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1108,16 +1038,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>PUE-?</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1194,16 +1114,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>CEN-A</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1280,16 +1190,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>CEN-B</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1366,16 +1266,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>CEN-G</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1452,16 +1342,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>CEN-K</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1538,16 +1418,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>NRA-M</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1624,16 +1494,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>CEN-J</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1710,16 +1570,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>BLO-B</t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1796,16 +1646,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>CLI-I</t>
-        </is>
-      </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1882,16 +1722,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>ALM-A</t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1968,16 +1798,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>ALM-B</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2054,16 +1874,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>ALM-D</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2140,16 +1950,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>CEN-P</t>
-        </is>
-      </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2226,16 +2026,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>COG-G</t>
-        </is>
-      </c>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2312,16 +2102,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>PUE-J</t>
-        </is>
-      </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2398,16 +2178,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>COG-L</t>
-        </is>
-      </c>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2484,16 +2254,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>PUE-K</t>
-        </is>
-      </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2570,16 +2330,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>ATH-H</t>
-        </is>
-      </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2656,16 +2406,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>BLO-J</t>
-        </is>
-      </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2742,16 +2482,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>BLO-I</t>
-        </is>
-      </c>
-      <c r="R27" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2828,16 +2558,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>BLO-L</t>
-        </is>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2914,16 +2634,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>PPT-P</t>
-        </is>
-      </c>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3000,16 +2710,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>COG-L</t>
-        </is>
-      </c>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3086,16 +2786,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>BLO-H</t>
-        </is>
-      </c>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3172,16 +2862,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>BLO-H</t>
-        </is>
-      </c>
-      <c r="R32" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3258,16 +2938,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q33" t="inlineStr">
-        <is>
-          <t>PPT-P</t>
-        </is>
-      </c>
-      <c r="R33" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3344,16 +3014,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>PPT-P</t>
-        </is>
-      </c>
-      <c r="R34" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3430,16 +3090,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>PUE-J</t>
-        </is>
-      </c>
-      <c r="R35" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3516,16 +3166,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>PPT-K</t>
-        </is>
-      </c>
-      <c r="R36" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3602,16 +3242,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>COG-A</t>
-        </is>
-      </c>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3688,16 +3318,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>CON-M</t>
-        </is>
-      </c>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3772,16 +3392,6 @@
       <c r="P39" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>CON-K</t>
-        </is>
-      </c>
-      <c r="R39" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-10-08 08:23:58)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,6 +514,16 @@
           <t>Zona</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>PD</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>N2</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -590,6 +600,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>CON-M</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -664,6 +684,16 @@
       <c r="P3" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>BLO-H</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -738,6 +768,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>RET-E</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1RET</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -814,6 +854,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>ATH-Q</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -888,6 +938,16 @@
       <c r="P6" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>CON-K</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -962,6 +1022,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>AGU-H</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1038,6 +1108,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>PUE-?</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1114,6 +1194,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>CEN-A</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1190,6 +1280,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>CEN-B</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1266,6 +1366,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>CEN-G</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1342,6 +1452,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>CEN-K</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1418,6 +1538,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>NRA-M</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1494,6 +1624,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>CEN-J</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1570,6 +1710,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>BLO-B</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1646,6 +1796,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>CLI-I</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1722,6 +1882,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>ALM-A</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1798,6 +1968,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>ALM-B</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1874,6 +2054,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>ALM-D</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1950,6 +2140,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>CEN-P</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2026,6 +2226,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>COG-G</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2102,6 +2312,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>PUE-J</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2178,6 +2398,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>COG-L</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2254,6 +2484,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>PUE-K</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2330,6 +2570,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>ATH-H</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2406,6 +2656,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>BLO-J</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2482,6 +2742,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>BLO-I</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2558,6 +2828,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>BLO-L</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2634,6 +2914,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>PPT-P</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2710,6 +3000,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>COG-L</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2786,6 +3086,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>BLO-H</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2862,6 +3172,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>BLO-H</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2938,6 +3258,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>PPT-P</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3014,6 +3344,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>PPT-P</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3090,6 +3430,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>PUE-J</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3166,6 +3516,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>PPT-K</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3242,6 +3602,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>COG-A</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3318,6 +3688,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>CON-M</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3392,6 +3772,16 @@
       <c r="P39" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>CON-K</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-10-08 14:22:42)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R39"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2154,7 +2154,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2164,17 +2164,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Conesa 2195</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804427439</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2189,7 +2189,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2211,14 +2211,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.463015</v>
+        <v>-58.507569</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.564505</v>
+        <v>-34.579623</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2228,7 +2228,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>COG-G</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2240,27 +2240,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2275,11 +2275,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2297,14 +2297,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.507569</v>
+        <v>-58.466348</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.579623</v>
+        <v>-34.556028</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2314,7 +2314,7 @@
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2326,27 +2326,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2383,14 +2383,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.466348</v>
+        <v>-58.497446</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.556028</v>
+        <v>-34.583455</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2400,7 +2400,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2412,27 +2412,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2465,18 +2465,18 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.497446</v>
+        <v>-58.454065</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.583455</v>
+        <v>-34.57105</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2486,7 +2486,7 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,27 +2498,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2551,28 +2551,28 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.454065</v>
+        <v>-58.436255</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.57105</v>
+        <v>-34.567733</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,7 +2584,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2594,7 +2594,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2604,7 +2604,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2637,14 +2637,14 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.436255</v>
+        <v>-58.43247</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.567733</v>
+        <v>-34.566492</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2658,7 +2658,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>BLO-I</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,17 +2670,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2690,7 +2690,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2723,28 +2723,28 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.43247</v>
+        <v>-58.44191</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.566492</v>
+        <v>-34.564245</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>BLO-I</t>
+          <t>BLO-L</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2809,28 +2809,28 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.44191</v>
+        <v>-58.438744</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.564245</v>
+        <v>-34.629929</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>BLO-L</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2877,7 +2877,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2895,28 +2895,28 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.438744</v>
+        <v>-58.473937</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.629929</v>
+        <v>-34.557355</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2928,27 +2928,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2985,24 +2985,24 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.473937</v>
+        <v>-58.434668</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.557355</v>
+        <v>-34.571258</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3014,17 +3014,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -3034,7 +3034,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3071,10 +3071,10 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.434668</v>
+        <v>-58.434194</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.571258</v>
+        <v>-34.571754</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -3100,27 +3100,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3153,18 +3153,18 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.434194</v>
+        <v>-58.440748</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.571754</v>
+        <v>-34.63245</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -3174,7 +3174,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3186,7 +3186,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3196,7 +3196,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -3206,7 +3206,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3239,14 +3239,14 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.440748</v>
+        <v>-58.44037</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.63245</v>
+        <v>-34.632249</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -3272,27 +3272,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3329,24 +3329,24 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.44037</v>
+        <v>-58.511732</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.632249</v>
+        <v>-34.578688</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -3358,27 +3358,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3415,24 +3415,24 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.511732</v>
+        <v>-58.404058</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.578688</v>
+        <v>-34.634341</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
@@ -3444,7 +3444,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3454,17 +3454,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3479,7 +3479,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3501,24 +3501,24 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.404058</v>
+        <v>-58.487821</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.634341</v>
+        <v>-34.554603</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -3530,7 +3530,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3540,17 +3540,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3565,7 +3565,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3573,7 +3573,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3583,28 +3583,28 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.487821</v>
+        <v>-58.382231</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.554603</v>
+        <v>-34.627676</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
@@ -3616,7 +3616,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3626,7 +3626,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3636,7 +3636,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3659,7 +3659,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3669,14 +3669,14 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.382231</v>
+        <v>-58.382261</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.627676</v>
+        <v>-34.62737</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3690,96 +3690,10 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>-555</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Lima 1649</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>808973201</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I39" t="n">
-        <v>1</v>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M39" t="n">
-        <v>-58.382261</v>
-      </c>
-      <c r="N39" t="n">
-        <v>-34.62737</v>
-      </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P39" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>CON-K</t>
-        </is>
-      </c>
-      <c r="R39" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-17 20:17:24)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="INCO" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="INCO" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-23 08:09:45)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -614,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BAEZ 489</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -649,11 +649,11 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -671,14 +671,14 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.432978</v>
+        <v>-58.386058</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.57094</v>
+        <v>-34.621209</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -700,27 +700,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -733,13 +733,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Columna inclinada</t>
+        </is>
+      </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -749,18 +753,18 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.39894</v>
+        <v>-58.382231</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.591084</v>
+        <v>-34.627676</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -770,39 +774,39 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>RET-E</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-28</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2/20/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ZABALA /ALT/ 2836</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>780340125</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -817,11 +821,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>ZABALA 2836 - Reemplazar C114</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -839,24 +843,24 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.452298</v>
+        <v>-58.382261</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.572157</v>
+        <v>-34.62737</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>ATH-Q</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -868,27 +872,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -903,11 +907,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -925,24 +929,24 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.390198</v>
+        <v>-58.480871</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.637568</v>
+        <v>-34.616598</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -954,7 +958,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -964,17 +968,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -987,7 +991,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Para cambiar columna fte al 3688</t>
+        </is>
+      </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
@@ -1007,24 +1015,24 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.400047</v>
+        <v>-58.499823</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.586358</v>
+        <v>-34.563809</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1036,17 +1044,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1056,7 +1064,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1071,7 +1079,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1093,10 +1101,10 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.499823</v>
+        <v>-58.507569</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.563809</v>
+        <v>-34.579623</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1110,7 +1118,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1122,27 +1130,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1157,11 +1165,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1179,24 +1187,24 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.386058</v>
+        <v>-58.497446</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.621209</v>
+        <v>-34.583455</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1208,27 +1216,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1243,11 +1251,11 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1265,24 +1273,24 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.395465</v>
+        <v>-58.473937</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.622784</v>
+        <v>-34.557355</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1294,27 +1302,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1329,11 +1337,11 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1351,24 +1359,24 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.394079</v>
+        <v>-58.511732</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.61051</v>
+        <v>-34.578688</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1380,27 +1388,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1415,11 +1423,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1437,24 +1445,24 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.404265</v>
+        <v>-58.487821</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.623154</v>
+        <v>-34.554603</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>CEN-K</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1466,27 +1474,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-28</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>2/20/2024</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>ZABALA /ALT/ 2836</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>780340125</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1501,11 +1509,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>ZABALA 2836 - Reemplazar C114</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1523,14 +1531,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.480871</v>
+        <v>-58.452298</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.616598</v>
+        <v>-34.572157</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1540,7 +1548,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>ATH-Q</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1552,27 +1560,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1587,11 +1595,11 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1609,24 +1617,24 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.407076</v>
+        <v>-58.439727</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.616016</v>
+        <v>-34.556261</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1638,17 +1646,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1658,7 +1666,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1673,11 +1681,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1695,10 +1703,10 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.439727</v>
+        <v>-58.466348</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.556261</v>
+        <v>-34.556028</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1712,7 +1720,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1724,27 +1732,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1763,7 +1771,7 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1777,28 +1785,28 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.415566</v>
+        <v>-58.454065</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.613244</v>
+        <v>-34.57105</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1810,27 +1818,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Treinta y Tres Orientales 905</t>
+          <t>BAEZ 489</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1845,11 +1853,11 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1867,14 +1875,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.423229</v>
+        <v>-58.432978</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.625103</v>
+        <v>-34.57094</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1884,7 +1892,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>ALM-A</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1896,27 +1904,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1935,7 +1943,7 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1953,14 +1961,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.418089</v>
+        <v>-58.436255</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.620313</v>
+        <v>-34.567733</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1970,7 +1978,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1982,27 +1990,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2021,7 +2029,7 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2035,18 +2043,18 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.427201</v>
+        <v>-58.43247</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.617131</v>
+        <v>-34.566492</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2056,7 +2064,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>BLO-I</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2068,27 +2076,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2107,7 +2115,7 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2125,24 +2133,24 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.414984</v>
+        <v>-58.44191</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.621386</v>
+        <v>-34.564245</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>BLO-L</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2154,27 +2162,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2189,11 +2197,11 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2211,24 +2219,24 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.507569</v>
+        <v>-58.434668</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.579623</v>
+        <v>-34.571258</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2240,27 +2248,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2297,24 +2305,24 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.466348</v>
+        <v>-58.434194</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.556028</v>
+        <v>-34.571754</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2326,27 +2334,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2359,13 +2367,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2383,56 +2387,56 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.497446</v>
+        <v>-58.39894</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.583455</v>
+        <v>-34.591084</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>RET-E</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2445,13 +2449,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2465,28 +2465,28 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.454065</v>
+        <v>-58.400047</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.57105</v>
+        <v>-34.586358</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,27 +2498,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2533,11 +2533,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2555,14 +2555,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.436255</v>
+        <v>-58.395465</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.567733</v>
+        <v>-34.622784</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2572,7 +2572,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,27 +2584,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2619,11 +2619,11 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2637,18 +2637,18 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.43247</v>
+        <v>-58.394079</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.566492</v>
+        <v>-34.61051</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>BLO-I</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>-111</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>7/12/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>CATAMARCA /ALT/ 1127</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>790298182</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2705,11 +2705,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2727,24 +2727,24 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.44191</v>
+        <v>-58.404265</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.564245</v>
+        <v>-34.623154</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>BLO-L</t>
+          <t>CEN-K</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2809,18 +2809,18 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.438744</v>
+        <v>-58.407076</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.629929</v>
+        <v>-34.616016</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2830,7 +2830,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2877,11 +2877,11 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2899,24 +2899,24 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.473937</v>
+        <v>-58.390198</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.557355</v>
+        <v>-34.637568</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2928,27 +2928,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2985,14 +2985,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.434668</v>
+        <v>-58.404058</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.571258</v>
+        <v>-34.634341</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -3002,7 +3002,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3014,27 +3014,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3053,7 +3053,7 @@
         </is>
       </c>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3071,14 +3071,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.434194</v>
+        <v>-58.415566</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.571754</v>
+        <v>-34.613244</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3088,7 +3088,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3100,27 +3100,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>Treinta y Tres Orientales 905</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3139,7 +3139,7 @@
         </is>
       </c>
       <c r="I32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3153,14 +3153,14 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.440748</v>
+        <v>-58.423229</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.63245</v>
+        <v>-34.625103</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3174,7 +3174,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>ALM-A</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3186,27 +3186,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3225,7 +3225,7 @@
         </is>
       </c>
       <c r="I33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3243,14 +3243,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.44037</v>
+        <v>-58.418089</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.632249</v>
+        <v>-34.620313</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3272,27 +3272,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3311,7 +3311,7 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3329,24 +3329,24 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.511732</v>
+        <v>-58.427201</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.578688</v>
+        <v>-34.617131</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -3358,27 +3358,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3397,7 +3397,7 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3415,14 +3415,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.404058</v>
+        <v>-58.414984</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.634341</v>
+        <v>-34.621386</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3432,7 +3432,7 @@
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
@@ -3444,27 +3444,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3479,7 +3479,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3497,28 +3497,28 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.487821</v>
+        <v>-58.438744</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.554603</v>
+        <v>-34.629929</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -3530,27 +3530,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3565,7 +3565,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3573,7 +3573,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3587,14 +3587,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.382231</v>
+        <v>-58.440748</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.627676</v>
+        <v>-34.63245</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3604,7 +3604,7 @@
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
@@ -3616,27 +3616,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Lima 1649</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3673,14 +3673,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.382261</v>
+        <v>-58.44037</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.62737</v>
+        <v>-34.632249</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3690,7 +3690,7 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-24 15:35:17)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -614,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>BAEZ 489</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -649,11 +649,11 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -671,14 +671,14 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.386058</v>
+        <v>-58.432978</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.621209</v>
+        <v>-34.57094</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -700,27 +700,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -733,17 +733,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Columna inclinada</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -753,18 +749,18 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.382231</v>
+        <v>-58.39894</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.627676</v>
+        <v>-34.591084</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -774,39 +770,39 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>RET-E</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-28</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/20/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Lima 1649</t>
+          <t>ZABALA /ALT/ 2836</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>780340125</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -821,11 +817,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>ZABALA 2836 - Reemplazar C114</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -843,24 +839,24 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.382261</v>
+        <v>-58.452298</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.62737</v>
+        <v>-34.572157</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>ATH-Q</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -872,27 +868,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -907,11 +903,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -929,24 +925,24 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.480871</v>
+        <v>-58.390198</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.616598</v>
+        <v>-34.637568</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -958,7 +954,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -968,17 +964,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -991,11 +987,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Para cambiar columna fte al 3688</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
         <v>0</v>
       </c>
@@ -1015,24 +1007,24 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.499823</v>
+        <v>-58.400047</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.563809</v>
+        <v>-34.586358</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1044,17 +1036,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1064,7 +1056,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1079,7 +1071,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1101,10 +1093,10 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.507569</v>
+        <v>-58.499823</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.579623</v>
+        <v>-34.563809</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1118,7 +1110,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1130,27 +1122,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1165,11 +1157,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1187,24 +1179,24 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.497446</v>
+        <v>-58.386058</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.583455</v>
+        <v>-34.621209</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1216,27 +1208,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1251,11 +1243,11 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1273,24 +1265,24 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.473937</v>
+        <v>-58.395465</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.557355</v>
+        <v>-34.622784</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1302,27 +1294,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1337,11 +1329,11 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1359,24 +1351,24 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.511732</v>
+        <v>-58.394079</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.578688</v>
+        <v>-34.61051</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1388,27 +1380,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-111</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>7/12/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>CATAMARCA /ALT/ 1127</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>790298182</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1423,11 +1415,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1445,24 +1437,24 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.487821</v>
+        <v>-58.404265</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.554603</v>
+        <v>-34.623154</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>CEN-K</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1474,27 +1466,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-28</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2/20/2024</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ZABALA /ALT/ 2836</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>780340125</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1509,11 +1501,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>ZABALA 2836 - Reemplazar C114</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1531,14 +1523,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.452298</v>
+        <v>-58.480871</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.572157</v>
+        <v>-34.616598</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1548,7 +1540,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>ATH-Q</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1560,27 +1552,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1595,11 +1587,11 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1617,24 +1609,24 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.439727</v>
+        <v>-58.407076</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.556261</v>
+        <v>-34.616016</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1646,17 +1638,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1666,7 +1658,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1681,11 +1673,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1703,10 +1695,10 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.466348</v>
+        <v>-58.439727</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.556028</v>
+        <v>-34.556261</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1720,7 +1712,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1732,27 +1724,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1771,7 +1763,7 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1785,28 +1777,28 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.454065</v>
+        <v>-58.415566</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.57105</v>
+        <v>-34.613244</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1818,27 +1810,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>BAEZ 489</t>
+          <t>Treinta y Tres Orientales 905</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1853,11 +1845,11 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1875,14 +1867,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.432978</v>
+        <v>-58.423229</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.57094</v>
+        <v>-34.625103</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1892,7 +1884,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>ALM-A</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1904,27 +1896,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1943,7 +1935,7 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1961,14 +1953,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.436255</v>
+        <v>-58.418089</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.567733</v>
+        <v>-34.620313</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1978,7 +1970,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1990,27 +1982,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2029,7 +2021,7 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2043,18 +2035,18 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.43247</v>
+        <v>-58.427201</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.566492</v>
+        <v>-34.617131</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2064,7 +2056,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>BLO-I</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2076,27 +2068,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2115,7 +2107,7 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2133,24 +2125,24 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.44191</v>
+        <v>-58.414984</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.564245</v>
+        <v>-34.621386</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>BLO-L</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2162,27 +2154,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2197,11 +2189,11 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2219,24 +2211,24 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.434668</v>
+        <v>-58.507569</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.571258</v>
+        <v>-34.579623</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2248,27 +2240,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2305,24 +2297,24 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.434194</v>
+        <v>-58.466348</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.571754</v>
+        <v>-34.556028</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2334,27 +2326,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2367,9 +2359,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2387,56 +2383,56 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.39894</v>
+        <v>-58.497446</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.591084</v>
+        <v>-34.583455</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>RET-E</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2449,9 +2445,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr"/>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2465,28 +2465,28 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.400047</v>
+        <v>-58.454065</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.586358</v>
+        <v>-34.57105</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,27 +2498,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2533,11 +2533,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2555,14 +2555,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.395465</v>
+        <v>-58.436255</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.622784</v>
+        <v>-34.567733</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2572,7 +2572,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,27 +2584,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2619,11 +2619,11 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2637,18 +2637,18 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.394079</v>
+        <v>-58.43247</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.61051</v>
+        <v>-34.566492</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>BLO-I</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2705,11 +2705,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2727,24 +2727,24 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.404265</v>
+        <v>-58.44191</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.623154</v>
+        <v>-34.564245</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>CEN-K</t>
+          <t>BLO-L</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2809,18 +2809,18 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.407076</v>
+        <v>-58.438744</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.616016</v>
+        <v>-34.629929</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2830,7 +2830,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2877,11 +2877,11 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2899,24 +2899,24 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.390198</v>
+        <v>-58.473937</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.637568</v>
+        <v>-34.557355</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2928,27 +2928,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2985,14 +2985,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.404058</v>
+        <v>-58.434668</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.634341</v>
+        <v>-34.571258</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -3002,7 +3002,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3014,27 +3014,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3053,7 +3053,7 @@
         </is>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3071,14 +3071,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.415566</v>
+        <v>-58.434194</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.613244</v>
+        <v>-34.571754</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3088,7 +3088,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3100,27 +3100,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Treinta y Tres Orientales 905</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3139,7 +3139,7 @@
         </is>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3153,14 +3153,14 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.423229</v>
+        <v>-58.440748</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.625103</v>
+        <v>-34.63245</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3174,7 +3174,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>ALM-A</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3186,27 +3186,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3225,7 +3225,7 @@
         </is>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3243,14 +3243,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.418089</v>
+        <v>-58.44037</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.620313</v>
+        <v>-34.632249</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3272,27 +3272,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3311,7 +3311,7 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3329,24 +3329,24 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.427201</v>
+        <v>-58.511732</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.617131</v>
+        <v>-34.578688</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -3358,27 +3358,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3397,7 +3397,7 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3415,14 +3415,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.414984</v>
+        <v>-58.404058</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.621386</v>
+        <v>-34.634341</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3432,7 +3432,7 @@
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
@@ -3444,27 +3444,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3479,7 +3479,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3497,28 +3497,28 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.438744</v>
+        <v>-58.487821</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.629929</v>
+        <v>-34.554603</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -3530,27 +3530,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3565,7 +3565,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3573,7 +3573,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3587,14 +3587,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.440748</v>
+        <v>-58.382231</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.63245</v>
+        <v>-34.627676</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3604,7 +3604,7 @@
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
@@ -3616,27 +3616,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3673,14 +3673,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.44037</v>
+        <v>-58.382261</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.632249</v>
+        <v>-34.62737</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3690,7 +3690,7 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-27 19:24:34)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R38"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1810,17 +1810,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Treinta y Tres Orientales 905</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1830,7 +1830,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1867,14 +1867,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.423229</v>
+        <v>-58.418089</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.625103</v>
+        <v>-34.620313</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1884,7 +1884,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>ALM-A</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1896,7 +1896,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1906,7 +1906,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1916,7 +1916,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1953,10 +1953,10 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.418089</v>
+        <v>-58.427201</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.620313</v>
+        <v>-34.617131</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1982,7 +1982,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1992,7 +1992,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -2002,7 +2002,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2039,14 +2039,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.427201</v>
+        <v>-58.414984</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.617131</v>
+        <v>-34.621386</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2056,7 +2056,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2068,27 +2068,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2103,7 +2103,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -2125,24 +2125,24 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.414984</v>
+        <v>-58.507569</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.621386</v>
+        <v>-34.579623</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2154,27 +2154,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2189,11 +2189,11 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2211,14 +2211,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.507569</v>
+        <v>-58.466348</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.579623</v>
+        <v>-34.556028</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2228,7 +2228,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2240,27 +2240,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2275,7 +2275,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2297,14 +2297,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.466348</v>
+        <v>-58.497446</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.556028</v>
+        <v>-34.583455</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2314,7 +2314,7 @@
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2326,27 +2326,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2379,18 +2379,18 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.497446</v>
+        <v>-58.454065</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.583455</v>
+        <v>-34.57105</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2400,7 +2400,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2412,27 +2412,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2465,28 +2465,28 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.454065</v>
+        <v>-58.436255</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.57105</v>
+        <v>-34.567733</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2508,7 +2508,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Benjamin Matienzo 1524</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2518,7 +2518,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>805655369</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2551,14 +2551,14 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.436255</v>
+        <v>-58.43247</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.567733</v>
+        <v>-34.566492</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2572,7 +2572,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>BLO-I</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,17 +2584,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2604,7 +2604,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2637,28 +2637,28 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.43247</v>
+        <v>-58.44191</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.566492</v>
+        <v>-34.564245</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>BLO-I</t>
+          <t>BLO-L</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2705,7 +2705,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2723,28 +2723,28 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.44191</v>
+        <v>-58.438744</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.564245</v>
+        <v>-34.629929</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>BLO-L</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2809,28 +2809,28 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.438744</v>
+        <v>-58.473937</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.629929</v>
+        <v>-34.557355</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2899,24 +2899,24 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.473937</v>
+        <v>-58.434668</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.557355</v>
+        <v>-34.571258</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2928,17 +2928,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2948,7 +2948,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2985,10 +2985,10 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.434668</v>
+        <v>-58.434194</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.571258</v>
+        <v>-34.571754</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -3014,27 +3014,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3067,18 +3067,18 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.434194</v>
+        <v>-58.440748</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.571754</v>
+        <v>-34.63245</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3088,7 +3088,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3100,7 +3100,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3110,7 +3110,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -3120,7 +3120,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3153,14 +3153,14 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.440748</v>
+        <v>-58.44037</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.63245</v>
+        <v>-34.632249</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3186,27 +3186,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3243,24 +3243,24 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.44037</v>
+        <v>-58.511732</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.632249</v>
+        <v>-34.578688</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3272,27 +3272,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3329,24 +3329,24 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.511732</v>
+        <v>-58.404058</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.578688</v>
+        <v>-34.634341</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -3358,7 +3358,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3368,17 +3368,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3393,7 +3393,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3415,24 +3415,24 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.404058</v>
+        <v>-58.487821</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.634341</v>
+        <v>-34.554603</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
@@ -3444,7 +3444,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3454,17 +3454,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3479,7 +3479,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3487,7 +3487,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3497,28 +3497,28 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.487821</v>
+        <v>-58.382231</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.554603</v>
+        <v>-34.627676</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -3530,7 +3530,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3540,7 +3540,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -3550,7 +3550,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3565,7 +3565,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3573,7 +3573,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3583,14 +3583,14 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.382231</v>
+        <v>-58.382261</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.627676</v>
+        <v>-34.62737</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -3604,96 +3604,10 @@
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>-555</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Lima 1649</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>808973201</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I38" t="n">
-        <v>1</v>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M38" t="n">
-        <v>-58.382261</v>
-      </c>
-      <c r="N38" t="n">
-        <v>-34.62737</v>
-      </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P38" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>CON-K</t>
-        </is>
-      </c>
-      <c r="R38" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-29 11:16:23)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2498,27 +2498,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Benjamin Matienzo 1524</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805655369</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2533,7 +2533,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2555,14 +2555,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.43247</v>
+        <v>-58.438744</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.566492</v>
+        <v>-34.629929</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2572,7 +2572,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>BLO-I</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,27 +2584,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2641,14 +2641,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.44191</v>
+        <v>-58.473937</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.564245</v>
+        <v>-34.557355</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>BLO-L</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2705,7 +2705,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2723,18 +2723,18 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.438744</v>
+        <v>-58.434668</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.629929</v>
+        <v>-34.571258</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2744,7 +2744,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2813,24 +2813,24 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.473937</v>
+        <v>-58.434194</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.557355</v>
+        <v>-34.571754</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2895,18 +2895,18 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.434668</v>
+        <v>-58.440748</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.571258</v>
+        <v>-34.63245</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2916,7 +2916,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2928,27 +2928,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2985,14 +2985,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.434194</v>
+        <v>-58.44037</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.571754</v>
+        <v>-34.632249</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -3002,7 +3002,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3014,27 +3014,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3067,28 +3067,28 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.440748</v>
+        <v>-58.511732</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.63245</v>
+        <v>-34.578688</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3100,27 +3100,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3157,14 +3157,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.44037</v>
+        <v>-58.404058</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.632249</v>
+        <v>-34.634341</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -3174,7 +3174,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3186,17 +3186,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -3206,7 +3206,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -3243,14 +3243,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.511732</v>
+        <v>-58.487821</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.578688</v>
+        <v>-34.554603</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3272,7 +3272,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3282,17 +3282,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3307,7 +3307,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -3315,7 +3315,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -3325,14 +3325,14 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.404058</v>
+        <v>-58.382231</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.634341</v>
+        <v>-34.627676</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3346,7 +3346,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -3358,7 +3358,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3368,17 +3368,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3393,7 +3393,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3415,199 +3415,27 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.487821</v>
+        <v>-58.382261</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.554603</v>
+        <v>-34.62737</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>-554</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Lima 1697</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>808973197</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>Columna inclinada</t>
-        </is>
-      </c>
-      <c r="I36" t="n">
-        <v>1</v>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M36" t="n">
-        <v>-58.382231</v>
-      </c>
-      <c r="N36" t="n">
-        <v>-34.627676</v>
-      </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P36" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>CON-M</t>
-        </is>
-      </c>
-      <c r="R36" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>-555</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Lima 1649</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>808973201</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I37" t="n">
-        <v>1</v>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M37" t="n">
-        <v>-58.382261</v>
-      </c>
-      <c r="N37" t="n">
-        <v>-34.62737</v>
-      </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P37" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>CON-K</t>
-        </is>
-      </c>
-      <c r="R37" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-31 15:06:15)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -782,27 +782,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-28</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2/20/2024</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ZABALA /ALT/ 2836</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>780340125</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -817,7 +817,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>ZABALA 2836 - Reemplazar C114</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -839,24 +839,24 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.452298</v>
+        <v>-58.390198</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.572157</v>
+        <v>-34.637568</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>ATH-Q</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -868,27 +868,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -901,11 +901,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
-        </is>
-      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
         <v>0</v>
       </c>
@@ -925,14 +921,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.390198</v>
+        <v>-58.400047</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.637568</v>
+        <v>-34.586358</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -942,7 +938,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -954,7 +950,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -964,17 +960,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -987,7 +983,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Para cambiar columna fte al 3688</t>
+        </is>
+      </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
@@ -1007,24 +1007,24 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.400047</v>
+        <v>-58.499823</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.586358</v>
+        <v>-34.563809</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1036,27 +1036,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1071,7 +1071,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1093,24 +1093,24 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.499823</v>
+        <v>-58.386058</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.563809</v>
+        <v>-34.621209</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1122,27 +1122,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1157,7 +1157,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1179,10 +1179,10 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.386058</v>
+        <v>-58.395465</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.621209</v>
+        <v>-34.622784</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1196,7 +1196,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1208,17 +1208,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1265,14 +1265,14 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.395465</v>
+        <v>-58.394079</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.622784</v>
+        <v>-34.61051</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1282,7 +1282,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1294,17 +1294,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-111</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>7/12/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>CATAMARCA /ALT/ 1127</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1314,7 +1314,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>790298182</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1351,14 +1351,14 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.394079</v>
+        <v>-58.404265</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.61051</v>
+        <v>-34.623154</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1368,7 +1368,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>CEN-K</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1380,27 +1380,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1415,11 +1415,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1437,24 +1437,24 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.404265</v>
+        <v>-58.480871</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.623154</v>
+        <v>-34.616598</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>CEN-K</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1466,27 +1466,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1523,24 +1523,24 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.480871</v>
+        <v>-58.407076</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.616598</v>
+        <v>-34.616016</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1552,27 +1552,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1587,11 +1587,11 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1609,24 +1609,24 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.407076</v>
+        <v>-58.439727</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.616016</v>
+        <v>-34.556261</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1638,27 +1638,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1695,24 +1695,24 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.439727</v>
+        <v>-58.415566</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.556261</v>
+        <v>-34.613244</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1724,17 +1724,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1744,7 +1744,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1781,10 +1781,10 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.415566</v>
+        <v>-58.418089</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.613244</v>
+        <v>-34.620313</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1798,7 +1798,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1810,7 +1810,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1820,7 +1820,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1830,7 +1830,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1867,10 +1867,10 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.418089</v>
+        <v>-58.427201</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.620313</v>
+        <v>-34.617131</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1884,7 +1884,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1896,7 +1896,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1906,7 +1906,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1916,7 +1916,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1953,14 +1953,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.427201</v>
+        <v>-58.414984</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.617131</v>
+        <v>-34.621386</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1970,7 +1970,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1982,27 +1982,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2017,7 +2017,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -2039,24 +2039,24 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.414984</v>
+        <v>-58.507569</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.621386</v>
+        <v>-34.579623</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2068,27 +2068,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2103,11 +2103,11 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2125,14 +2125,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.507569</v>
+        <v>-58.466348</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.579623</v>
+        <v>-34.556028</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2142,7 +2142,7 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2154,27 +2154,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2189,7 +2189,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2211,14 +2211,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.466348</v>
+        <v>-58.497446</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.556028</v>
+        <v>-34.583455</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2228,7 +2228,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2240,27 +2240,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2275,7 +2275,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2293,18 +2293,18 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.497446</v>
+        <v>-58.454065</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.583455</v>
+        <v>-34.57105</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2314,7 +2314,7 @@
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2326,27 +2326,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2379,28 +2379,28 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.454065</v>
+        <v>-58.436255</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.57105</v>
+        <v>-34.567733</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2412,27 +2412,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2465,18 +2465,18 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.436255</v>
+        <v>-58.438744</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.567733</v>
+        <v>-34.629929</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2486,7 +2486,7 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,27 +2498,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2533,7 +2533,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2551,28 +2551,28 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.438744</v>
+        <v>-58.473937</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.629929</v>
+        <v>-34.557355</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,27 +2584,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2641,24 +2641,24 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.473937</v>
+        <v>-58.434668</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.557355</v>
+        <v>-34.571258</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,17 +2670,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2690,7 +2690,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2727,10 +2727,10 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.434668</v>
+        <v>-58.434194</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.571258</v>
+        <v>-34.571754</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2756,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2809,18 +2809,18 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.434194</v>
+        <v>-58.440748</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.571754</v>
+        <v>-34.63245</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2830,7 +2830,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,7 +2842,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2852,7 +2852,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2862,7 +2862,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2895,14 +2895,14 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.440748</v>
+        <v>-58.44037</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.63245</v>
+        <v>-34.632249</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2928,27 +2928,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2985,24 +2985,24 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.44037</v>
+        <v>-58.511732</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.632249</v>
+        <v>-34.578688</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3014,27 +3014,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3071,24 +3071,24 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.511732</v>
+        <v>-58.404058</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.578688</v>
+        <v>-34.634341</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3100,7 +3100,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3110,17 +3110,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3135,7 +3135,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -3157,24 +3157,24 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.404058</v>
+        <v>-58.487821</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.634341</v>
+        <v>-34.554603</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3186,7 +3186,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3196,17 +3196,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -3229,7 +3229,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -3239,28 +3239,28 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.487821</v>
+        <v>-58.382231</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.554603</v>
+        <v>-34.627676</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3272,7 +3272,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3282,7 +3282,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -3292,7 +3292,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3307,7 +3307,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -3315,7 +3315,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -3325,14 +3325,14 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.382231</v>
+        <v>-58.382261</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.627676</v>
+        <v>-34.62737</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3346,96 +3346,10 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>-555</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Lima 1649</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>808973201</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I35" t="n">
-        <v>1</v>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M35" t="n">
-        <v>-58.382261</v>
-      </c>
-      <c r="N35" t="n">
-        <v>-34.62737</v>
-      </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P35" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>CON-K</t>
-        </is>
-      </c>
-      <c r="R35" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-06 10:01:46)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="INCO" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="INCO" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-06 10:38:22)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,11 +563,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -585,10 +585,10 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.390269</v>
+        <v>-58.404058</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.625079</v>
+        <v>-34.634341</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -614,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BAEZ 489</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -649,7 +649,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -671,24 +671,24 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.432978</v>
+        <v>-58.487821</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.57094</v>
+        <v>-34.554603</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -700,27 +700,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -733,13 +733,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Columna inclinada</t>
+        </is>
+      </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -749,18 +753,18 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.39894</v>
+        <v>-58.382231</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.591084</v>
+        <v>-34.627676</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -770,39 +774,39 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>RET-E</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -817,11 +821,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -839,10 +843,10 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.390198</v>
+        <v>-58.382261</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.637568</v>
+        <v>-34.62737</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -868,27 +872,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -901,9 +905,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -921,24 +929,24 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.400047</v>
+        <v>-58.511732</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.586358</v>
+        <v>-34.578688</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -950,27 +958,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -985,11 +993,11 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1003,28 +1011,28 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.499823</v>
+        <v>-58.440748</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.563809</v>
+        <v>-34.63245</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1036,27 +1044,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1071,11 +1079,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1093,14 +1101,14 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.386058</v>
+        <v>-58.44037</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.621209</v>
+        <v>-34.632249</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1110,7 +1118,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1122,27 +1130,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1157,11 +1165,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1179,14 +1187,14 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.395465</v>
+        <v>-58.434194</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.622784</v>
+        <v>-34.571754</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1196,7 +1204,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1208,27 +1216,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1243,11 +1251,11 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1265,14 +1273,14 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.394079</v>
+        <v>-58.434668</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.61051</v>
+        <v>-34.571258</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1282,7 +1290,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1294,27 +1302,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1329,11 +1337,11 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1351,24 +1359,24 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.404265</v>
+        <v>-58.473937</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.623154</v>
+        <v>-34.557355</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>CEN-K</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1380,27 +1388,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1415,7 +1423,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1433,28 +1441,28 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.480871</v>
+        <v>-58.438744</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.616598</v>
+        <v>-34.629929</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1466,27 +1474,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1501,7 +1509,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1523,14 +1531,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.407076</v>
+        <v>-58.436255</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.616016</v>
+        <v>-34.567733</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1540,7 +1548,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1552,17 +1560,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1572,7 +1580,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1587,11 +1595,11 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1605,18 +1613,18 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.439727</v>
+        <v>-58.454065</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.556261</v>
+        <v>-34.57105</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1626,7 +1634,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1638,27 +1646,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1673,11 +1681,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1695,24 +1703,24 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.415566</v>
+        <v>-58.497446</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.613244</v>
+        <v>-34.583455</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1724,27 +1732,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1763,7 +1771,7 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1781,24 +1789,24 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.418089</v>
+        <v>-58.466348</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.620313</v>
+        <v>-34.556028</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1810,27 +1818,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1845,7 +1853,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1867,24 +1875,24 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.427201</v>
+        <v>-58.507569</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.617131</v>
+        <v>-34.579623</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1896,7 +1904,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1906,7 +1914,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1916,7 +1924,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1953,14 +1961,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.414984</v>
+        <v>-58.418089</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.621386</v>
+        <v>-34.620313</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1970,7 +1978,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1982,27 +1990,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2017,7 +2025,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -2039,24 +2047,24 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.507569</v>
+        <v>-58.427201</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.579623</v>
+        <v>-34.617131</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2068,27 +2076,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2107,7 +2115,7 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2125,24 +2133,24 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.466348</v>
+        <v>-58.414984</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.556028</v>
+        <v>-34.621386</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2154,27 +2162,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2189,11 +2197,11 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2211,24 +2219,24 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.497446</v>
+        <v>-58.415566</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.583455</v>
+        <v>-34.613244</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2240,17 +2248,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2260,7 +2268,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2275,11 +2283,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2293,18 +2301,18 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.454065</v>
+        <v>-58.439727</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.57105</v>
+        <v>-34.556261</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2314,7 +2322,7 @@
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2326,27 +2334,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2361,7 +2369,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2383,14 +2391,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.436255</v>
+        <v>-58.407076</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.567733</v>
+        <v>-34.616016</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2400,7 +2408,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2412,27 +2420,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2447,7 +2455,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2465,28 +2473,28 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.438744</v>
+        <v>-58.480871</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.629929</v>
+        <v>-34.616598</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,27 +2506,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-111</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/12/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>CATAMARCA /ALT/ 1127</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>790298182</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2533,11 +2541,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2555,24 +2563,24 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.473937</v>
+        <v>-58.404265</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.557355</v>
+        <v>-34.623154</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CEN-K</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,27 +2592,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2619,11 +2627,11 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2641,14 +2649,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.434668</v>
+        <v>-58.394079</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.571258</v>
+        <v>-34.61051</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2658,7 +2666,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,27 +2678,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2705,11 +2713,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2727,14 +2735,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.434194</v>
+        <v>-58.395465</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.571754</v>
+        <v>-34.622784</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2744,7 +2752,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2764,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2791,11 +2799,11 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2809,18 +2817,18 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.440748</v>
+        <v>-58.386058</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.63245</v>
+        <v>-34.621209</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2830,7 +2838,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,27 +2850,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2875,13 +2883,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H29" t="inlineStr"/>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2899,14 +2903,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.44037</v>
+        <v>-58.400047</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.632249</v>
+        <v>-34.586358</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2916,7 +2920,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2928,17 +2932,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2948,7 +2952,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2963,11 +2967,11 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2985,10 +2989,10 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.511732</v>
+        <v>-58.499823</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.578688</v>
+        <v>-34.563809</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -3002,7 +3006,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3014,17 +3018,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -3034,7 +3038,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3049,11 +3053,11 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3071,10 +3075,10 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.404058</v>
+        <v>-58.390198</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.634341</v>
+        <v>-34.637568</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -3088,7 +3092,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3100,27 +3104,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>BAEZ 489</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3135,7 +3139,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -3157,24 +3161,24 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.487821</v>
+        <v>-58.432978</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.554603</v>
+        <v>-34.57094</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3186,27 +3190,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3219,17 +3223,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>Columna inclinada</t>
-        </is>
-      </c>
+      <c r="H33" t="inlineStr"/>
       <c r="I33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -3239,18 +3239,18 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.382231</v>
+        <v>-58.39894</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.627676</v>
+        <v>-34.591084</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -3260,29 +3260,29 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>RET-E</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Lima 1649</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -3292,7 +3292,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3307,11 +3307,11 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3329,10 +3329,10 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.382261</v>
+        <v>-58.390269</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.62737</v>
+        <v>-34.625079</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3346,7 +3346,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-07 08:50:24)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,11 +563,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -585,10 +585,10 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.404058</v>
+        <v>-58.390269</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.634341</v>
+        <v>-34.625079</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -614,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>BAEZ 489</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -649,7 +649,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -671,24 +671,24 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.487821</v>
+        <v>-58.432978</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.554603</v>
+        <v>-34.57094</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -700,27 +700,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -733,17 +733,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Columna inclinada</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -753,18 +749,18 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.382231</v>
+        <v>-58.39894</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.627676</v>
+        <v>-34.591084</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -774,39 +770,39 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>RET-E</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Lima 1649</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -821,11 +817,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -843,10 +839,10 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.382261</v>
+        <v>-58.390198</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.62737</v>
+        <v>-34.637568</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -872,27 +868,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -905,13 +901,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -929,24 +921,24 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.511732</v>
+        <v>-58.400047</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.578688</v>
+        <v>-34.586358</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -958,27 +950,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -993,11 +985,11 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1011,28 +1003,28 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.440748</v>
+        <v>-58.499823</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.63245</v>
+        <v>-34.563809</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1044,27 +1036,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1079,11 +1071,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1101,14 +1093,14 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.44037</v>
+        <v>-58.386058</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.632249</v>
+        <v>-34.621209</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1118,7 +1110,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1130,27 +1122,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1165,11 +1157,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1187,14 +1179,14 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.434194</v>
+        <v>-58.395465</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.571754</v>
+        <v>-34.622784</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1204,7 +1196,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1216,27 +1208,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1251,11 +1243,11 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1273,14 +1265,14 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.434668</v>
+        <v>-58.394079</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.571258</v>
+        <v>-34.61051</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1290,7 +1282,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1302,27 +1294,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-111</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/12/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>CATAMARCA /ALT/ 1127</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>790298182</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1337,11 +1329,11 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1359,24 +1351,24 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.473937</v>
+        <v>-58.404265</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.557355</v>
+        <v>-34.623154</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CEN-K</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1388,27 +1380,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1423,7 +1415,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1441,28 +1433,28 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.438744</v>
+        <v>-58.480871</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.629929</v>
+        <v>-34.616598</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1474,27 +1466,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1509,7 +1501,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1531,14 +1523,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.436255</v>
+        <v>-58.407076</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.567733</v>
+        <v>-34.616016</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1548,7 +1540,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1560,17 +1552,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1580,7 +1572,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1595,11 +1587,11 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1613,18 +1605,18 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.454065</v>
+        <v>-58.439727</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.57105</v>
+        <v>-34.556261</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1634,7 +1626,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1646,27 +1638,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1681,11 +1673,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1703,24 +1695,24 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.497446</v>
+        <v>-58.415566</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.583455</v>
+        <v>-34.613244</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1732,27 +1724,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1771,7 +1763,7 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1789,24 +1781,24 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.466348</v>
+        <v>-58.418089</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.556028</v>
+        <v>-34.620313</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1818,27 +1810,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1853,7 +1845,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1875,24 +1867,24 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.507569</v>
+        <v>-58.427201</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.579623</v>
+        <v>-34.617131</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1904,7 +1896,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1914,7 +1906,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1924,7 +1916,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1961,14 +1953,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.418089</v>
+        <v>-58.414984</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.620313</v>
+        <v>-34.621386</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1978,7 +1970,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1990,27 +1982,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2025,7 +2017,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -2047,24 +2039,24 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.427201</v>
+        <v>-58.507569</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.617131</v>
+        <v>-34.579623</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2076,27 +2068,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2115,7 +2107,7 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2133,24 +2125,24 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.414984</v>
+        <v>-58.466348</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.621386</v>
+        <v>-34.556028</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2162,27 +2154,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2197,11 +2189,11 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2219,24 +2211,24 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.415566</v>
+        <v>-58.497446</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.613244</v>
+        <v>-34.583455</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2248,17 +2240,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2268,7 +2260,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2283,11 +2275,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2301,18 +2293,18 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.439727</v>
+        <v>-58.454065</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.556261</v>
+        <v>-34.57105</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2322,7 +2314,7 @@
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2334,27 +2326,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2369,7 +2361,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2391,14 +2383,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.407076</v>
+        <v>-58.436255</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.616016</v>
+        <v>-34.567733</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2408,7 +2400,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2420,27 +2412,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2455,7 +2447,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2473,28 +2465,28 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.480871</v>
+        <v>-58.438744</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.616598</v>
+        <v>-34.629929</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2506,27 +2498,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2541,11 +2533,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2563,24 +2555,24 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.404265</v>
+        <v>-58.473937</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.623154</v>
+        <v>-34.557355</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>CEN-K</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2592,27 +2584,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2627,11 +2619,11 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2649,14 +2641,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.394079</v>
+        <v>-58.434668</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.61051</v>
+        <v>-34.571258</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2666,7 +2658,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2678,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2713,11 +2705,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2735,14 +2727,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.395465</v>
+        <v>-58.434194</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.622784</v>
+        <v>-34.571754</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2752,7 +2744,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2764,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2799,11 +2791,11 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2817,18 +2809,18 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.386058</v>
+        <v>-58.440748</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.621209</v>
+        <v>-34.63245</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2838,7 +2830,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2850,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2883,9 +2875,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2903,14 +2899,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.400047</v>
+        <v>-58.44037</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.586358</v>
+        <v>-34.632249</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2920,7 +2916,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2932,17 +2928,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2952,7 +2948,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2967,11 +2963,11 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2989,10 +2985,10 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.499823</v>
+        <v>-58.511732</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.563809</v>
+        <v>-34.578688</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -3006,7 +3002,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3018,17 +3014,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -3038,7 +3034,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3053,11 +3049,11 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3075,10 +3071,10 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.390198</v>
+        <v>-58.404058</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.637568</v>
+        <v>-34.634341</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -3092,7 +3088,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3104,27 +3100,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>BAEZ 489</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3139,7 +3135,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -3161,24 +3157,24 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.432978</v>
+        <v>-58.487821</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.57094</v>
+        <v>-34.554603</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3190,27 +3186,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3223,13 +3219,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr"/>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Columna inclinada</t>
+        </is>
+      </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -3239,18 +3239,18 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.39894</v>
+        <v>-58.382231</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.591084</v>
+        <v>-34.627676</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -3260,29 +3260,29 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>RET-E</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -3292,7 +3292,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3307,11 +3307,11 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3329,10 +3329,10 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.390269</v>
+        <v>-58.382261</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.625079</v>
+        <v>-34.62737</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3346,7 +3346,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-11 07:55:41)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="INCO" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="INCO" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,7 +563,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -585,14 +585,14 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.390269</v>
+        <v>-58.394079</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.625079</v>
+        <v>-34.61051</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -614,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BAEZ 489</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -649,7 +649,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -667,28 +667,28 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.432978</v>
+        <v>-58.454065</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.57094</v>
+        <v>-34.57105</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -700,27 +700,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -733,7 +733,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+        </is>
+      </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
@@ -753,14 +757,14 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.39894</v>
+        <v>-58.390198</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.591084</v>
+        <v>-34.637568</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -770,39 +774,39 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>RET-E</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -817,11 +821,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -835,18 +839,18 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.390198</v>
+        <v>-58.440748</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.637568</v>
+        <v>-34.63245</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -856,7 +860,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -868,27 +872,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -901,9 +905,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -921,14 +929,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.400047</v>
+        <v>-58.44037</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.586358</v>
+        <v>-34.632249</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -938,7 +946,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -950,17 +958,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -970,7 +978,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -985,11 +993,11 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1007,14 +1015,14 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.499823</v>
+        <v>-58.473937</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.563809</v>
+        <v>-34.557355</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1024,7 +1032,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1036,27 +1044,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1071,7 +1079,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1093,10 +1101,10 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.386058</v>
+        <v>-58.395465</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.621209</v>
+        <v>-34.622784</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1110,7 +1118,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1122,27 +1130,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1157,7 +1165,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1179,14 +1187,14 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.395465</v>
+        <v>-58.427201</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.622784</v>
+        <v>-34.617131</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1196,7 +1204,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1208,27 +1216,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1243,11 +1251,11 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1265,24 +1273,24 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.394079</v>
+        <v>-58.466348</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.61051</v>
+        <v>-34.556028</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1294,27 +1302,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1329,7 +1337,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1351,14 +1359,14 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.404265</v>
+        <v>-58.414984</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.623154</v>
+        <v>-34.621386</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1368,7 +1376,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>CEN-K</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1380,27 +1388,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1415,7 +1423,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1437,24 +1445,24 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.480871</v>
+        <v>-58.434668</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.616598</v>
+        <v>-34.571258</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1466,27 +1474,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1501,7 +1509,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1523,14 +1531,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.407076</v>
+        <v>-58.434194</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.616016</v>
+        <v>-34.571754</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1540,7 +1548,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1552,27 +1560,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1587,15 +1595,15 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1605,28 +1613,28 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.439727</v>
+        <v>-58.382231</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.556261</v>
+        <v>-34.627676</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1638,27 +1646,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1677,7 +1685,7 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1695,14 +1703,14 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.415566</v>
+        <v>-58.382261</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.613244</v>
+        <v>-34.62737</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1712,7 +1720,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1724,27 +1732,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1759,7 +1767,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1781,24 +1789,24 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.418089</v>
+        <v>-58.439727</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.620313</v>
+        <v>-34.556261</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1810,27 +1818,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1845,7 +1853,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1867,14 +1875,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.427201</v>
+        <v>-58.386058</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.617131</v>
+        <v>-34.621209</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1884,7 +1892,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1896,27 +1904,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1931,11 +1939,11 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1953,24 +1961,24 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.414984</v>
+        <v>-58.487821</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.621386</v>
+        <v>-34.554603</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1982,27 +1990,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2017,11 +2025,11 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2039,10 +2047,10 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.507569</v>
+        <v>-58.480871</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.579623</v>
+        <v>-34.616598</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -2056,7 +2064,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2068,27 +2076,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2101,13 +2109,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2125,56 +2129,56 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.466348</v>
+        <v>-58.39894</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.556028</v>
+        <v>-34.591084</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>RET-E</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2207,28 +2211,28 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.497446</v>
+        <v>-58.438744</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.583455</v>
+        <v>-34.629929</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2240,27 +2244,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2275,7 +2279,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2293,28 +2297,28 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.454065</v>
+        <v>-58.407076</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.57105</v>
+        <v>-34.616016</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2326,27 +2330,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2361,11 +2365,11 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2383,14 +2387,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.436255</v>
+        <v>-58.390269</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.567733</v>
+        <v>-34.625079</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2400,7 +2404,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2412,27 +2416,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2447,11 +2451,11 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2465,18 +2469,18 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.438744</v>
+        <v>-58.418089</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.629929</v>
+        <v>-34.620313</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2486,7 +2490,7 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,17 +2502,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2518,7 +2522,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2533,11 +2537,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2555,14 +2559,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.473937</v>
+        <v>-58.507569</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.557355</v>
+        <v>-34.579623</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2572,7 +2576,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,27 +2588,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2641,14 +2645,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.434668</v>
+        <v>-58.404058</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.571258</v>
+        <v>-34.634341</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2658,7 +2662,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,27 +2674,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-111</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/12/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>CATAMARCA /ALT/ 1127</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>790298182</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2705,11 +2709,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2727,14 +2731,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.434194</v>
+        <v>-58.404265</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.571754</v>
+        <v>-34.623154</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2744,7 +2748,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-K</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2760,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>BAEZ 489</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2791,7 +2795,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2809,18 +2813,18 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.440748</v>
+        <v>-58.432978</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.63245</v>
+        <v>-34.57094</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2830,7 +2834,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,27 +2846,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2881,7 +2885,7 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2899,14 +2903,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.44037</v>
+        <v>-58.415566</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.632249</v>
+        <v>-34.613244</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2916,7 +2920,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2928,17 +2932,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2948,7 +2952,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2963,7 +2967,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2985,10 +2989,10 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.511732</v>
+        <v>-58.497446</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.578688</v>
+        <v>-34.583455</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -3002,7 +3006,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3014,27 +3018,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3071,14 +3075,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.404058</v>
+        <v>-58.436255</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.634341</v>
+        <v>-34.567733</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3088,7 +3092,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3100,17 +3104,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -3120,7 +3124,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3135,11 +3139,11 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3157,14 +3161,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.487821</v>
+        <v>-58.499823</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.554603</v>
+        <v>-34.563809</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -3174,7 +3178,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3186,27 +3190,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3221,7 +3225,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -3229,7 +3233,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -3239,28 +3243,28 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.382231</v>
+        <v>-58.511732</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.627676</v>
+        <v>-34.578688</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3272,27 +3276,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Lima 1649</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3305,13 +3309,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H34" t="inlineStr"/>
       <c r="I34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3329,14 +3329,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.382261</v>
+        <v>-58.400047</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.62737</v>
+        <v>-34.586358</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3346,7 +3346,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-12 08:40:54)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,7 +563,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -585,14 +585,14 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.394079</v>
+        <v>-58.390269</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.61051</v>
+        <v>-34.625079</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -614,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>BAEZ 489</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>780035752</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -649,7 +649,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -667,28 +667,28 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.454065</v>
+        <v>-58.432978</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.57105</v>
+        <v>-34.57094</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -700,27 +700,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -733,11 +733,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
         <v>0</v>
       </c>
@@ -757,14 +753,14 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.390198</v>
+        <v>-58.39894</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.637568</v>
+        <v>-34.591084</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -774,39 +770,39 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>RET-E</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -821,11 +817,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -839,18 +835,18 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.440748</v>
+        <v>-58.390198</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.63245</v>
+        <v>-34.637568</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -860,7 +856,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -872,27 +868,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -905,13 +901,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -929,14 +921,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.44037</v>
+        <v>-58.400047</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.632249</v>
+        <v>-34.586358</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -946,7 +938,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -958,17 +950,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -978,7 +970,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -993,11 +985,11 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1015,14 +1007,14 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.473937</v>
+        <v>-58.499823</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.557355</v>
+        <v>-34.563809</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1032,7 +1024,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1044,27 +1036,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1079,7 +1071,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1101,10 +1093,10 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.395465</v>
+        <v>-58.386058</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.622784</v>
+        <v>-34.621209</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1118,7 +1110,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1130,27 +1122,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1165,7 +1157,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1187,14 +1179,14 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.427201</v>
+        <v>-58.395465</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.617131</v>
+        <v>-34.622784</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1204,7 +1196,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1216,27 +1208,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1251,11 +1243,11 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1273,24 +1265,24 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.466348</v>
+        <v>-58.394079</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.556028</v>
+        <v>-34.61051</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1302,27 +1294,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>-111</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>7/12/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>CATAMARCA /ALT/ 1127</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>790298182</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1337,7 +1329,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1359,14 +1351,14 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.414984</v>
+        <v>-58.404265</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.621386</v>
+        <v>-34.623154</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1376,7 +1368,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>CEN-K</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1388,27 +1380,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1423,7 +1415,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1445,24 +1437,24 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.434668</v>
+        <v>-58.480871</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.571258</v>
+        <v>-34.616598</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1474,27 +1466,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1509,7 +1501,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1531,14 +1523,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.434194</v>
+        <v>-58.407076</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.571754</v>
+        <v>-34.616016</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1548,7 +1540,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1560,27 +1552,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1595,15 +1587,15 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1613,28 +1605,28 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.382231</v>
+        <v>-58.439727</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.627676</v>
+        <v>-34.556261</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1646,27 +1638,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Lima 1649</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1685,7 +1677,7 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1703,14 +1695,14 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.382261</v>
+        <v>-58.415566</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.62737</v>
+        <v>-34.613244</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1720,7 +1712,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1732,27 +1724,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1767,7 +1759,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1789,24 +1781,24 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.439727</v>
+        <v>-58.418089</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.556261</v>
+        <v>-34.620313</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1818,27 +1810,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1853,7 +1845,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1875,14 +1867,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.386058</v>
+        <v>-58.427201</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.621209</v>
+        <v>-34.617131</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1892,7 +1884,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1904,27 +1896,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1939,11 +1931,11 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1961,24 +1953,24 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.487821</v>
+        <v>-58.414984</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.554603</v>
+        <v>-34.621386</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1990,27 +1982,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2025,11 +2017,11 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2047,10 +2039,10 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.480871</v>
+        <v>-58.507569</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.616598</v>
+        <v>-34.579623</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -2064,7 +2056,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2076,27 +2068,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2109,9 +2101,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2129,56 +2125,56 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.39894</v>
+        <v>-58.466348</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.591084</v>
+        <v>-34.556028</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>RET-E</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2211,28 +2207,28 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.438744</v>
+        <v>-58.497446</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.629929</v>
+        <v>-34.583455</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2244,27 +2240,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2279,7 +2275,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2297,28 +2293,28 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.407076</v>
+        <v>-58.454065</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.616016</v>
+        <v>-34.57105</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2330,27 +2326,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2365,11 +2361,11 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2387,14 +2383,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.390269</v>
+        <v>-58.436255</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.625079</v>
+        <v>-34.567733</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2404,7 +2400,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2416,27 +2412,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2451,11 +2447,11 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2469,18 +2465,18 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.418089</v>
+        <v>-58.438744</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.620313</v>
+        <v>-34.629929</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2490,7 +2486,7 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2502,17 +2498,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2522,7 +2518,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2537,11 +2533,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2559,14 +2555,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.507569</v>
+        <v>-58.473937</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.579623</v>
+        <v>-34.557355</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2576,7 +2572,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2588,27 +2584,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2645,14 +2641,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.404058</v>
+        <v>-58.434668</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.634341</v>
+        <v>-34.571258</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2662,7 +2658,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2674,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2709,11 +2705,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2731,14 +2727,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.404265</v>
+        <v>-58.434194</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.623154</v>
+        <v>-34.571754</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2748,7 +2744,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>CEN-K</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2760,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>BAEZ 489</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2795,7 +2791,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2813,18 +2809,18 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.432978</v>
+        <v>-58.440748</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.57094</v>
+        <v>-34.63245</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2834,7 +2830,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2846,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2885,7 +2881,7 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2903,14 +2899,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.415566</v>
+        <v>-58.44037</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.613244</v>
+        <v>-34.632249</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2920,7 +2916,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2932,17 +2928,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2952,7 +2948,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2967,7 +2963,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2989,10 +2985,10 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.497446</v>
+        <v>-58.511732</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.583455</v>
+        <v>-34.578688</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -3006,7 +3002,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3018,27 +3014,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3075,14 +3071,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.436255</v>
+        <v>-58.404058</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.567733</v>
+        <v>-34.634341</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3092,7 +3088,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3104,17 +3100,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -3124,7 +3120,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3139,11 +3135,11 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3161,14 +3157,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.499823</v>
+        <v>-58.487821</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.563809</v>
+        <v>-34.554603</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -3178,7 +3174,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3190,27 +3186,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3225,7 +3221,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -3233,7 +3229,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -3243,28 +3239,28 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.511732</v>
+        <v>-58.382231</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.578688</v>
+        <v>-34.627676</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3276,27 +3272,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3309,9 +3305,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr"/>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3329,14 +3329,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.400047</v>
+        <v>-58.382261</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.586358</v>
+        <v>-34.62737</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3346,7 +3346,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-13 19:31:09)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1294,27 +1294,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1329,11 +1329,11 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1351,24 +1351,24 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.404265</v>
+        <v>-58.480871</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.623154</v>
+        <v>-34.616598</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>CEN-K</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1380,27 +1380,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1415,7 +1415,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1437,24 +1437,24 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.480871</v>
+        <v>-58.407076</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.616598</v>
+        <v>-34.616016</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1466,27 +1466,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1501,11 +1501,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1523,24 +1523,24 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.407076</v>
+        <v>-58.439727</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.616016</v>
+        <v>-34.556261</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1552,27 +1552,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1587,7 +1587,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1609,24 +1609,24 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.439727</v>
+        <v>-58.415566</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.556261</v>
+        <v>-34.613244</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1638,17 +1638,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1658,7 +1658,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1695,10 +1695,10 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.415566</v>
+        <v>-58.418089</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.613244</v>
+        <v>-34.620313</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1724,7 +1724,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1734,7 +1734,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1744,7 +1744,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1781,10 +1781,10 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.418089</v>
+        <v>-58.427201</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.620313</v>
+        <v>-34.617131</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1798,7 +1798,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1810,7 +1810,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1820,7 +1820,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1830,7 +1830,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1867,14 +1867,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.427201</v>
+        <v>-58.414984</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.617131</v>
+        <v>-34.621386</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1884,7 +1884,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1896,27 +1896,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1931,7 +1931,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1953,24 +1953,24 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.414984</v>
+        <v>-58.507569</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.621386</v>
+        <v>-34.579623</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1982,27 +1982,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2017,11 +2017,11 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2039,14 +2039,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.507569</v>
+        <v>-58.466348</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.579623</v>
+        <v>-34.556028</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2056,7 +2056,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2068,27 +2068,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2103,7 +2103,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -2125,14 +2125,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.466348</v>
+        <v>-58.497446</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.556028</v>
+        <v>-34.583455</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2142,7 +2142,7 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2154,27 +2154,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2189,7 +2189,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2207,18 +2207,18 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.497446</v>
+        <v>-58.454065</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.583455</v>
+        <v>-34.57105</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2228,7 +2228,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2240,27 +2240,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2293,28 +2293,28 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.454065</v>
+        <v>-58.436255</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.57105</v>
+        <v>-34.567733</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2326,27 +2326,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2379,18 +2379,18 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.436255</v>
+        <v>-58.438744</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.567733</v>
+        <v>-34.629929</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2400,7 +2400,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2412,27 +2412,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2465,28 +2465,28 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.438744</v>
+        <v>-58.473937</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.629929</v>
+        <v>-34.557355</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,27 +2498,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2555,24 +2555,24 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.473937</v>
+        <v>-58.434668</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.557355</v>
+        <v>-34.571258</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,17 +2584,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2604,7 +2604,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2641,10 +2641,10 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.434668</v>
+        <v>-58.434194</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.571258</v>
+        <v>-34.571754</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2670,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2723,18 +2723,18 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.434194</v>
+        <v>-58.440748</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.571754</v>
+        <v>-34.63245</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2744,7 +2744,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,7 +2756,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2766,7 +2766,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2776,7 +2776,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2809,14 +2809,14 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.440748</v>
+        <v>-58.44037</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.63245</v>
+        <v>-34.632249</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2842,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2899,24 +2899,24 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.44037</v>
+        <v>-58.511732</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.632249</v>
+        <v>-34.578688</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2928,27 +2928,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2985,24 +2985,24 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.511732</v>
+        <v>-58.404058</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.578688</v>
+        <v>-34.634341</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3014,7 +3014,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3024,17 +3024,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -3071,24 +3071,24 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.404058</v>
+        <v>-58.487821</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.634341</v>
+        <v>-34.554603</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3100,7 +3100,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3110,17 +3110,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3135,7 +3135,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -3143,7 +3143,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -3153,28 +3153,28 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.487821</v>
+        <v>-58.382231</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.554603</v>
+        <v>-34.627676</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3186,7 +3186,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3196,7 +3196,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -3206,7 +3206,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -3229,7 +3229,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -3239,14 +3239,14 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.382231</v>
+        <v>-58.382261</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.627676</v>
+        <v>-34.62737</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -3260,96 +3260,10 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>-555</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Lima 1649</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>808973201</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I34" t="n">
-        <v>1</v>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M34" t="n">
-        <v>-58.382261</v>
-      </c>
-      <c r="N34" t="n">
-        <v>-34.62737</v>
-      </c>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P34" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>CON-K</t>
-        </is>
-      </c>
-      <c r="R34" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-18 10:04:48)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,11 +563,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -585,10 +585,10 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.390269</v>
+        <v>-58.404058</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.625079</v>
+        <v>-34.634341</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -614,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BAEZ 489</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>780035752</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -649,7 +649,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -671,24 +671,24 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.432978</v>
+        <v>-58.487821</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.57094</v>
+        <v>-34.554603</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -700,27 +700,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -733,13 +733,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Columna inclinada</t>
+        </is>
+      </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -749,18 +753,18 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.39894</v>
+        <v>-58.382231</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.591084</v>
+        <v>-34.627676</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -770,39 +774,39 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>RET-E</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -817,11 +821,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -839,10 +843,10 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.390198</v>
+        <v>-58.382261</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.637568</v>
+        <v>-34.62737</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -868,27 +872,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -901,9 +905,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -921,24 +929,24 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.400047</v>
+        <v>-58.511732</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.586358</v>
+        <v>-34.578688</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -950,27 +958,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -985,11 +993,11 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1003,28 +1011,28 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.499823</v>
+        <v>-58.440748</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.563809</v>
+        <v>-34.63245</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1036,27 +1044,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1071,11 +1079,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1093,14 +1101,14 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.386058</v>
+        <v>-58.44037</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.621209</v>
+        <v>-34.632249</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1110,7 +1118,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1122,27 +1130,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1157,11 +1165,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1179,14 +1187,14 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.395465</v>
+        <v>-58.434194</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.622784</v>
+        <v>-34.571754</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1196,7 +1204,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1208,27 +1216,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1243,11 +1251,11 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1265,14 +1273,14 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.394079</v>
+        <v>-58.434668</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.61051</v>
+        <v>-34.571258</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1282,7 +1290,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1294,27 +1302,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1329,7 +1337,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1351,14 +1359,14 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.480871</v>
+        <v>-58.473937</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.616598</v>
+        <v>-34.557355</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1368,7 +1376,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1380,27 +1388,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1415,7 +1423,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1433,18 +1441,18 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.407076</v>
+        <v>-58.438744</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.616016</v>
+        <v>-34.629929</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1454,7 +1462,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1466,27 +1474,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1501,11 +1509,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1523,24 +1531,24 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.439727</v>
+        <v>-58.436255</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.556261</v>
+        <v>-34.567733</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1552,27 +1560,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1591,7 +1599,7 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1605,28 +1613,28 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.415566</v>
+        <v>-58.454065</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.613244</v>
+        <v>-34.57105</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1638,27 +1646,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1673,11 +1681,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1695,24 +1703,24 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.418089</v>
+        <v>-58.497446</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.620313</v>
+        <v>-34.583455</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1724,27 +1732,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1763,7 +1771,7 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1781,24 +1789,24 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.427201</v>
+        <v>-58.466348</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.617131</v>
+        <v>-34.556028</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1810,27 +1818,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1845,7 +1853,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1867,24 +1875,24 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.414984</v>
+        <v>-58.507569</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.621386</v>
+        <v>-34.579623</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1896,27 +1904,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1931,7 +1939,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1953,24 +1961,24 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.507569</v>
+        <v>-58.418089</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.579623</v>
+        <v>-34.620313</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1982,27 +1990,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2021,7 +2029,7 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2039,24 +2047,24 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.466348</v>
+        <v>-58.427201</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.556028</v>
+        <v>-34.617131</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2068,27 +2076,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2103,11 +2111,11 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2125,24 +2133,24 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.497446</v>
+        <v>-58.414984</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.583455</v>
+        <v>-34.621386</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2154,27 +2162,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2193,7 +2201,7 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2207,28 +2215,28 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.454065</v>
+        <v>-58.415566</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.57105</v>
+        <v>-34.613244</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2240,27 +2248,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2275,11 +2283,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2297,24 +2305,24 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.436255</v>
+        <v>-58.439727</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.567733</v>
+        <v>-34.556261</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2326,27 +2334,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2361,7 +2369,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2379,18 +2387,18 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.438744</v>
+        <v>-58.407076</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.629929</v>
+        <v>-34.616016</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2400,7 +2408,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2412,27 +2420,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2447,7 +2455,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2469,14 +2477,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.473937</v>
+        <v>-58.480871</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.557355</v>
+        <v>-34.616598</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2486,7 +2494,7 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,27 +2506,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2533,11 +2541,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2555,14 +2563,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.434668</v>
+        <v>-58.394079</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.571258</v>
+        <v>-34.61051</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2572,7 +2580,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,27 +2592,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2619,11 +2627,11 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2641,14 +2649,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.434194</v>
+        <v>-58.395465</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.571754</v>
+        <v>-34.622784</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2658,7 +2666,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,27 +2678,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2705,11 +2713,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2723,18 +2731,18 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.440748</v>
+        <v>-58.386058</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.63245</v>
+        <v>-34.621209</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2744,7 +2752,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2764,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2789,13 +2797,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H28" t="inlineStr"/>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2813,14 +2817,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.44037</v>
+        <v>-58.400047</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.632249</v>
+        <v>-34.586358</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2830,7 +2834,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,17 +2846,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2862,7 +2866,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2877,11 +2881,11 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2899,10 +2903,10 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.511732</v>
+        <v>-58.499823</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.578688</v>
+        <v>-34.563809</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2916,7 +2920,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2928,17 +2932,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2948,7 +2952,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2963,11 +2967,11 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2985,10 +2989,10 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.404058</v>
+        <v>-58.390198</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.634341</v>
+        <v>-34.637568</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -3002,7 +3006,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3014,27 +3018,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3047,13 +3051,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
-        </is>
-      </c>
+      <c r="H31" t="inlineStr"/>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3071,46 +3071,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.487821</v>
+        <v>-58.39894</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.554603</v>
+        <v>-34.591084</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>RET-E</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -3120,7 +3120,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3135,15 +3135,15 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -3153,14 +3153,14 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.382231</v>
+        <v>-58.390269</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.627676</v>
+        <v>-34.625079</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3178,92 +3178,6 @@
         </is>
       </c>
       <c r="R32" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>-555</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Lima 1649</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>808973201</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I33" t="n">
-        <v>1</v>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M33" t="n">
-        <v>-58.382261</v>
-      </c>
-      <c r="N33" t="n">
-        <v>-34.62737</v>
-      </c>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P33" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q33" t="inlineStr">
-        <is>
-          <t>CON-K</t>
-        </is>
-      </c>
-      <c r="R33" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-21 15:59:29)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,11 +563,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -585,10 +585,10 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.404058</v>
+        <v>-58.390269</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.634341</v>
+        <v>-34.625079</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -614,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -647,13 +647,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -671,56 +667,56 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.487821</v>
+        <v>-58.39894</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.554603</v>
+        <v>-34.591084</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>RET-E</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -735,15 +731,15 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -753,14 +749,14 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.382231</v>
+        <v>-58.390198</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.627676</v>
+        <v>-34.637568</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -774,7 +770,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -786,27 +782,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Lima 1649</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -819,13 +815,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -843,14 +835,14 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.382261</v>
+        <v>-58.400047</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.62737</v>
+        <v>-34.586358</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -860,7 +852,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -872,17 +864,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -892,7 +884,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -907,11 +899,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -929,10 +921,10 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.511732</v>
+        <v>-58.499823</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.578688</v>
+        <v>-34.563809</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -946,7 +938,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -958,27 +950,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -993,11 +985,11 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1011,18 +1003,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.440748</v>
+        <v>-58.386058</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.63245</v>
+        <v>-34.621209</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1032,7 +1024,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1044,27 +1036,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1079,11 +1071,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1101,14 +1093,14 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.44037</v>
+        <v>-58.395465</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.632249</v>
+        <v>-34.622784</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1118,7 +1110,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1130,27 +1122,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1165,11 +1157,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1187,14 +1179,14 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.434194</v>
+        <v>-58.394079</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.571754</v>
+        <v>-34.61051</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1204,7 +1196,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1216,27 +1208,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1251,7 +1243,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1273,24 +1265,24 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.434668</v>
+        <v>-58.480871</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.571258</v>
+        <v>-34.616598</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1302,27 +1294,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1337,7 +1329,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1359,24 +1351,24 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.473937</v>
+        <v>-58.407076</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.557355</v>
+        <v>-34.616016</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1388,27 +1380,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1423,11 +1415,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1441,28 +1433,28 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.438744</v>
+        <v>-58.439727</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.629929</v>
+        <v>-34.556261</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1474,27 +1466,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1513,7 +1505,7 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1531,14 +1523,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.436255</v>
+        <v>-58.415566</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.567733</v>
+        <v>-34.613244</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1548,7 +1540,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1560,27 +1552,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1599,7 +1591,7 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1613,28 +1605,28 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.454065</v>
+        <v>-58.418089</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.57105</v>
+        <v>-34.620313</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1646,27 +1638,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1681,11 +1673,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1703,24 +1695,24 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.497446</v>
+        <v>-58.427201</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.583455</v>
+        <v>-34.617131</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1732,27 +1724,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1771,7 +1763,7 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1789,24 +1781,24 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.466348</v>
+        <v>-58.414984</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.556028</v>
+        <v>-34.621386</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1904,27 +1896,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1943,7 +1935,7 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1961,24 +1953,24 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.418089</v>
+        <v>-58.466348</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.620313</v>
+        <v>-34.556028</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1990,27 +1982,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2025,11 +2017,11 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2047,24 +2039,24 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.427201</v>
+        <v>-58.497446</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.617131</v>
+        <v>-34.583455</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2076,27 +2068,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2115,7 +2107,7 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2129,28 +2121,28 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.414984</v>
+        <v>-58.454065</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.621386</v>
+        <v>-34.57105</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2162,27 +2154,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2201,7 +2193,7 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2219,14 +2211,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.415566</v>
+        <v>-58.436255</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.613244</v>
+        <v>-34.567733</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2236,7 +2228,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2248,27 +2240,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2283,11 +2275,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2301,28 +2293,28 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.439727</v>
+        <v>-58.438744</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.556261</v>
+        <v>-34.629929</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2334,27 +2326,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2369,7 +2361,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2391,24 +2383,24 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.407076</v>
+        <v>-58.473937</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.616016</v>
+        <v>-34.557355</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2420,27 +2412,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2455,7 +2447,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2477,24 +2469,24 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.480871</v>
+        <v>-58.434668</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.616598</v>
+        <v>-34.571258</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2506,27 +2498,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2541,11 +2533,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2563,14 +2555,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.394079</v>
+        <v>-58.434194</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.61051</v>
+        <v>-34.571754</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2580,7 +2572,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2592,27 +2584,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2627,11 +2619,11 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2645,18 +2637,18 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.395465</v>
+        <v>-58.440748</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.622784</v>
+        <v>-34.63245</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2666,7 +2658,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2678,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2713,11 +2705,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2735,14 +2727,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.386058</v>
+        <v>-58.44037</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.621209</v>
+        <v>-34.632249</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2752,7 +2744,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2764,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2797,9 +2789,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr"/>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2817,24 +2813,24 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.400047</v>
+        <v>-58.511732</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.586358</v>
+        <v>-34.578688</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2846,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2881,11 +2877,11 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2903,24 +2899,24 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.499823</v>
+        <v>-58.404058</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.563809</v>
+        <v>-34.634341</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2932,27 +2928,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2967,11 +2963,11 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2989,24 +2985,24 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.390198</v>
+        <v>-58.487821</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.637568</v>
+        <v>-34.554603</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3018,27 +3014,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3051,13 +3047,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr"/>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Columna inclinada</t>
+        </is>
+      </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -3067,18 +3067,18 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.39894</v>
+        <v>-58.382231</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.591084</v>
+        <v>-34.627676</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3088,29 +3088,29 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>RET-E</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -3120,7 +3120,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3135,11 +3135,11 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3157,10 +3157,10 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.390269</v>
+        <v>-58.382261</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.625079</v>
+        <v>-34.62737</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3174,7 +3174,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-12-16 09:37:16)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,11 +563,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -585,10 +585,10 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.390269</v>
+        <v>-58.404058</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.625079</v>
+        <v>-34.634341</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -614,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -647,9 +647,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+        </is>
+      </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -667,56 +671,56 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.39894</v>
+        <v>-58.487821</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.591084</v>
+        <v>-34.554603</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>RET-E</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -731,15 +735,15 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -749,14 +753,14 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.390198</v>
+        <v>-58.382231</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.637568</v>
+        <v>-34.627676</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -770,7 +774,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -782,27 +786,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -815,9 +819,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -835,14 +843,14 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.400047</v>
+        <v>-58.382261</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.586358</v>
+        <v>-34.62737</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -852,7 +860,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -864,17 +872,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -884,7 +892,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -899,11 +907,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -921,10 +929,10 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.499823</v>
+        <v>-58.511732</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.563809</v>
+        <v>-34.578688</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -938,7 +946,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -950,27 +958,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -985,11 +993,11 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1003,18 +1011,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.386058</v>
+        <v>-58.440748</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.621209</v>
+        <v>-34.63245</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1024,7 +1032,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1036,27 +1044,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1071,11 +1079,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1093,14 +1101,14 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.395465</v>
+        <v>-58.44037</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.622784</v>
+        <v>-34.632249</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1110,7 +1118,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1122,27 +1130,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1157,11 +1165,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1179,14 +1187,14 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.394079</v>
+        <v>-58.434194</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.61051</v>
+        <v>-34.571754</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1196,7 +1204,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1208,27 +1216,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1243,7 +1251,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1265,24 +1273,24 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.480871</v>
+        <v>-58.434668</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.616598</v>
+        <v>-34.571258</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1294,27 +1302,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1329,7 +1337,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1351,24 +1359,24 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.407076</v>
+        <v>-58.473937</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.616016</v>
+        <v>-34.557355</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1380,27 +1388,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1415,11 +1423,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1433,28 +1441,28 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.439727</v>
+        <v>-58.438744</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.556261</v>
+        <v>-34.629929</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1466,27 +1474,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1505,7 +1513,7 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1523,14 +1531,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.415566</v>
+        <v>-58.436255</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.613244</v>
+        <v>-34.567733</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1540,7 +1548,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1552,27 +1560,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1591,7 +1599,7 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1605,28 +1613,28 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.418089</v>
+        <v>-58.454065</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.620313</v>
+        <v>-34.57105</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1638,27 +1646,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1673,11 +1681,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1695,24 +1703,24 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.427201</v>
+        <v>-58.497446</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.617131</v>
+        <v>-34.583455</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1724,27 +1732,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1763,7 +1771,7 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1781,24 +1789,24 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.414984</v>
+        <v>-58.466348</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.621386</v>
+        <v>-34.556028</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1896,27 +1904,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1935,7 +1943,7 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1953,24 +1961,24 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.466348</v>
+        <v>-58.418089</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.556028</v>
+        <v>-34.620313</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1982,27 +1990,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2017,11 +2025,11 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2039,24 +2047,24 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.497446</v>
+        <v>-58.427201</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.583455</v>
+        <v>-34.617131</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2068,27 +2076,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2107,7 +2115,7 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2121,28 +2129,28 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.454065</v>
+        <v>-58.414984</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.57105</v>
+        <v>-34.621386</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2154,27 +2162,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2193,7 +2201,7 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2211,14 +2219,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.436255</v>
+        <v>-58.415566</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.567733</v>
+        <v>-34.613244</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2228,7 +2236,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2240,27 +2248,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2275,11 +2283,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2293,28 +2301,28 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.438744</v>
+        <v>-58.439727</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.629929</v>
+        <v>-34.556261</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2326,27 +2334,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2361,7 +2369,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2383,24 +2391,24 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.473937</v>
+        <v>-58.407076</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.557355</v>
+        <v>-34.616016</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2412,27 +2420,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2447,7 +2455,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2469,24 +2477,24 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.434668</v>
+        <v>-58.480871</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.571258</v>
+        <v>-34.616598</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,27 +2506,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2533,11 +2541,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2555,14 +2563,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.434194</v>
+        <v>-58.394079</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.571754</v>
+        <v>-34.61051</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2572,7 +2580,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,27 +2592,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2619,11 +2627,11 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2637,18 +2645,18 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.440748</v>
+        <v>-58.395465</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.63245</v>
+        <v>-34.622784</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2658,7 +2666,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,27 +2678,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2705,11 +2713,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2727,14 +2735,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.44037</v>
+        <v>-58.386058</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.632249</v>
+        <v>-34.621209</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2744,7 +2752,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2764,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2789,13 +2797,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H28" t="inlineStr"/>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2813,24 +2817,24 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.511732</v>
+        <v>-58.400047</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.578688</v>
+        <v>-34.586358</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,27 +2846,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2877,11 +2881,11 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2899,24 +2903,24 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.404058</v>
+        <v>-58.499823</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.634341</v>
+        <v>-34.563809</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2928,27 +2932,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2963,11 +2967,11 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2985,24 +2989,24 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.487821</v>
+        <v>-58.390198</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.554603</v>
+        <v>-34.637568</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3014,27 +3018,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3047,17 +3051,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Columna inclinada</t>
-        </is>
-      </c>
+      <c r="H31" t="inlineStr"/>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -3067,18 +3067,18 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.382231</v>
+        <v>-58.39894</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.627676</v>
+        <v>-34.591084</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3088,29 +3088,29 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>RET-E</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Lima 1649</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -3120,7 +3120,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3135,11 +3135,11 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3157,10 +3157,10 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.382261</v>
+        <v>-58.390269</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.62737</v>
+        <v>-34.625079</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3174,7 +3174,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-12-19 18:00:32)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,11 +563,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -585,10 +585,10 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.404058</v>
+        <v>-58.390269</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.634341</v>
+        <v>-34.625079</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -614,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -647,13 +647,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -671,56 +667,56 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.487821</v>
+        <v>-58.39894</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.554603</v>
+        <v>-34.591084</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>RET-E</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -735,15 +731,15 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -753,14 +749,14 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.382231</v>
+        <v>-58.390198</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.627676</v>
+        <v>-34.637568</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -774,7 +770,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -786,27 +782,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Lima 1649</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -819,13 +815,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -843,14 +835,14 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.382261</v>
+        <v>-58.400047</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.62737</v>
+        <v>-34.586358</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -860,7 +852,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -872,17 +864,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -892,7 +884,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -907,11 +899,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -929,10 +921,10 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.511732</v>
+        <v>-58.499823</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.578688</v>
+        <v>-34.563809</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -946,7 +938,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -958,27 +950,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -993,11 +985,11 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1011,18 +1003,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.440748</v>
+        <v>-58.386058</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.63245</v>
+        <v>-34.621209</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1032,7 +1024,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1044,27 +1036,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1079,11 +1071,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1101,14 +1093,14 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.44037</v>
+        <v>-58.395465</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.632249</v>
+        <v>-34.622784</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1118,7 +1110,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1130,27 +1122,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1165,11 +1157,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1187,14 +1179,14 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.434194</v>
+        <v>-58.394079</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.571754</v>
+        <v>-34.61051</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1204,7 +1196,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1216,27 +1208,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1251,7 +1243,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1273,24 +1265,24 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.434668</v>
+        <v>-58.480871</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.571258</v>
+        <v>-34.616598</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1302,27 +1294,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1337,7 +1329,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1359,24 +1351,24 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.473937</v>
+        <v>-58.407076</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.557355</v>
+        <v>-34.616016</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1388,27 +1380,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1423,11 +1415,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1441,28 +1433,28 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.438744</v>
+        <v>-58.439727</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.629929</v>
+        <v>-34.556261</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1474,27 +1466,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1513,7 +1505,7 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1531,14 +1523,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.436255</v>
+        <v>-58.415566</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.567733</v>
+        <v>-34.613244</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1548,7 +1540,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1560,27 +1552,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1599,7 +1591,7 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1613,28 +1605,28 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.454065</v>
+        <v>-58.418089</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.57105</v>
+        <v>-34.620313</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1646,27 +1638,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1681,11 +1673,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1703,24 +1695,24 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.497446</v>
+        <v>-58.427201</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.583455</v>
+        <v>-34.617131</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1732,27 +1724,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1771,7 +1763,7 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1789,24 +1781,24 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.466348</v>
+        <v>-58.414984</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.556028</v>
+        <v>-34.621386</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1904,27 +1896,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1943,7 +1935,7 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1961,24 +1953,24 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.418089</v>
+        <v>-58.466348</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.620313</v>
+        <v>-34.556028</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1990,27 +1982,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2025,11 +2017,11 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2047,24 +2039,24 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.427201</v>
+        <v>-58.497446</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.617131</v>
+        <v>-34.583455</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2076,27 +2068,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2115,7 +2107,7 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2129,28 +2121,28 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.414984</v>
+        <v>-58.454065</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.621386</v>
+        <v>-34.57105</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2162,27 +2154,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2201,7 +2193,7 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2219,14 +2211,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.415566</v>
+        <v>-58.436255</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.613244</v>
+        <v>-34.567733</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2236,7 +2228,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2248,27 +2240,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2283,11 +2275,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2301,28 +2293,28 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.439727</v>
+        <v>-58.438744</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.556261</v>
+        <v>-34.629929</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2334,27 +2326,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2369,7 +2361,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2391,24 +2383,24 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.407076</v>
+        <v>-58.473937</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.616016</v>
+        <v>-34.557355</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2420,27 +2412,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2455,7 +2447,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2477,24 +2469,24 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.480871</v>
+        <v>-58.434668</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.616598</v>
+        <v>-34.571258</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2506,27 +2498,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2541,11 +2533,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2563,14 +2555,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.394079</v>
+        <v>-58.434194</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.61051</v>
+        <v>-34.571754</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2580,7 +2572,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2592,27 +2584,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2627,11 +2619,11 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2645,18 +2637,18 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.395465</v>
+        <v>-58.440748</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.622784</v>
+        <v>-34.63245</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2666,7 +2658,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2678,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2713,11 +2705,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2735,14 +2727,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.386058</v>
+        <v>-58.44037</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.621209</v>
+        <v>-34.632249</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2752,7 +2744,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2764,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2797,9 +2789,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr"/>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2817,24 +2813,24 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.400047</v>
+        <v>-58.511732</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.586358</v>
+        <v>-34.578688</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2846,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2881,11 +2877,11 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2903,24 +2899,24 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.499823</v>
+        <v>-58.404058</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.563809</v>
+        <v>-34.634341</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2932,27 +2928,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2967,11 +2963,11 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2989,24 +2985,24 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.390198</v>
+        <v>-58.487821</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.637568</v>
+        <v>-34.554603</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3018,27 +3014,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3051,13 +3047,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr"/>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Columna inclinada</t>
+        </is>
+      </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -3067,18 +3067,18 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.39894</v>
+        <v>-58.382231</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.591084</v>
+        <v>-34.627676</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3088,29 +3088,29 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>RET-E</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -3120,7 +3120,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3135,11 +3135,11 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3157,10 +3157,10 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.390269</v>
+        <v>-58.382261</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.625079</v>
+        <v>-34.62737</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3174,7 +3174,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-12-26 16:41:35)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,11 +563,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -585,10 +585,10 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.390269</v>
+        <v>-58.404058</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.625079</v>
+        <v>-34.634341</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -614,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -647,9 +647,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+        </is>
+      </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -667,56 +671,56 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.39894</v>
+        <v>-58.487821</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.591084</v>
+        <v>-34.554603</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>RET-E</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -731,15 +735,15 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -749,14 +753,14 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.390198</v>
+        <v>-58.382231</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.637568</v>
+        <v>-34.627676</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -770,7 +774,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -782,27 +786,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -815,9 +819,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -835,14 +843,14 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.400047</v>
+        <v>-58.382261</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.586358</v>
+        <v>-34.62737</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -852,7 +860,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -864,17 +872,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -884,7 +892,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -899,11 +907,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -921,10 +929,10 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.499823</v>
+        <v>-58.511732</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.563809</v>
+        <v>-34.578688</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -938,7 +946,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -950,27 +958,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -985,11 +993,11 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1003,18 +1011,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.386058</v>
+        <v>-58.440748</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.621209</v>
+        <v>-34.63245</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1024,7 +1032,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1036,27 +1044,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1071,11 +1079,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1093,14 +1101,14 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.395465</v>
+        <v>-58.44037</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.622784</v>
+        <v>-34.632249</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1110,7 +1118,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1122,27 +1130,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1157,11 +1165,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1179,14 +1187,14 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.394079</v>
+        <v>-58.434194</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.61051</v>
+        <v>-34.571754</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1196,7 +1204,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1208,27 +1216,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1243,7 +1251,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1265,24 +1273,24 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.480871</v>
+        <v>-58.434668</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.616598</v>
+        <v>-34.571258</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1294,27 +1302,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1329,7 +1337,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1351,24 +1359,24 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.407076</v>
+        <v>-58.473937</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.616016</v>
+        <v>-34.557355</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1380,27 +1388,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1415,11 +1423,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1433,28 +1441,28 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.439727</v>
+        <v>-58.438744</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.556261</v>
+        <v>-34.629929</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1466,27 +1474,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1505,7 +1513,7 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1523,14 +1531,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.415566</v>
+        <v>-58.436255</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.613244</v>
+        <v>-34.567733</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1540,7 +1548,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1552,27 +1560,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1591,7 +1599,7 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1605,28 +1613,28 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.418089</v>
+        <v>-58.454065</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.620313</v>
+        <v>-34.57105</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1638,27 +1646,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1673,11 +1681,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1695,24 +1703,24 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.427201</v>
+        <v>-58.497446</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.617131</v>
+        <v>-34.583455</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1724,27 +1732,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Quesada 2710</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>804568979</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1763,7 +1771,7 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1781,24 +1789,24 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.414984</v>
+        <v>-58.466348</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.621386</v>
+        <v>-34.556028</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1896,27 +1904,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Quesada 2710</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804568979</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1935,7 +1943,7 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1953,24 +1961,24 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.466348</v>
+        <v>-58.418089</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.556028</v>
+        <v>-34.620313</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1982,27 +1990,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Quito 4292</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804270068</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2017,11 +2025,11 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2039,24 +2047,24 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.497446</v>
+        <v>-58.427201</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.583455</v>
+        <v>-34.617131</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2068,27 +2076,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2107,7 +2115,7 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2121,28 +2129,28 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.454065</v>
+        <v>-58.414984</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.57105</v>
+        <v>-34.621386</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2154,27 +2162,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2193,7 +2201,7 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2211,14 +2219,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.436255</v>
+        <v>-58.415566</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.567733</v>
+        <v>-34.613244</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2228,7 +2236,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2240,27 +2248,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>LA PAMPA 1001</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>803608208</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2275,11 +2283,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2293,28 +2301,28 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.438744</v>
+        <v>-58.439727</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.629929</v>
+        <v>-34.556261</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2326,27 +2334,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2361,7 +2369,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2383,24 +2391,24 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.473937</v>
+        <v>-58.407076</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.557355</v>
+        <v>-34.616016</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2412,27 +2420,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2447,7 +2455,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2469,24 +2477,24 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.434668</v>
+        <v>-58.480871</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.571258</v>
+        <v>-34.616598</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,27 +2506,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2533,11 +2541,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2555,14 +2563,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.434194</v>
+        <v>-58.394079</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.571754</v>
+        <v>-34.61051</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2572,7 +2580,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,27 +2592,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2619,11 +2627,11 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2637,18 +2645,18 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.440748</v>
+        <v>-58.395465</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.63245</v>
+        <v>-34.622784</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2658,7 +2666,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,27 +2678,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2705,11 +2713,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2727,14 +2735,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.44037</v>
+        <v>-58.386058</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.632249</v>
+        <v>-34.621209</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2744,7 +2752,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2764,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2789,13 +2797,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H28" t="inlineStr"/>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2813,24 +2817,24 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.511732</v>
+        <v>-58.400047</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.578688</v>
+        <v>-34.586358</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,27 +2846,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2877,11 +2881,11 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2899,24 +2903,24 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.404058</v>
+        <v>-58.499823</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.634341</v>
+        <v>-34.563809</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2928,27 +2932,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2963,11 +2967,11 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2985,24 +2989,24 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.487821</v>
+        <v>-58.390198</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.554603</v>
+        <v>-34.637568</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3014,27 +3018,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3047,17 +3051,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Columna inclinada</t>
-        </is>
-      </c>
+      <c r="H31" t="inlineStr"/>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -3067,18 +3067,18 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.382231</v>
+        <v>-58.39894</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.627676</v>
+        <v>-34.591084</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3088,29 +3088,29 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>RET-E</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Lima 1649</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -3120,7 +3120,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3135,11 +3135,11 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3157,10 +3157,10 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.382261</v>
+        <v>-58.390269</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.62737</v>
+        <v>-34.625079</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3174,7 +3174,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2026-01-07 09:32:28)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,11 +563,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -585,10 +585,10 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.404058</v>
+        <v>-58.390269</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.634341</v>
+        <v>-34.625079</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -614,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -647,13 +647,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -671,56 +667,56 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.487821</v>
+        <v>-58.39894</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.554603</v>
+        <v>-34.591084</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>RET-E</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -735,15 +731,15 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -753,14 +749,14 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.382231</v>
+        <v>-58.390198</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.627676</v>
+        <v>-34.637568</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -774,7 +770,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -786,27 +782,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Lima 1649</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -819,13 +815,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -843,14 +835,14 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.382261</v>
+        <v>-58.400047</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.62737</v>
+        <v>-34.586358</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -860,7 +852,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -872,17 +864,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -892,7 +884,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -907,11 +899,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -929,10 +921,10 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.511732</v>
+        <v>-58.499823</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.578688</v>
+        <v>-34.563809</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -946,7 +938,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -958,27 +950,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -993,11 +985,11 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1011,18 +1003,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.440748</v>
+        <v>-58.386058</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.63245</v>
+        <v>-34.621209</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1032,7 +1024,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1044,27 +1036,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1079,11 +1071,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1101,14 +1093,14 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.44037</v>
+        <v>-58.395465</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.632249</v>
+        <v>-34.622784</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1118,7 +1110,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1130,27 +1122,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1165,11 +1157,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1187,14 +1179,14 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.434194</v>
+        <v>-58.394079</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.571754</v>
+        <v>-34.61051</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1204,7 +1196,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1216,27 +1208,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1251,7 +1243,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1273,24 +1265,24 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.434668</v>
+        <v>-58.480871</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.571258</v>
+        <v>-34.616598</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1302,27 +1294,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1337,7 +1329,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1359,24 +1351,24 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.473937</v>
+        <v>-58.407076</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.557355</v>
+        <v>-34.616016</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1388,27 +1380,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1423,11 +1415,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1441,18 +1433,18 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.438744</v>
+        <v>-58.415566</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.629929</v>
+        <v>-34.613244</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1462,7 +1454,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1474,27 +1466,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1513,7 +1505,7 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1531,14 +1523,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.436255</v>
+        <v>-58.418089</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.567733</v>
+        <v>-34.620313</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1548,7 +1540,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1560,27 +1552,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1599,7 +1591,7 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1613,28 +1605,28 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.454065</v>
+        <v>-58.414984</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.57105</v>
+        <v>-34.621386</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1646,17 +1638,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1666,7 +1658,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1685,7 +1677,7 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1703,10 +1695,10 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.497446</v>
+        <v>-58.507569</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.583455</v>
+        <v>-34.579623</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1720,7 +1712,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1818,17 +1810,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1838,7 +1830,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1857,7 +1849,7 @@
         </is>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1875,10 +1867,10 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.507569</v>
+        <v>-58.497446</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.579623</v>
+        <v>-34.583455</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1892,7 +1884,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1904,27 +1896,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1943,7 +1935,7 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1957,28 +1949,28 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.418089</v>
+        <v>-58.454065</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.620313</v>
+        <v>-34.57105</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1990,27 +1982,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Quito 4292</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804270068</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2029,7 +2021,7 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2047,14 +2039,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.427201</v>
+        <v>-58.436255</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.617131</v>
+        <v>-34.567733</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2064,7 +2056,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2076,27 +2068,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2111,11 +2103,11 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2129,14 +2121,14 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.414984</v>
+        <v>-58.438744</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.621386</v>
+        <v>-34.629929</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -2150,7 +2142,7 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2162,27 +2154,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2201,7 +2193,7 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2219,24 +2211,24 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.415566</v>
+        <v>-58.473937</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.613244</v>
+        <v>-34.557355</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2248,27 +2240,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>LA PAMPA 1001</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>803608208</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2283,11 +2275,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna base corroida prioridad media </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2305,24 +2297,24 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.439727</v>
+        <v>-58.434668</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.556261</v>
+        <v>-34.571258</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2334,27 +2326,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2369,7 +2361,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2391,14 +2383,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.407076</v>
+        <v>-58.434194</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.616016</v>
+        <v>-34.571754</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2408,7 +2400,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2420,27 +2412,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2455,7 +2447,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2473,28 +2465,28 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.480871</v>
+        <v>-58.440748</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.616598</v>
+        <v>-34.63245</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2506,27 +2498,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2541,11 +2533,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2563,14 +2555,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.394079</v>
+        <v>-58.44037</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.61051</v>
+        <v>-34.632249</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2580,7 +2572,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2592,27 +2584,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2627,11 +2619,11 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2649,24 +2641,24 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.395465</v>
+        <v>-58.511732</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.622784</v>
+        <v>-34.578688</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2678,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2713,11 +2705,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2735,10 +2727,10 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.386058</v>
+        <v>-58.404058</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.621209</v>
+        <v>-34.634341</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2752,7 +2744,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2764,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2797,9 +2789,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr"/>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+        </is>
+      </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2817,24 +2813,24 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.400047</v>
+        <v>-58.487821</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.586358</v>
+        <v>-34.554603</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2846,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2881,15 +2877,15 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2899,28 +2895,28 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.499823</v>
+        <v>-58.382231</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.563809</v>
+        <v>-34.627676</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2932,27 +2928,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2967,11 +2963,11 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2989,10 +2985,10 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.390198</v>
+        <v>-58.382261</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.637568</v>
+        <v>-34.62737</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -3010,174 +3006,6 @@
         </is>
       </c>
       <c r="R30" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>-23</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>2/7/2024</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>FRENCH /ALT/ 2380</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>780043028</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="n">
-        <v>0</v>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M31" t="n">
-        <v>-58.39894</v>
-      </c>
-      <c r="N31" t="n">
-        <v>-34.591084</v>
-      </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>Recoleta</t>
-        </is>
-      </c>
-      <c r="P31" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>RET-E</t>
-        </is>
-      </c>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.1RET</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>-20</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>2/6/2024</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>780027603</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>Direccion correcta 1736</t>
-        </is>
-      </c>
-      <c r="I32" t="n">
-        <v>0</v>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M32" t="n">
-        <v>-58.390269</v>
-      </c>
-      <c r="N32" t="n">
-        <v>-34.625079</v>
-      </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P32" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>CON-M</t>
-        </is>
-      </c>
-      <c r="R32" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2026-01-14 13:23:36)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,11 +563,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -585,10 +585,10 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.390269</v>
+        <v>-58.404058</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.625079</v>
+        <v>-34.634341</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -614,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -647,9 +647,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+        </is>
+      </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -667,56 +671,56 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.39894</v>
+        <v>-58.487821</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.591084</v>
+        <v>-34.554603</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>RET-E</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -731,15 +735,15 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -749,14 +753,14 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.390198</v>
+        <v>-58.382231</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.637568</v>
+        <v>-34.627676</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -770,7 +774,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -782,27 +786,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -815,9 +819,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -835,14 +843,14 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.400047</v>
+        <v>-58.382261</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.586358</v>
+        <v>-34.62737</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -852,7 +860,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -864,17 +872,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -884,7 +892,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -899,11 +907,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -921,10 +929,10 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.499823</v>
+        <v>-58.511732</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.563809</v>
+        <v>-34.578688</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -938,7 +946,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -950,27 +958,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -985,11 +993,11 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1003,18 +1011,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.386058</v>
+        <v>-58.440748</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.621209</v>
+        <v>-34.63245</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1024,7 +1032,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1036,27 +1044,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1071,11 +1079,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1093,14 +1101,14 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.395465</v>
+        <v>-58.44037</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.622784</v>
+        <v>-34.632249</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1110,7 +1118,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1122,27 +1130,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1157,11 +1165,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1179,14 +1187,14 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.394079</v>
+        <v>-58.434194</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.61051</v>
+        <v>-34.571754</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1196,7 +1204,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1208,27 +1216,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1243,7 +1251,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1265,24 +1273,24 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.480871</v>
+        <v>-58.434668</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.616598</v>
+        <v>-34.571258</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1294,27 +1302,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1329,7 +1337,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1351,24 +1359,24 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.407076</v>
+        <v>-58.473937</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.616016</v>
+        <v>-34.557355</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1380,27 +1388,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1415,11 +1423,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1433,18 +1441,18 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.415566</v>
+        <v>-58.438744</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.613244</v>
+        <v>-34.629929</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1454,7 +1462,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1466,27 +1474,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1505,7 +1513,7 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1523,14 +1531,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.418089</v>
+        <v>-58.436255</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.620313</v>
+        <v>-34.567733</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1540,7 +1548,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1552,27 +1560,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1591,7 +1599,7 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1605,28 +1613,28 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.414984</v>
+        <v>-58.454065</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.621386</v>
+        <v>-34.57105</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1638,17 +1646,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1658,7 +1666,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1677,7 +1685,7 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1695,10 +1703,10 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.507569</v>
+        <v>-58.497446</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.579623</v>
+        <v>-34.583455</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1712,7 +1720,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1810,17 +1818,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1830,7 +1838,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1849,7 +1857,7 @@
         </is>
       </c>
       <c r="I17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1867,10 +1875,10 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.497446</v>
+        <v>-58.507569</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.583455</v>
+        <v>-34.579623</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1884,7 +1892,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1896,27 +1904,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1935,7 +1943,7 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1949,28 +1957,28 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.454065</v>
+        <v>-58.418089</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.57105</v>
+        <v>-34.620313</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1982,27 +1990,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2021,7 +2029,7 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2039,14 +2047,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.436255</v>
+        <v>-58.414984</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.567733</v>
+        <v>-34.621386</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2056,7 +2064,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2068,27 +2076,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2103,11 +2111,11 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2121,18 +2129,18 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.438744</v>
+        <v>-58.415566</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.629929</v>
+        <v>-34.613244</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2142,7 +2150,7 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2154,27 +2162,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2189,7 +2197,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2211,24 +2219,24 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.473937</v>
+        <v>-58.407076</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.557355</v>
+        <v>-34.616016</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2240,27 +2248,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2275,7 +2283,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2297,24 +2305,24 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.434668</v>
+        <v>-58.480871</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.571258</v>
+        <v>-34.616598</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2326,27 +2334,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2361,11 +2369,11 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2383,14 +2391,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.434194</v>
+        <v>-58.394079</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.571754</v>
+        <v>-34.61051</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2400,7 +2408,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2412,27 +2420,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2447,11 +2455,11 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2465,18 +2473,18 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.440748</v>
+        <v>-58.395465</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.63245</v>
+        <v>-34.622784</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2486,7 +2494,7 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,27 +2506,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2533,11 +2541,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2555,14 +2563,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.44037</v>
+        <v>-58.386058</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.632249</v>
+        <v>-34.621209</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2572,7 +2580,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,27 +2592,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2617,13 +2625,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H26" t="inlineStr"/>
       <c r="I26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2641,24 +2645,24 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.511732</v>
+        <v>-58.400047</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.578688</v>
+        <v>-34.586358</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,27 +2674,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2705,11 +2709,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2727,24 +2731,24 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.404058</v>
+        <v>-58.499823</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.634341</v>
+        <v>-34.563809</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2760,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2791,11 +2795,11 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2813,24 +2817,24 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.487821</v>
+        <v>-58.390198</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.554603</v>
+        <v>-34.637568</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,27 +2846,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2875,17 +2879,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>Columna inclinada</t>
-        </is>
-      </c>
+      <c r="H29" t="inlineStr"/>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2895,18 +2895,18 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.382231</v>
+        <v>-58.39894</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.627676</v>
+        <v>-34.591084</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2916,29 +2916,29 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>RET-E</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Lima 1649</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2948,7 +2948,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2963,11 +2963,11 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2985,10 +2985,10 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.382261</v>
+        <v>-58.390269</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.62737</v>
+        <v>-34.625079</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2026-01-16 15:21:36)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -476,22 +476,22 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>Tipo de tarea</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Equipo</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Tipo de Elemento</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>Attachments</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Tipo de tarea</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Equipo</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Tipo de Elemento</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,32 +563,32 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
+          <t>Direccion correcta 1736</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
           <t>Pasante</t>
         </is>
       </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
       <c r="M2" t="n">
-        <v>-58.404058</v>
+        <v>-58.390269</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.634341</v>
+        <v>-34.625079</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -614,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -647,80 +647,76 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
           <t>Pasante</t>
         </is>
       </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
       <c r="M3" t="n">
-        <v>-58.487821</v>
+        <v>-58.39894</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.554603</v>
+        <v>-34.591084</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>RET-E</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -735,32 +731,32 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>-58.382231</v>
+        <v>-58.390198</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.627676</v>
+        <v>-34.637568</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -774,7 +770,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -786,27 +782,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Lima 1649</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -819,38 +815,34 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>1</v>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
           <t>Pasante</t>
         </is>
       </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
       <c r="M5" t="n">
-        <v>-58.382261</v>
+        <v>-58.400047</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.62737</v>
+        <v>-34.586358</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -860,7 +852,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -872,17 +864,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -892,7 +884,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -907,32 +899,32 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>1</v>
+          <t>Para cambiar columna fte al 3688</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
           <t>Pasante</t>
         </is>
       </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
       <c r="M6" t="n">
-        <v>-58.511732</v>
+        <v>-58.499823</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.578688</v>
+        <v>-34.563809</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -946,7 +938,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -958,27 +950,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -993,36 +985,36 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>1</v>
+          <t>Cambio de columna.-</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>-58.440748</v>
+        <v>-58.386058</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.63245</v>
+        <v>-34.621209</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1032,7 +1024,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1044,27 +1036,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1079,36 +1071,36 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>1</v>
+          <t>recambio de columna podrida en la base</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
           <t>Pasante</t>
         </is>
       </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
       <c r="M8" t="n">
-        <v>-58.44037</v>
+        <v>-58.395465</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.632249</v>
+        <v>-34.622784</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1118,7 +1110,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1130,27 +1122,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1165,36 +1157,36 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
-        <v>1</v>
+          <t>Cambio de columna.-</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
           <t>Pasante</t>
         </is>
       </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
       <c r="M9" t="n">
-        <v>-58.434194</v>
+        <v>-58.394079</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.571754</v>
+        <v>-34.61051</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1204,7 +1196,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1216,27 +1208,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1251,46 +1243,46 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
+          <t>Base picada</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
         <v>1</v>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
       <c r="M10" t="n">
-        <v>-58.434668</v>
+        <v>-58.480871</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.571258</v>
+        <v>-34.616598</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1302,27 +1294,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1337,46 +1329,46 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I11" t="n">
+          <t xml:space="preserve">Propia diámetro 114mm </t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="L11" t="n">
         <v>1</v>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
       <c r="M11" t="n">
-        <v>-58.473937</v>
+        <v>-58.407076</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.557355</v>
+        <v>-34.616016</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1388,27 +1380,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1423,36 +1415,36 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>1</v>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>-58.438744</v>
+        <v>-58.415566</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.629929</v>
+        <v>-34.613244</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1462,7 +1454,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1474,27 +1466,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1512,33 +1504,33 @@
           <t>Picada</t>
         </is>
       </c>
-      <c r="I13" t="n">
-        <v>1</v>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
           <t>Pasante</t>
         </is>
       </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
       <c r="M13" t="n">
-        <v>-58.436255</v>
+        <v>-58.418089</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.567733</v>
+        <v>-34.620313</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1548,7 +1540,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1560,27 +1552,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1598,43 +1590,43 @@
           <t>Picada</t>
         </is>
       </c>
-      <c r="I14" t="n">
-        <v>1</v>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
       </c>
       <c r="M14" t="n">
-        <v>-58.454065</v>
+        <v>-58.414984</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.57105</v>
+        <v>-34.621386</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1646,17 +1638,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1666,7 +1658,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1684,29 +1676,29 @@
           <t>Cambiar</t>
         </is>
       </c>
-      <c r="I15" t="n">
-        <v>1</v>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
           <t>Pasante</t>
         </is>
       </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
       <c r="M15" t="n">
-        <v>-58.497446</v>
+        <v>-58.507569</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.583455</v>
+        <v>-34.579623</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1720,7 +1712,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1770,23 +1762,23 @@
           <t>Picada</t>
         </is>
       </c>
-      <c r="I16" t="n">
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="L16" t="n">
         <v>1</v>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
       </c>
       <c r="M16" t="n">
         <v>-58.466348</v>
@@ -1818,17 +1810,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1838,7 +1830,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1856,29 +1848,29 @@
           <t>Cambiar</t>
         </is>
       </c>
-      <c r="I17" t="n">
-        <v>0</v>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
           <t>Pasante</t>
         </is>
       </c>
+      <c r="L17" t="n">
+        <v>1</v>
+      </c>
       <c r="M17" t="n">
-        <v>-58.507569</v>
+        <v>-58.497446</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.579623</v>
+        <v>-34.583455</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1892,7 +1884,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1904,27 +1896,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1942,43 +1934,43 @@
           <t>Picada</t>
         </is>
       </c>
-      <c r="I18" t="n">
-        <v>0</v>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="L18" t="n">
+        <v>1</v>
       </c>
       <c r="M18" t="n">
-        <v>-58.418089</v>
+        <v>-58.454065</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.620313</v>
+        <v>-34.57105</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1990,27 +1982,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2028,33 +2020,33 @@
           <t>Picada</t>
         </is>
       </c>
-      <c r="I19" t="n">
-        <v>0</v>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
           <t>Pasante</t>
         </is>
       </c>
+      <c r="L19" t="n">
+        <v>1</v>
+      </c>
       <c r="M19" t="n">
-        <v>-58.414984</v>
+        <v>-58.436255</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.621386</v>
+        <v>-34.567733</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2064,7 +2056,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2076,27 +2068,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2111,36 +2103,36 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I20" t="n">
-        <v>0</v>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="L20" t="n">
+        <v>1</v>
       </c>
       <c r="M20" t="n">
-        <v>-58.415566</v>
+        <v>-58.438744</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.613244</v>
+        <v>-34.629929</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2150,7 +2142,7 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2162,27 +2154,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2197,46 +2189,46 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
-        </is>
-      </c>
-      <c r="I21" t="n">
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="L21" t="n">
         <v>1</v>
       </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
       <c r="M21" t="n">
-        <v>-58.407076</v>
+        <v>-58.473937</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.616016</v>
+        <v>-34.557355</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2248,27 +2240,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2283,46 +2275,46 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Base picada</t>
-        </is>
-      </c>
-      <c r="I22" t="n">
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="L22" t="n">
         <v>1</v>
       </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
       <c r="M22" t="n">
-        <v>-58.480871</v>
+        <v>-58.434668</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.616598</v>
+        <v>-34.571258</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2334,27 +2326,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2369,36 +2361,36 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
-        </is>
-      </c>
-      <c r="I23" t="n">
-        <v>0</v>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
           <t>Pasante</t>
         </is>
       </c>
+      <c r="L23" t="n">
+        <v>1</v>
+      </c>
       <c r="M23" t="n">
-        <v>-58.394079</v>
+        <v>-58.434194</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.61051</v>
+        <v>-34.571754</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2408,7 +2400,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2420,27 +2412,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2455,36 +2447,36 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
-        </is>
-      </c>
-      <c r="I24" t="n">
-        <v>0</v>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="L24" t="n">
+        <v>1</v>
       </c>
       <c r="M24" t="n">
-        <v>-58.395465</v>
+        <v>-58.440748</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.622784</v>
+        <v>-34.63245</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2494,7 +2486,7 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2506,27 +2498,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2541,36 +2533,36 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
-        </is>
-      </c>
-      <c r="I25" t="n">
-        <v>0</v>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
           <t>Pasante</t>
         </is>
       </c>
+      <c r="L25" t="n">
+        <v>1</v>
+      </c>
       <c r="M25" t="n">
-        <v>-58.386058</v>
+        <v>-58.44037</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.621209</v>
+        <v>-34.632249</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2580,7 +2572,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2592,27 +2584,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2625,44 +2617,48 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="n">
-        <v>0</v>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
           <t>Pasante</t>
         </is>
       </c>
+      <c r="L26" t="n">
+        <v>1</v>
+      </c>
       <c r="M26" t="n">
-        <v>-58.400047</v>
+        <v>-58.511732</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.586358</v>
+        <v>-34.578688</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2674,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2709,46 +2705,46 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
-        </is>
-      </c>
-      <c r="I27" t="n">
-        <v>0</v>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L27" t="inlineStr">
-        <is>
           <t>Pasante</t>
         </is>
       </c>
+      <c r="L27" t="n">
+        <v>1</v>
+      </c>
       <c r="M27" t="n">
-        <v>-58.499823</v>
+        <v>-58.404058</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.563809</v>
+        <v>-34.634341</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2760,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2795,46 +2791,46 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
-        </is>
-      </c>
-      <c r="I28" t="n">
-        <v>0</v>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
           <t>Pasante</t>
         </is>
       </c>
+      <c r="L28" t="n">
+        <v>1</v>
+      </c>
       <c r="M28" t="n">
-        <v>-58.390198</v>
+        <v>-58.487821</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.637568</v>
+        <v>-34.554603</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2846,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2879,34 +2875,38 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="n">
-        <v>0</v>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Columna inclinada</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="L29" t="n">
+        <v>1</v>
       </c>
       <c r="M29" t="n">
-        <v>-58.39894</v>
+        <v>-58.382231</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.591084</v>
+        <v>-34.627676</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2916,29 +2916,29 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>RET-E</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2948,7 +2948,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2963,32 +2963,32 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
-        </is>
-      </c>
-      <c r="I30" t="n">
-        <v>0</v>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L30" t="inlineStr">
-        <is>
           <t>Pasante</t>
         </is>
       </c>
+      <c r="L30" t="n">
+        <v>1</v>
+      </c>
       <c r="M30" t="n">
-        <v>-58.390269</v>
+        <v>-58.382261</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.625079</v>
+        <v>-34.62737</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2026-01-23 16:17:38)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_INCO.xlsx
+++ b/mapa_interactivo_INCO.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -434,92 +422,92 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Caso</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>F. De Reclamo</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Direccion</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Comuna</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>OT</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Proveedor Asignado</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Estado</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Observaciones</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Tipo de tarea</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Equipo</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Tipo de Elemento</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Attachments</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>Coordenada_X</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>Coordenada_Y</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>Operacion</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>Zona</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>PD</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>N2</t>
         </is>
@@ -528,27 +516,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2/6/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CONSTITUCION /ALT/ 1739</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>780027603</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,7 +551,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Direccion correcta 1736</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -582,13 +570,13 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>-58.390269</v>
+        <v>-58.404058</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.625079</v>
+        <v>-34.634341</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -602,7 +590,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -614,27 +602,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>-23</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2/7/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>FRENCH /ALT/ 2380</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>780043028</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -647,7 +635,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+        </is>
+      </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>Cambio</t>
@@ -664,59 +656,59 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>-58.39894</v>
+        <v>-58.487821</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.591084</v>
+        <v>-34.554603</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>RET-E</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-43</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3/11/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
+          <t>Lima 1697</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>781392461</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -731,12 +723,12 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -746,17 +738,17 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>-58.390198</v>
+        <v>-58.382231</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.637568</v>
+        <v>-34.627676</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -770,7 +762,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -782,27 +774,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>AGUERO /ALT/ 2310</t>
+          <t>Lima 1649</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>784675618</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -815,7 +807,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>Cambio</t>
@@ -832,17 +828,17 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" t="n">
-        <v>-58.400047</v>
+        <v>-58.382261</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.586358</v>
+        <v>-34.62737</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -852,7 +848,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>AGU-H</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -864,17 +860,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-71</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 3696</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -884,7 +880,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>784675639</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -899,7 +895,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Para cambiar columna fte al 3688</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -918,13 +914,13 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>-58.499823</v>
+        <v>-58.511732</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.563809</v>
+        <v>-34.578688</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -938,7 +934,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>PUE-?</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -950,27 +946,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-100</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6/11/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>HUMBERTO PRIMO /ALT/ 1416</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>788000212</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -985,7 +981,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -1000,21 +996,21 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>-58.386058</v>
+        <v>-58.440748</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.621209</v>
+        <v>-34.63245</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1024,7 +1020,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>CEN-A</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1036,27 +1032,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-105</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6/24/2024</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>RINCON /ALT/ 1191</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>789151020</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1071,7 +1067,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>recambio de columna podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1090,17 +1086,17 @@
         </is>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" t="n">
-        <v>-58.395465</v>
+        <v>-58.44037</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.622784</v>
+        <v>-34.632249</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1110,7 +1106,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>CEN-B</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1122,27 +1118,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-109</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>790175801</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1157,7 +1153,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1176,17 +1172,17 @@
         </is>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" t="n">
-        <v>-58.394079</v>
+        <v>-58.434194</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.61051</v>
+        <v>-34.571754</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1196,7 +1192,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1208,27 +1204,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-271</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1/27/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>HELGUERA /ALT/ 1405</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>802925468</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1243,7 +1239,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1265,24 +1261,24 @@
         <v>1</v>
       </c>
       <c r="M10" t="n">
-        <v>-58.480871</v>
+        <v>-58.434668</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.616598</v>
+        <v>-34.571258</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>BLO-H</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1294,27 +1290,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-275</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>DEAN FUNES /ALT/ 481</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>803039902</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1329,7 +1325,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Propia diámetro 114mm </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1351,24 +1347,24 @@
         <v>1</v>
       </c>
       <c r="M11" t="n">
-        <v>-58.407076</v>
+        <v>-58.473937</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.616016</v>
+        <v>-34.557355</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>CEN-J</t>
+          <t>COG-L</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1380,27 +1376,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Av. Hipólito Yrigoyen 3451</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>804161204</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1415,7 +1411,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1430,21 +1426,21 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" t="n">
-        <v>-58.415566</v>
+        <v>-58.438744</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.613244</v>
+        <v>-34.629929</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1454,7 +1450,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>PPT-P</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1466,27 +1462,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Colombres 636</t>
+          <t>Arce 867</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804270064</t>
+          <t>805655355</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1520,17 +1516,17 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" t="n">
-        <v>-58.418089</v>
+        <v>-58.436255</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.620313</v>
+        <v>-34.567733</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1540,7 +1536,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1552,27 +1548,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3/21/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Maza 836</t>
+          <t>Virrey Arredondo 2821</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804270074</t>
+          <t>805507192</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1602,31 +1598,31 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" t="n">
-        <v>-58.414984</v>
+        <v>-58.454065</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.621386</v>
+        <v>-34.57105</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>ATH-H</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1638,17 +1634,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Cochrane 2864</t>
+          <t>Av. Gral. Mosconi 2490</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1658,7 +1654,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804427444</t>
+          <t>804736517</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1692,13 +1688,13 @@
         </is>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" t="n">
-        <v>-58.507569</v>
+        <v>-58.497446</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.579623</v>
+        <v>-34.583455</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1712,7 +1708,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1810,17 +1806,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 2490</t>
+          <t>Cochrane 2864</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1830,7 +1826,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804736517</t>
+          <t>804427444</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1864,13 +1860,13 @@
         </is>
       </c>
       <c r="L17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" t="n">
-        <v>-58.497446</v>
+        <v>-58.507569</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.583455</v>
+        <v>-34.579623</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1884,7 +1880,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1896,27 +1892,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Virrey Arredondo 2821</t>
+          <t>Colombres 636</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>805507192</t>
+          <t>804270064</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1946,31 +1942,31 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" t="n">
-        <v>-58.454065</v>
+        <v>-58.418089</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.57105</v>
+        <v>-34.620313</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>ATH-H</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1982,27 +1978,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>3/21/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Arce 867</t>
+          <t>Maza 836</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>805655355</t>
+          <t>804270074</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2036,17 +2032,17 @@
         </is>
       </c>
       <c r="L19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>-58.436255</v>
+        <v>-58.414984</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.567733</v>
+        <v>-34.621386</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2056,7 +2052,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2068,27 +2064,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Av. Hipólito Yrigoyen 3451</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>804161204</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2103,7 +2099,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -2118,21 +2114,21 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20" t="n">
-        <v>-58.438744</v>
+        <v>-58.415566</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.629929</v>
+        <v>-34.613244</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2142,7 +2138,7 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2154,27 +2150,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>DEAN FUNES /ALT/ 481</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>803039902</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2189,7 +2185,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Propia diámetro 114mm </t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2211,24 +2207,24 @@
         <v>1</v>
       </c>
       <c r="M21" t="n">
-        <v>-58.473937</v>
+        <v>-58.407076</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.557355</v>
+        <v>-34.616016</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>COG-L</t>
+          <t>CEN-J</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2240,27 +2236,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-271</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>1/27/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>HELGUERA /ALT/ 1405</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>802925468</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2275,7 +2271,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -2297,24 +2293,24 @@
         <v>1</v>
       </c>
       <c r="M22" t="n">
-        <v>-58.434668</v>
+        <v>-58.480871</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.571258</v>
+        <v>-34.616598</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2326,27 +2322,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-109</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/8/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>YRIGOYEN HIPOLITO /ALT/ 1938</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>790175801</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2361,7 +2357,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -2380,17 +2376,17 @@
         </is>
       </c>
       <c r="L23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23" t="n">
-        <v>-58.434194</v>
+        <v>-58.394079</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.571754</v>
+        <v>-34.61051</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2400,7 +2396,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>BLO-H</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2412,27 +2408,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/24/2024</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>RINCON /ALT/ 1191</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>789151020</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2447,7 +2443,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>recambio de columna podrida en la base</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -2462,21 +2458,21 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="L24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24" t="n">
-        <v>-58.440748</v>
+        <v>-58.395465</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.63245</v>
+        <v>-34.622784</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2486,7 +2482,7 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-B</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,27 +2494,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-100</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>6/11/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>HUMBERTO PRIMO /ALT/ 1416</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>788000212</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2533,7 +2529,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio de columna.-</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -2552,17 +2548,17 @@
         </is>
       </c>
       <c r="L25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25" t="n">
-        <v>-58.44037</v>
+        <v>-58.386058</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.632249</v>
+        <v>-34.621209</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2572,7 +2568,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>PPT-P</t>
+          <t>CEN-A</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,27 +2580,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>-70</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>AGUERO /ALT/ 2310</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>784675618</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2617,11 +2613,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr">
         <is>
           <t>Cambio</t>
@@ -2638,27 +2630,27 @@
         </is>
       </c>
       <c r="L26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26" t="n">
-        <v>-58.511732</v>
+        <v>-58.400047</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.578688</v>
+        <v>-34.586358</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>AGU-H</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,27 +2662,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-552</t>
+          <t>-71</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Catulo Castillo 2890</t>
+          <t>ANDONAEGUI /ALT/ 3696</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>808973183</t>
+          <t>784675639</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2705,7 +2697,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Para cambiar columna fte al 3688</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -2724,27 +2716,27 @@
         </is>
       </c>
       <c r="L27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27" t="n">
-        <v>-58.404058</v>
+        <v>-58.499823</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.634341</v>
+        <v>-34.563809</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>PUE-?</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2748,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-553</t>
+          <t>-43</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>3/11/2024</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>VELEZ SARSFIELD ,AV. /ALT/ 299</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>808973192</t>
+          <t>781392461</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2791,7 +2783,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
+          <t xml:space="preserve">Poste metal cv con base con leve corrosión y superficie inclinada sin riesgo de caída </t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2810,27 +2802,27 @@
         </is>
       </c>
       <c r="L28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28" t="n">
-        <v>-58.487821</v>
+        <v>-58.390198</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.554603</v>
+        <v>-34.637568</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>CON-K</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,27 +2834,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-554</t>
+          <t>-23</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/7/2024</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Lima 1697</t>
+          <t>FRENCH /ALT/ 2380</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>808973197</t>
+          <t>780043028</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2875,14 +2867,10 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>Columna inclinada</t>
-        </is>
-      </c>
+      <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -2892,21 +2880,21 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="L29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M29" t="n">
-        <v>-58.382231</v>
+        <v>-58.39894</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.627676</v>
+        <v>-34.591084</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2916,29 +2904,29 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>RET-E</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-555</t>
+          <t>-20</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>2/6/2024</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Lima 1649</t>
+          <t>CONSTITUCION /ALT/ 1739</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2948,7 +2936,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>808973201</t>
+          <t>780027603</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2963,7 +2951,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Direccion correcta 1736</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2982,13 +2970,13 @@
         </is>
       </c>
       <c r="L30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M30" t="n">
-        <v>-58.382261</v>
+        <v>-58.390269</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.62737</v>
+        <v>-34.625079</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -3002,7 +2990,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>CON-K</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">

</xml_diff>